<commit_message>
Update + adding LA County to per capita plot.
</commit_message>
<xml_diff>
--- a/Clark_Data.xlsx
+++ b/Clark_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -40,6 +40,12 @@
     <t>Unnamed: 0.1.1.1.1.1.1.1</t>
   </si>
   <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
@@ -332,6 +338,18 @@
   </si>
   <si>
     <t>06-17-2020</t>
+  </si>
+  <si>
+    <t>06-18-2020</t>
+  </si>
+  <si>
+    <t>06-19-2020</t>
+  </si>
+  <si>
+    <t>06-20-2020</t>
+  </si>
+  <si>
+    <t>06-21-2020</t>
   </si>
 </sst>
 </file>
@@ -689,13 +707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,8 +753,14 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -768,19 +792,25 @@
         <v>0</v>
       </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -809,22 +839,28 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
-        <v>14</v>
+      <c r="L3">
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -853,22 +889,28 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -897,22 +939,28 @@
         <v>3</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>2</v>
       </c>
-      <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -941,22 +989,28 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>2</v>
       </c>
-      <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -985,22 +1039,28 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>126</v>
       </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7">
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1029,22 +1089,28 @@
         <v>6</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>126</v>
       </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8">
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8">
         <v>4</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1073,22 +1139,28 @@
         <v>7</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
         <v>212</v>
       </c>
-      <c r="L9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9">
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9">
         <v>4</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1117,22 +1189,28 @@
         <v>8</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
         <v>249</v>
       </c>
-      <c r="L10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10">
+      <c r="N10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10">
         <v>6</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1161,22 +1239,28 @@
         <v>9</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
         <v>350</v>
       </c>
-      <c r="L11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11">
+      <c r="N11" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11">
         <v>6</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1205,22 +1289,28 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>443</v>
       </c>
-      <c r="L12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12">
+      <c r="N12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12">
         <v>10</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1249,22 +1339,28 @@
         <v>11</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>443</v>
       </c>
-      <c r="L13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13">
+      <c r="N13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13">
         <v>10</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1293,22 +1389,28 @@
         <v>12</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>528</v>
       </c>
-      <c r="L14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14">
+      <c r="N14" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14">
         <v>14</v>
       </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1337,22 +1439,28 @@
         <v>13</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K15">
+        <v>13</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>753</v>
       </c>
-      <c r="L15" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15">
+      <c r="N15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15">
         <v>14</v>
       </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1381,22 +1489,28 @@
         <v>14</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>869</v>
       </c>
-      <c r="L16" t="s">
-        <v>27</v>
-      </c>
-      <c r="M16">
+      <c r="N16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16">
         <v>23</v>
       </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1425,22 +1539,28 @@
         <v>15</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K17">
+        <v>15</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>961</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17">
         <v>28</v>
       </c>
-      <c r="M17">
-        <v>28</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1469,22 +1589,28 @@
         <v>16</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K18">
+        <v>16</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>1125</v>
       </c>
-      <c r="L18" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18">
+      <c r="N18" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18">
         <v>34</v>
       </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="P18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1513,22 +1639,28 @@
         <v>17</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K19">
+        <v>17</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
         <v>1279</v>
       </c>
-      <c r="L19" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19">
+      <c r="N19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19">
         <v>39</v>
       </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1557,22 +1689,28 @@
         <v>18</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K20">
+        <v>18</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
         <v>1418</v>
       </c>
-      <c r="L20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M20">
+      <c r="N20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20">
         <v>41</v>
       </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="P20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1601,22 +1739,28 @@
         <v>19</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K21">
+        <v>19</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>1519</v>
       </c>
-      <c r="L21" t="s">
-        <v>32</v>
-      </c>
-      <c r="M21">
+      <c r="N21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O21">
         <v>41</v>
       </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1645,22 +1789,28 @@
         <v>20</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K22">
+        <v>20</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
         <v>1608</v>
       </c>
-      <c r="L22" t="s">
-        <v>33</v>
-      </c>
-      <c r="M22">
+      <c r="N22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22">
         <v>41</v>
       </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1689,22 +1839,28 @@
         <v>21</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="K23">
+        <v>21</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
         <v>1734</v>
       </c>
-      <c r="L23" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23">
+      <c r="N23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O23">
         <v>54</v>
       </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1733,22 +1889,28 @@
         <v>22</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K24">
+        <v>22</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <v>1878</v>
       </c>
-      <c r="L24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M24">
+      <c r="N24" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24">
         <v>65</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1777,22 +1939,28 @@
         <v>23</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K25">
+        <v>23</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>2009</v>
       </c>
-      <c r="L25" t="s">
-        <v>36</v>
-      </c>
-      <c r="M25">
+      <c r="N25" t="s">
+        <v>38</v>
+      </c>
+      <c r="O25">
         <v>71</v>
       </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1821,22 +1989,28 @@
         <v>24</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K26">
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>2144</v>
       </c>
-      <c r="L26" t="s">
-        <v>37</v>
-      </c>
-      <c r="M26">
+      <c r="N26" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26">
         <v>75</v>
       </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="P26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1865,22 +2039,28 @@
         <v>25</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K27">
+        <v>25</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
         <v>2144</v>
       </c>
-      <c r="L27" t="s">
-        <v>38</v>
-      </c>
-      <c r="M27">
+      <c r="N27" t="s">
+        <v>40</v>
+      </c>
+      <c r="O27">
         <v>75</v>
       </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1909,22 +2089,28 @@
         <v>26</v>
       </c>
       <c r="J28">
+        <v>26</v>
+      </c>
+      <c r="K28">
+        <v>26</v>
+      </c>
+      <c r="L28">
         <v>2224</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>2324</v>
       </c>
-      <c r="L28" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28">
+      <c r="N28" t="s">
+        <v>41</v>
+      </c>
+      <c r="O28">
         <v>100</v>
       </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1953,22 +2139,28 @@
         <v>27</v>
       </c>
       <c r="J29">
+        <v>27</v>
+      </c>
+      <c r="K29">
+        <v>27</v>
+      </c>
+      <c r="L29">
         <v>2343</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>2444</v>
       </c>
-      <c r="L29" t="s">
-        <v>40</v>
-      </c>
-      <c r="M29">
+      <c r="N29" t="s">
+        <v>42</v>
+      </c>
+      <c r="O29">
         <v>101</v>
       </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1997,22 +2189,28 @@
         <v>28</v>
       </c>
       <c r="J30">
+        <v>28</v>
+      </c>
+      <c r="K30">
+        <v>28</v>
+      </c>
+      <c r="L30">
         <v>2403</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>2509</v>
       </c>
-      <c r="L30" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30">
+      <c r="N30" t="s">
+        <v>43</v>
+      </c>
+      <c r="O30">
         <v>106</v>
       </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="P30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2041,22 +2239,28 @@
         <v>29</v>
       </c>
       <c r="J31">
+        <v>29</v>
+      </c>
+      <c r="K31">
+        <v>29</v>
+      </c>
+      <c r="L31">
         <v>2444</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>2559</v>
       </c>
-      <c r="L31" t="s">
-        <v>42</v>
-      </c>
-      <c r="M31">
+      <c r="N31" t="s">
+        <v>44</v>
+      </c>
+      <c r="O31">
         <v>115</v>
       </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2085,22 +2289,28 @@
         <v>30</v>
       </c>
       <c r="J32">
+        <v>30</v>
+      </c>
+      <c r="K32">
+        <v>30</v>
+      </c>
+      <c r="L32">
         <v>2444</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>2559</v>
       </c>
-      <c r="L32" t="s">
-        <v>43</v>
-      </c>
-      <c r="M32">
+      <c r="N32" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32">
         <v>115</v>
       </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="P32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2129,22 +2339,28 @@
         <v>31</v>
       </c>
       <c r="J33">
+        <v>31</v>
+      </c>
+      <c r="K33">
+        <v>31</v>
+      </c>
+      <c r="L33">
         <v>2614</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>2738</v>
       </c>
-      <c r="L33" t="s">
-        <v>44</v>
-      </c>
-      <c r="M33">
+      <c r="N33" t="s">
+        <v>46</v>
+      </c>
+      <c r="O33">
         <v>124</v>
       </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2173,22 +2389,28 @@
         <v>32</v>
       </c>
       <c r="J34">
+        <v>32</v>
+      </c>
+      <c r="K34">
+        <v>32</v>
+      </c>
+      <c r="L34">
         <v>2749</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>2882</v>
       </c>
-      <c r="L34" t="s">
-        <v>45</v>
-      </c>
-      <c r="M34">
+      <c r="N34" t="s">
+        <v>47</v>
+      </c>
+      <c r="O34">
         <v>133</v>
       </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2217,22 +2439,28 @@
         <v>33</v>
       </c>
       <c r="J35">
+        <v>33</v>
+      </c>
+      <c r="K35">
+        <v>33</v>
+      </c>
+      <c r="L35">
         <v>2803</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>2940</v>
       </c>
-      <c r="L35" t="s">
-        <v>46</v>
-      </c>
-      <c r="M35">
+      <c r="N35" t="s">
+        <v>48</v>
+      </c>
+      <c r="O35">
         <v>137</v>
       </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="P35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2261,22 +2489,28 @@
         <v>34</v>
       </c>
       <c r="J36">
+        <v>34</v>
+      </c>
+      <c r="K36">
+        <v>34</v>
+      </c>
+      <c r="L36">
         <v>2861</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>2998</v>
       </c>
-      <c r="L36" t="s">
-        <v>47</v>
-      </c>
-      <c r="M36">
+      <c r="N36" t="s">
+        <v>49</v>
+      </c>
+      <c r="O36">
         <v>137</v>
       </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="P36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2305,22 +2539,28 @@
         <v>35</v>
       </c>
       <c r="J37">
+        <v>35</v>
+      </c>
+      <c r="K37">
+        <v>35</v>
+      </c>
+      <c r="L37">
         <v>2958</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>3099</v>
       </c>
-      <c r="L37" t="s">
-        <v>48</v>
-      </c>
-      <c r="M37">
+      <c r="N37" t="s">
+        <v>50</v>
+      </c>
+      <c r="O37">
         <v>141</v>
       </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2349,22 +2589,28 @@
         <v>36</v>
       </c>
       <c r="J38">
+        <v>36</v>
+      </c>
+      <c r="K38">
+        <v>36</v>
+      </c>
+      <c r="L38">
         <v>3068</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>3218</v>
       </c>
-      <c r="L38" t="s">
-        <v>49</v>
-      </c>
-      <c r="M38">
+      <c r="N38" t="s">
+        <v>51</v>
+      </c>
+      <c r="O38">
         <v>150</v>
       </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2393,22 +2639,28 @@
         <v>37</v>
       </c>
       <c r="J39">
+        <v>37</v>
+      </c>
+      <c r="K39">
+        <v>37</v>
+      </c>
+      <c r="L39">
         <v>3151</v>
       </c>
-      <c r="K39">
+      <c r="M39">
         <v>3314</v>
       </c>
-      <c r="L39" t="s">
-        <v>50</v>
-      </c>
-      <c r="M39">
+      <c r="N39" t="s">
+        <v>52</v>
+      </c>
+      <c r="O39">
         <v>163</v>
       </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="P39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2437,22 +2689,28 @@
         <v>38</v>
       </c>
       <c r="J40">
+        <v>38</v>
+      </c>
+      <c r="K40">
+        <v>38</v>
+      </c>
+      <c r="L40">
         <v>3275</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>3443</v>
       </c>
-      <c r="L40" t="s">
-        <v>51</v>
-      </c>
-      <c r="M40">
+      <c r="N40" t="s">
+        <v>53</v>
+      </c>
+      <c r="O40">
         <v>168</v>
       </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2481,22 +2739,28 @@
         <v>39</v>
       </c>
       <c r="J41">
+        <v>39</v>
+      </c>
+      <c r="K41">
+        <v>39</v>
+      </c>
+      <c r="L41">
         <v>3396</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>3570</v>
       </c>
-      <c r="L41" t="s">
-        <v>52</v>
-      </c>
-      <c r="M41">
+      <c r="N41" t="s">
+        <v>54</v>
+      </c>
+      <c r="O41">
         <v>174</v>
       </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2525,22 +2789,28 @@
         <v>40</v>
       </c>
       <c r="J42">
+        <v>40</v>
+      </c>
+      <c r="K42">
+        <v>40</v>
+      </c>
+      <c r="L42">
         <v>3491</v>
       </c>
-      <c r="K42">
+      <c r="M42">
         <v>3665</v>
       </c>
-      <c r="L42" t="s">
-        <v>53</v>
-      </c>
-      <c r="M42">
+      <c r="N42" t="s">
+        <v>55</v>
+      </c>
+      <c r="O42">
         <v>174</v>
       </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2569,22 +2839,28 @@
         <v>41</v>
       </c>
       <c r="J43">
+        <v>41</v>
+      </c>
+      <c r="K43">
+        <v>41</v>
+      </c>
+      <c r="L43">
         <v>3543</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>3717</v>
       </c>
-      <c r="L43" t="s">
-        <v>54</v>
-      </c>
-      <c r="M43">
+      <c r="N43" t="s">
+        <v>56</v>
+      </c>
+      <c r="O43">
         <v>174</v>
       </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="P43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2613,22 +2889,28 @@
         <v>42</v>
       </c>
       <c r="J44">
+        <v>42</v>
+      </c>
+      <c r="K44">
+        <v>42</v>
+      </c>
+      <c r="L44">
         <v>3607</v>
       </c>
-      <c r="K44">
+      <c r="M44">
         <v>3793</v>
       </c>
-      <c r="L44" t="s">
-        <v>55</v>
-      </c>
-      <c r="M44">
+      <c r="N44" t="s">
+        <v>57</v>
+      </c>
+      <c r="O44">
         <v>186</v>
       </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="P44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2657,22 +2939,28 @@
         <v>43</v>
       </c>
       <c r="J45">
+        <v>43</v>
+      </c>
+      <c r="K45">
+        <v>43</v>
+      </c>
+      <c r="L45">
         <v>3695</v>
       </c>
-      <c r="K45">
+      <c r="M45">
         <v>3891</v>
       </c>
-      <c r="L45" t="s">
-        <v>56</v>
-      </c>
-      <c r="M45">
+      <c r="N45" t="s">
+        <v>58</v>
+      </c>
+      <c r="O45">
         <v>196</v>
       </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2701,22 +2989,28 @@
         <v>44</v>
       </c>
       <c r="J46">
+        <v>44</v>
+      </c>
+      <c r="K46">
+        <v>44</v>
+      </c>
+      <c r="L46">
         <v>3777</v>
       </c>
-      <c r="K46">
+      <c r="M46">
         <v>3979</v>
       </c>
-      <c r="L46" t="s">
-        <v>57</v>
-      </c>
-      <c r="M46">
+      <c r="N46" t="s">
+        <v>59</v>
+      </c>
+      <c r="O46">
         <v>202</v>
       </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="P46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2745,22 +3039,28 @@
         <v>45</v>
       </c>
       <c r="J47">
+        <v>45</v>
+      </c>
+      <c r="K47">
+        <v>45</v>
+      </c>
+      <c r="L47">
         <v>3912</v>
       </c>
-      <c r="K47">
+      <c r="M47">
         <v>4118</v>
       </c>
-      <c r="L47" t="s">
-        <v>58</v>
-      </c>
-      <c r="M47">
+      <c r="N47" t="s">
+        <v>60</v>
+      </c>
+      <c r="O47">
         <v>206</v>
       </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="P47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2789,22 +3089,28 @@
         <v>46</v>
       </c>
       <c r="J48">
+        <v>46</v>
+      </c>
+      <c r="K48">
+        <v>46</v>
+      </c>
+      <c r="L48">
         <v>4010</v>
       </c>
-      <c r="K48">
+      <c r="M48">
         <v>4225</v>
       </c>
-      <c r="L48" t="s">
-        <v>59</v>
-      </c>
-      <c r="M48">
+      <c r="N48" t="s">
+        <v>61</v>
+      </c>
+      <c r="O48">
         <v>215</v>
       </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2833,22 +3139,28 @@
         <v>47</v>
       </c>
       <c r="J49">
+        <v>47</v>
+      </c>
+      <c r="K49">
+        <v>47</v>
+      </c>
+      <c r="L49">
         <v>4056</v>
       </c>
-      <c r="K49">
+      <c r="M49">
         <v>4274</v>
       </c>
-      <c r="L49" t="s">
-        <v>60</v>
-      </c>
-      <c r="M49">
+      <c r="N49" t="s">
+        <v>62</v>
+      </c>
+      <c r="O49">
         <v>218</v>
       </c>
-      <c r="N49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="P49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2877,22 +3189,28 @@
         <v>48</v>
       </c>
       <c r="J50">
+        <v>48</v>
+      </c>
+      <c r="K50">
+        <v>48</v>
+      </c>
+      <c r="L50">
         <v>4188</v>
       </c>
-      <c r="K50">
+      <c r="M50">
         <v>4411</v>
       </c>
-      <c r="L50" t="s">
-        <v>61</v>
-      </c>
-      <c r="M50">
+      <c r="N50" t="s">
+        <v>63</v>
+      </c>
+      <c r="O50">
         <v>223</v>
       </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="P50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2921,22 +3239,28 @@
         <v>49</v>
       </c>
       <c r="J51">
+        <v>49</v>
+      </c>
+      <c r="K51">
+        <v>49</v>
+      </c>
+      <c r="L51">
         <v>4182</v>
       </c>
-      <c r="K51">
+      <c r="M51">
         <v>4408</v>
       </c>
-      <c r="L51" t="s">
-        <v>62</v>
-      </c>
-      <c r="M51">
+      <c r="N51" t="s">
+        <v>64</v>
+      </c>
+      <c r="O51">
         <v>226</v>
       </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="P51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2965,22 +3289,28 @@
         <v>50</v>
       </c>
       <c r="J52">
+        <v>50</v>
+      </c>
+      <c r="K52">
+        <v>50</v>
+      </c>
+      <c r="L52">
         <v>4235</v>
       </c>
-      <c r="K52">
+      <c r="M52">
         <v>4473</v>
       </c>
-      <c r="L52" t="s">
-        <v>63</v>
-      </c>
-      <c r="M52">
+      <c r="N52" t="s">
+        <v>65</v>
+      </c>
+      <c r="O52">
         <v>238</v>
       </c>
-      <c r="N52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="P52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3009,22 +3339,28 @@
         <v>51</v>
       </c>
       <c r="J53">
+        <v>51</v>
+      </c>
+      <c r="K53">
+        <v>51</v>
+      </c>
+      <c r="L53">
         <v>4328</v>
       </c>
-      <c r="K53">
+      <c r="M53">
         <v>4573</v>
       </c>
-      <c r="L53" t="s">
-        <v>64</v>
-      </c>
-      <c r="M53">
+      <c r="N53" t="s">
+        <v>66</v>
+      </c>
+      <c r="O53">
         <v>245</v>
       </c>
-      <c r="N53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="P53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3053,22 +3389,28 @@
         <v>52</v>
       </c>
       <c r="J54">
+        <v>52</v>
+      </c>
+      <c r="K54">
+        <v>52</v>
+      </c>
+      <c r="L54">
         <v>4328</v>
       </c>
-      <c r="K54">
+      <c r="M54">
         <v>4573</v>
       </c>
-      <c r="L54" t="s">
-        <v>65</v>
-      </c>
-      <c r="M54">
+      <c r="N54" t="s">
+        <v>67</v>
+      </c>
+      <c r="O54">
         <v>245</v>
       </c>
-      <c r="N54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="P54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3097,22 +3439,28 @@
         <v>53</v>
       </c>
       <c r="J55">
+        <v>53</v>
+      </c>
+      <c r="K55">
+        <v>53</v>
+      </c>
+      <c r="L55">
         <v>4448</v>
       </c>
-      <c r="K55">
+      <c r="M55">
         <v>4704</v>
       </c>
-      <c r="L55" t="s">
-        <v>66</v>
-      </c>
-      <c r="M55">
+      <c r="N55" t="s">
+        <v>68</v>
+      </c>
+      <c r="O55">
         <v>256</v>
       </c>
-      <c r="N55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="P55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3141,22 +3489,28 @@
         <v>54</v>
       </c>
       <c r="J56">
+        <v>54</v>
+      </c>
+      <c r="K56">
+        <v>54</v>
+      </c>
+      <c r="L56">
         <v>4490</v>
       </c>
-      <c r="K56">
+      <c r="M56">
         <v>4750</v>
       </c>
-      <c r="L56" t="s">
-        <v>67</v>
-      </c>
-      <c r="M56">
+      <c r="N56" t="s">
+        <v>69</v>
+      </c>
+      <c r="O56">
         <v>260</v>
       </c>
-      <c r="N56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="P56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3185,22 +3539,28 @@
         <v>55</v>
       </c>
       <c r="J57">
+        <v>55</v>
+      </c>
+      <c r="K57">
+        <v>55</v>
+      </c>
+      <c r="L57">
         <v>4502</v>
       </c>
-      <c r="K57">
+      <c r="M57">
         <v>4762</v>
       </c>
-      <c r="L57" t="s">
-        <v>68</v>
-      </c>
-      <c r="M57">
+      <c r="N57" t="s">
+        <v>70</v>
+      </c>
+      <c r="O57">
         <v>260</v>
       </c>
-      <c r="N57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+      <c r="P57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3229,22 +3589,28 @@
         <v>56</v>
       </c>
       <c r="J58">
+        <v>56</v>
+      </c>
+      <c r="K58">
+        <v>56</v>
+      </c>
+      <c r="L58">
         <v>4602</v>
       </c>
-      <c r="K58">
+      <c r="M58">
         <v>4869</v>
       </c>
-      <c r="L58" t="s">
-        <v>69</v>
-      </c>
-      <c r="M58">
+      <c r="N58" t="s">
+        <v>71</v>
+      </c>
+      <c r="O58">
         <v>267</v>
       </c>
-      <c r="N58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3273,22 +3639,28 @@
         <v>57</v>
       </c>
       <c r="J59">
+        <v>57</v>
+      </c>
+      <c r="K59">
+        <v>57</v>
+      </c>
+      <c r="L59">
         <v>4770</v>
       </c>
-      <c r="K59">
+      <c r="M59">
         <v>5045</v>
       </c>
-      <c r="L59" t="s">
-        <v>70</v>
-      </c>
-      <c r="M59">
+      <c r="N59" t="s">
+        <v>72</v>
+      </c>
+      <c r="O59">
         <v>275</v>
       </c>
-      <c r="N59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="P59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3317,22 +3689,28 @@
         <v>58</v>
       </c>
       <c r="J60">
+        <v>58</v>
+      </c>
+      <c r="K60">
+        <v>58</v>
+      </c>
+      <c r="L60">
         <v>4770</v>
       </c>
-      <c r="K60">
+      <c r="M60">
         <v>5045</v>
       </c>
-      <c r="L60" t="s">
-        <v>71</v>
-      </c>
-      <c r="M60">
+      <c r="N60" t="s">
+        <v>73</v>
+      </c>
+      <c r="O60">
         <v>275</v>
       </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+      <c r="P60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3361,22 +3739,28 @@
         <v>59</v>
       </c>
       <c r="J61">
+        <v>59</v>
+      </c>
+      <c r="K61">
+        <v>59</v>
+      </c>
+      <c r="L61">
         <v>4944</v>
       </c>
-      <c r="K61">
+      <c r="M61">
         <v>5235</v>
       </c>
-      <c r="L61" t="s">
-        <v>72</v>
-      </c>
-      <c r="M61">
+      <c r="N61" t="s">
+        <v>74</v>
+      </c>
+      <c r="O61">
         <v>291</v>
       </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3405,22 +3789,28 @@
         <v>60</v>
       </c>
       <c r="J62">
+        <v>60</v>
+      </c>
+      <c r="K62">
+        <v>60</v>
+      </c>
+      <c r="L62">
         <v>5005</v>
       </c>
-      <c r="K62">
+      <c r="M62">
         <v>5298</v>
       </c>
-      <c r="L62" t="s">
-        <v>73</v>
-      </c>
-      <c r="M62">
+      <c r="N62" t="s">
+        <v>75</v>
+      </c>
+      <c r="O62">
         <v>293</v>
       </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3449,22 +3839,28 @@
         <v>61</v>
       </c>
       <c r="J63">
+        <v>61</v>
+      </c>
+      <c r="K63">
+        <v>61</v>
+      </c>
+      <c r="L63">
         <v>5070</v>
       </c>
-      <c r="K63">
+      <c r="M63">
         <v>5366</v>
       </c>
-      <c r="L63" t="s">
-        <v>74</v>
-      </c>
-      <c r="M63">
+      <c r="N63" t="s">
+        <v>76</v>
+      </c>
+      <c r="O63">
         <v>296</v>
       </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="P63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3493,22 +3889,28 @@
         <v>62</v>
       </c>
       <c r="J64">
+        <v>62</v>
+      </c>
+      <c r="K64">
+        <v>62</v>
+      </c>
+      <c r="L64">
         <v>5167</v>
       </c>
-      <c r="K64">
+      <c r="M64">
         <v>5463</v>
       </c>
-      <c r="L64" t="s">
-        <v>75</v>
-      </c>
-      <c r="M64">
+      <c r="N64" t="s">
+        <v>77</v>
+      </c>
+      <c r="O64">
         <v>296</v>
       </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="P64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3537,22 +3939,28 @@
         <v>63</v>
       </c>
       <c r="J65">
+        <v>63</v>
+      </c>
+      <c r="K65">
+        <v>63</v>
+      </c>
+      <c r="L65">
         <v>5167</v>
       </c>
-      <c r="K65">
+      <c r="M65">
         <v>5463</v>
       </c>
-      <c r="L65" t="s">
-        <v>76</v>
-      </c>
-      <c r="M65">
+      <c r="N65" t="s">
+        <v>78</v>
+      </c>
+      <c r="O65">
         <v>296</v>
       </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="P65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3581,22 +3989,28 @@
         <v>64</v>
       </c>
       <c r="J66">
+        <v>64</v>
+      </c>
+      <c r="K66">
+        <v>64</v>
+      </c>
+      <c r="L66">
         <v>5336</v>
       </c>
-      <c r="K66">
+      <c r="M66">
         <v>5650</v>
       </c>
-      <c r="L66" t="s">
-        <v>77</v>
-      </c>
-      <c r="M66">
+      <c r="N66" t="s">
+        <v>79</v>
+      </c>
+      <c r="O66">
         <v>314</v>
       </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="P66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3625,22 +4039,28 @@
         <v>65</v>
       </c>
       <c r="J67">
+        <v>65</v>
+      </c>
+      <c r="K67">
+        <v>65</v>
+      </c>
+      <c r="L67">
         <v>5414</v>
       </c>
-      <c r="K67">
+      <c r="M67">
         <v>5734</v>
       </c>
-      <c r="L67" t="s">
-        <v>78</v>
-      </c>
-      <c r="M67">
+      <c r="N67" t="s">
+        <v>80</v>
+      </c>
+      <c r="O67">
         <v>320</v>
       </c>
-      <c r="N67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="P67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3669,22 +4089,28 @@
         <v>66</v>
       </c>
       <c r="J68">
+        <v>66</v>
+      </c>
+      <c r="K68">
+        <v>66</v>
+      </c>
+      <c r="L68">
         <v>5493</v>
       </c>
-      <c r="K68">
+      <c r="M68">
         <v>5815</v>
       </c>
-      <c r="L68" t="s">
-        <v>79</v>
-      </c>
-      <c r="M68">
+      <c r="N68" t="s">
+        <v>81</v>
+      </c>
+      <c r="O68">
         <v>322</v>
       </c>
-      <c r="N68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="P68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3713,22 +4139,28 @@
         <v>67</v>
       </c>
       <c r="J69">
+        <v>67</v>
+      </c>
+      <c r="K69">
+        <v>67</v>
+      </c>
+      <c r="L69">
         <v>5493</v>
       </c>
-      <c r="K69">
+      <c r="M69">
         <v>5815</v>
       </c>
-      <c r="L69" t="s">
-        <v>80</v>
-      </c>
-      <c r="M69">
+      <c r="N69" t="s">
+        <v>82</v>
+      </c>
+      <c r="O69">
         <v>322</v>
       </c>
-      <c r="N69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="P69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3757,22 +4189,28 @@
         <v>68</v>
       </c>
       <c r="J70">
+        <v>68</v>
+      </c>
+      <c r="K70">
+        <v>68</v>
+      </c>
+      <c r="L70">
         <v>5818</v>
       </c>
-      <c r="K70">
+      <c r="M70">
         <v>6140</v>
       </c>
-      <c r="L70" t="s">
-        <v>81</v>
-      </c>
-      <c r="M70">
+      <c r="N70" t="s">
+        <v>83</v>
+      </c>
+      <c r="O70">
         <v>322</v>
       </c>
-      <c r="N70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+      <c r="P70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3801,22 +4239,28 @@
         <v>69</v>
       </c>
       <c r="J71">
+        <v>69</v>
+      </c>
+      <c r="K71">
+        <v>69</v>
+      </c>
+      <c r="L71">
         <v>5853</v>
       </c>
-      <c r="K71">
+      <c r="M71">
         <v>6182</v>
       </c>
-      <c r="L71" t="s">
-        <v>82</v>
-      </c>
-      <c r="M71">
+      <c r="N71" t="s">
+        <v>84</v>
+      </c>
+      <c r="O71">
         <v>329</v>
       </c>
-      <c r="N71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="P71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3845,22 +4289,28 @@
         <v>70</v>
       </c>
       <c r="J72">
+        <v>70</v>
+      </c>
+      <c r="K72">
+        <v>70</v>
+      </c>
+      <c r="L72">
         <v>5897</v>
       </c>
-      <c r="K72">
+      <c r="M72">
         <v>6226</v>
       </c>
-      <c r="L72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M72">
+      <c r="N72" t="s">
+        <v>85</v>
+      </c>
+      <c r="O72">
         <v>329</v>
       </c>
-      <c r="N72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="P72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3889,22 +4339,28 @@
         <v>71</v>
       </c>
       <c r="J73">
+        <v>71</v>
+      </c>
+      <c r="K73">
+        <v>71</v>
+      </c>
+      <c r="L73">
         <v>5956</v>
       </c>
-      <c r="K73">
+      <c r="M73">
         <v>6287</v>
       </c>
-      <c r="L73" t="s">
-        <v>84</v>
-      </c>
-      <c r="M73">
+      <c r="N73" t="s">
+        <v>86</v>
+      </c>
+      <c r="O73">
         <v>331</v>
       </c>
-      <c r="N73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="P73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3933,22 +4389,28 @@
         <v>72</v>
       </c>
       <c r="J74">
+        <v>72</v>
+      </c>
+      <c r="K74">
+        <v>72</v>
+      </c>
+      <c r="L74">
         <v>6013</v>
       </c>
-      <c r="K74">
+      <c r="M74">
         <v>6352</v>
       </c>
-      <c r="L74" t="s">
-        <v>85</v>
-      </c>
-      <c r="M74">
+      <c r="N74" t="s">
+        <v>87</v>
+      </c>
+      <c r="O74">
         <v>339</v>
       </c>
-      <c r="N74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="P74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3977,22 +4439,28 @@
         <v>73</v>
       </c>
       <c r="J75">
+        <v>73</v>
+      </c>
+      <c r="K75">
+        <v>73</v>
+      </c>
+      <c r="L75">
         <v>6118</v>
       </c>
-      <c r="K75">
+      <c r="M75">
         <v>6457</v>
       </c>
-      <c r="L75" t="s">
-        <v>86</v>
-      </c>
-      <c r="M75">
+      <c r="N75" t="s">
+        <v>88</v>
+      </c>
+      <c r="O75">
         <v>339</v>
       </c>
-      <c r="N75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="P75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4021,22 +4489,28 @@
         <v>74</v>
       </c>
       <c r="J76">
+        <v>74</v>
+      </c>
+      <c r="K76">
+        <v>74</v>
+      </c>
+      <c r="L76">
         <v>6236</v>
       </c>
-      <c r="K76">
+      <c r="M76">
         <v>6579</v>
       </c>
-      <c r="L76" t="s">
-        <v>87</v>
-      </c>
-      <c r="M76">
+      <c r="N76" t="s">
+        <v>89</v>
+      </c>
+      <c r="O76">
         <v>343</v>
       </c>
-      <c r="N76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
+      <c r="P76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4065,22 +4539,28 @@
         <v>75</v>
       </c>
       <c r="J77">
+        <v>75</v>
+      </c>
+      <c r="K77">
+        <v>75</v>
+      </c>
+      <c r="L77">
         <v>6314</v>
       </c>
-      <c r="K77">
+      <c r="M77">
         <v>6657</v>
       </c>
-      <c r="L77" t="s">
-        <v>88</v>
-      </c>
-      <c r="M77">
+      <c r="N77" t="s">
+        <v>90</v>
+      </c>
+      <c r="O77">
         <v>343</v>
       </c>
-      <c r="N77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="P77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4109,22 +4589,28 @@
         <v>76</v>
       </c>
       <c r="J78">
+        <v>76</v>
+      </c>
+      <c r="K78">
+        <v>76</v>
+      </c>
+      <c r="L78">
         <v>6376</v>
       </c>
-      <c r="K78">
+      <c r="M78">
         <v>6719</v>
       </c>
-      <c r="L78" t="s">
-        <v>89</v>
-      </c>
-      <c r="M78">
+      <c r="N78" t="s">
+        <v>91</v>
+      </c>
+      <c r="O78">
         <v>343</v>
       </c>
-      <c r="N78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="P78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4153,22 +4639,28 @@
         <v>77</v>
       </c>
       <c r="J79">
+        <v>77</v>
+      </c>
+      <c r="K79">
+        <v>77</v>
+      </c>
+      <c r="L79">
         <v>6502</v>
       </c>
-      <c r="K79">
+      <c r="M79">
         <v>6845</v>
       </c>
-      <c r="L79" t="s">
-        <v>90</v>
-      </c>
-      <c r="M79">
+      <c r="N79" t="s">
+        <v>92</v>
+      </c>
+      <c r="O79">
         <v>343</v>
       </c>
-      <c r="N79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="P79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4197,22 +4689,28 @@
         <v>78</v>
       </c>
       <c r="J80">
+        <v>78</v>
+      </c>
+      <c r="K80">
+        <v>78</v>
+      </c>
+      <c r="L80">
         <v>6568</v>
       </c>
-      <c r="K80">
+      <c r="M80">
         <v>6923</v>
       </c>
-      <c r="L80" t="s">
-        <v>91</v>
-      </c>
-      <c r="M80">
+      <c r="N80" t="s">
+        <v>93</v>
+      </c>
+      <c r="O80">
         <v>355</v>
       </c>
-      <c r="N80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14">
+      <c r="P80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4241,22 +4739,28 @@
         <v>79</v>
       </c>
       <c r="J81">
+        <v>79</v>
+      </c>
+      <c r="K81">
+        <v>79</v>
+      </c>
+      <c r="L81">
         <v>6701</v>
       </c>
-      <c r="K81">
+      <c r="M81">
         <v>7056</v>
       </c>
-      <c r="L81" t="s">
-        <v>92</v>
-      </c>
-      <c r="M81">
+      <c r="N81" t="s">
+        <v>94</v>
+      </c>
+      <c r="O81">
         <v>355</v>
       </c>
-      <c r="N81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+      <c r="P81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4285,22 +4789,28 @@
         <v>80</v>
       </c>
       <c r="J82">
+        <v>80</v>
+      </c>
+      <c r="K82">
+        <v>80</v>
+      </c>
+      <c r="L82">
         <v>6829</v>
       </c>
-      <c r="K82">
+      <c r="M82">
         <v>7186</v>
       </c>
-      <c r="L82" t="s">
-        <v>93</v>
-      </c>
-      <c r="M82">
+      <c r="N82" t="s">
+        <v>95</v>
+      </c>
+      <c r="O82">
         <v>357</v>
       </c>
-      <c r="N82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="P82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4329,22 +4839,28 @@
         <v>81</v>
       </c>
       <c r="J83">
+        <v>81</v>
+      </c>
+      <c r="K83">
+        <v>81</v>
+      </c>
+      <c r="L83">
         <v>6973</v>
       </c>
-      <c r="K83">
+      <c r="M83">
         <v>7331</v>
       </c>
-      <c r="L83" t="s">
-        <v>94</v>
-      </c>
-      <c r="M83">
+      <c r="N83" t="s">
+        <v>96</v>
+      </c>
+      <c r="O83">
         <v>358</v>
       </c>
-      <c r="N83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="P83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4373,22 +4889,28 @@
         <v>82</v>
       </c>
       <c r="J84">
+        <v>82</v>
+      </c>
+      <c r="K84">
+        <v>82</v>
+      </c>
+      <c r="L84">
         <v>7124</v>
       </c>
-      <c r="K84">
+      <c r="M84">
         <v>7483</v>
       </c>
-      <c r="L84" t="s">
-        <v>95</v>
-      </c>
-      <c r="M84">
+      <c r="N84" t="s">
+        <v>97</v>
+      </c>
+      <c r="O84">
         <v>359</v>
       </c>
-      <c r="N84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="P84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4417,22 +4939,28 @@
         <v>83</v>
       </c>
       <c r="J85">
+        <v>83</v>
+      </c>
+      <c r="K85">
+        <v>83</v>
+      </c>
+      <c r="L85">
         <v>7229</v>
       </c>
-      <c r="K85">
+      <c r="M85">
         <v>7592</v>
       </c>
-      <c r="L85" t="s">
-        <v>96</v>
-      </c>
-      <c r="M85">
+      <c r="N85" t="s">
+        <v>98</v>
+      </c>
+      <c r="O85">
         <v>363</v>
       </c>
-      <c r="N85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
+      <c r="P85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4461,22 +4989,28 @@
         <v>84</v>
       </c>
       <c r="J86">
+        <v>84</v>
+      </c>
+      <c r="K86">
+        <v>84</v>
+      </c>
+      <c r="L86">
         <v>7434</v>
       </c>
-      <c r="K86">
+      <c r="M86">
         <v>7799</v>
       </c>
-      <c r="L86" t="s">
-        <v>97</v>
-      </c>
-      <c r="M86">
+      <c r="N86" t="s">
+        <v>99</v>
+      </c>
+      <c r="O86">
         <v>365</v>
       </c>
-      <c r="N86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14">
+      <c r="P86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4505,22 +5039,28 @@
         <v>85</v>
       </c>
       <c r="J87">
+        <v>85</v>
+      </c>
+      <c r="K87">
+        <v>85</v>
+      </c>
+      <c r="L87">
         <v>7548</v>
       </c>
-      <c r="K87">
+      <c r="M87">
         <v>7915</v>
       </c>
-      <c r="L87" t="s">
-        <v>98</v>
-      </c>
-      <c r="M87">
+      <c r="N87" t="s">
+        <v>100</v>
+      </c>
+      <c r="O87">
         <v>367</v>
       </c>
-      <c r="N87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="P87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4549,22 +5089,28 @@
         <v>86</v>
       </c>
       <c r="J88">
+        <v>86</v>
+      </c>
+      <c r="K88">
+        <v>86</v>
+      </c>
+      <c r="L88">
         <v>7725</v>
       </c>
-      <c r="K88">
+      <c r="M88">
         <v>8100</v>
       </c>
-      <c r="L88" t="s">
-        <v>99</v>
-      </c>
-      <c r="M88">
+      <c r="N88" t="s">
+        <v>101</v>
+      </c>
+      <c r="O88">
         <v>375</v>
       </c>
-      <c r="N88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="P88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4593,22 +5139,28 @@
         <v>87</v>
       </c>
       <c r="J89">
+        <v>87</v>
+      </c>
+      <c r="K89">
+        <v>87</v>
+      </c>
+      <c r="L89">
         <v>7937</v>
       </c>
-      <c r="K89">
+      <c r="M89">
         <v>8314</v>
       </c>
-      <c r="L89" t="s">
-        <v>100</v>
-      </c>
-      <c r="M89">
+      <c r="N89" t="s">
+        <v>102</v>
+      </c>
+      <c r="O89">
         <v>377</v>
       </c>
-      <c r="N89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="P89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4637,22 +5189,28 @@
         <v>88</v>
       </c>
       <c r="J90">
+        <v>88</v>
+      </c>
+      <c r="K90">
+        <v>88</v>
+      </c>
+      <c r="L90">
         <v>8179</v>
       </c>
-      <c r="K90">
+      <c r="M90">
         <v>8556</v>
       </c>
-      <c r="L90" t="s">
-        <v>101</v>
-      </c>
-      <c r="M90">
+      <c r="N90" t="s">
+        <v>103</v>
+      </c>
+      <c r="O90">
         <v>377</v>
       </c>
-      <c r="N90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="P90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4662,85 +5220,201 @@
       <c r="C91">
         <v>89</v>
       </c>
-      <c r="J91">
+      <c r="D91">
+        <v>89</v>
+      </c>
+      <c r="E91">
+        <v>89</v>
+      </c>
+      <c r="L91">
         <v>8357</v>
       </c>
-      <c r="K91">
+      <c r="M91">
         <v>8735</v>
       </c>
-      <c r="L91" t="s">
-        <v>102</v>
-      </c>
-      <c r="M91">
+      <c r="N91" t="s">
+        <v>104</v>
+      </c>
+      <c r="O91">
         <v>378</v>
       </c>
-      <c r="N91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14">
+      <c r="P91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92">
         <v>90</v>
       </c>
-      <c r="J92">
+      <c r="C92">
+        <v>90</v>
+      </c>
+      <c r="D92">
+        <v>90</v>
+      </c>
+      <c r="L92">
         <v>8436</v>
       </c>
-      <c r="K92">
+      <c r="M92">
         <v>8815</v>
       </c>
-      <c r="L92" t="s">
-        <v>103</v>
-      </c>
-      <c r="M92">
+      <c r="N92" t="s">
+        <v>105</v>
+      </c>
+      <c r="O92">
         <v>379</v>
       </c>
-      <c r="N92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14">
+      <c r="P92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93">
         <v>91</v>
       </c>
-      <c r="J93">
+      <c r="C93">
+        <v>91</v>
+      </c>
+      <c r="D93">
+        <v>91</v>
+      </c>
+      <c r="L93">
         <v>8777</v>
       </c>
-      <c r="K93">
+      <c r="M93">
         <v>9157</v>
       </c>
-      <c r="L93" t="s">
-        <v>104</v>
-      </c>
-      <c r="M93">
+      <c r="N93" t="s">
+        <v>106</v>
+      </c>
+      <c r="O93">
         <v>380</v>
       </c>
-      <c r="N93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14">
+      <c r="P93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="J94">
+      <c r="B94">
+        <v>92</v>
+      </c>
+      <c r="C94">
+        <v>92</v>
+      </c>
+      <c r="L94">
         <v>8932</v>
       </c>
-      <c r="K94">
+      <c r="M94">
         <v>9318</v>
       </c>
-      <c r="L94" t="s">
-        <v>105</v>
-      </c>
-      <c r="M94">
+      <c r="N94" t="s">
+        <v>107</v>
+      </c>
+      <c r="O94">
         <v>386</v>
       </c>
-      <c r="N94">
+      <c r="P94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>93</v>
+      </c>
+      <c r="L95">
+        <v>9148</v>
+      </c>
+      <c r="M95">
+        <v>9535</v>
+      </c>
+      <c r="N95" t="s">
+        <v>108</v>
+      </c>
+      <c r="O95">
+        <v>387</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>94</v>
+      </c>
+      <c r="L96">
+        <v>9462</v>
+      </c>
+      <c r="M96">
+        <v>9852</v>
+      </c>
+      <c r="N96" t="s">
+        <v>109</v>
+      </c>
+      <c r="O96">
+        <v>390</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>95</v>
+      </c>
+      <c r="L97">
+        <v>9862</v>
+      </c>
+      <c r="M97">
+        <v>10259</v>
+      </c>
+      <c r="N97" t="s">
+        <v>110</v>
+      </c>
+      <c r="O97">
+        <v>397</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>96</v>
+      </c>
+      <c r="L98">
+        <v>10088</v>
+      </c>
+      <c r="M98">
+        <v>10486</v>
+      </c>
+      <c r="N98" t="s">
+        <v>111</v>
+      </c>
+      <c r="O98">
+        <v>398</v>
+      </c>
+      <c r="P98">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed error in Utah county showing the wrong data.
</commit_message>
<xml_diff>
--- a/Clark_Data.xlsx
+++ b/Clark_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Active</t>
@@ -707,13 +716,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:S98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:19">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +768,17 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -798,19 +816,28 @@
         <v>0</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -845,22 +872,31 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
-        <v>16</v>
+      <c r="N3">
+        <v>1</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -895,22 +931,31 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -945,22 +990,31 @@
         <v>3</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>2</v>
       </c>
-      <c r="N5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -995,22 +1049,31 @@
         <v>4</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>2</v>
       </c>
-      <c r="N6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1045,22 +1108,31 @@
         <v>5</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>126</v>
       </c>
-      <c r="N7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7">
+      <c r="Q7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7">
         <v>2</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1095,22 +1167,31 @@
         <v>6</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>126</v>
       </c>
-      <c r="N8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8">
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8">
         <v>4</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1145,22 +1226,31 @@
         <v>7</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>212</v>
       </c>
-      <c r="N9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9">
+      <c r="Q9" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9">
         <v>4</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1195,22 +1285,31 @@
         <v>8</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
         <v>249</v>
       </c>
-      <c r="N10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10">
+      <c r="Q10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10">
         <v>6</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1245,22 +1344,31 @@
         <v>9</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>350</v>
       </c>
-      <c r="N11" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11">
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11">
         <v>6</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1295,22 +1403,31 @@
         <v>10</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>443</v>
       </c>
-      <c r="N12" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12">
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12">
         <v>10</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1345,22 +1462,31 @@
         <v>11</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M13">
+        <v>11</v>
+      </c>
+      <c r="N13">
+        <v>11</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
         <v>443</v>
       </c>
-      <c r="N13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13">
+      <c r="Q13" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13">
         <v>10</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1395,22 +1521,31 @@
         <v>12</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>528</v>
       </c>
-      <c r="N14" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14">
+      <c r="Q14" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14">
         <v>14</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1445,22 +1580,31 @@
         <v>13</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15">
+        <v>13</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
         <v>753</v>
       </c>
-      <c r="N15" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15">
+      <c r="Q15" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15">
         <v>14</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1495,22 +1639,31 @@
         <v>14</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M16">
+        <v>14</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
         <v>869</v>
       </c>
-      <c r="N16" t="s">
-        <v>29</v>
-      </c>
-      <c r="O16">
+      <c r="Q16" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16">
         <v>23</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1545,22 +1698,31 @@
         <v>15</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M17">
+        <v>15</v>
+      </c>
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>961</v>
       </c>
-      <c r="N17" t="s">
-        <v>30</v>
-      </c>
-      <c r="O17">
+      <c r="Q17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R17">
         <v>28</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1595,22 +1757,31 @@
         <v>16</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M18">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
         <v>1125</v>
       </c>
-      <c r="N18" t="s">
-        <v>31</v>
-      </c>
-      <c r="O18">
+      <c r="Q18" t="s">
         <v>34</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="R18">
+        <v>34</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1645,22 +1816,31 @@
         <v>17</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="M19">
+        <v>17</v>
+      </c>
+      <c r="N19">
+        <v>17</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
         <v>1279</v>
       </c>
-      <c r="N19" t="s">
-        <v>32</v>
-      </c>
-      <c r="O19">
+      <c r="Q19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19">
         <v>39</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1695,22 +1875,31 @@
         <v>18</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="M20">
+        <v>18</v>
+      </c>
+      <c r="N20">
+        <v>18</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
         <v>1418</v>
       </c>
-      <c r="N20" t="s">
-        <v>33</v>
-      </c>
-      <c r="O20">
+      <c r="Q20" t="s">
+        <v>36</v>
+      </c>
+      <c r="R20">
         <v>41</v>
       </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1745,22 +1934,31 @@
         <v>19</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="M21">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <v>19</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
         <v>1519</v>
       </c>
-      <c r="N21" t="s">
-        <v>34</v>
-      </c>
-      <c r="O21">
+      <c r="Q21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R21">
         <v>41</v>
       </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1795,22 +1993,31 @@
         <v>20</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
         <v>1608</v>
       </c>
-      <c r="N22" t="s">
-        <v>35</v>
-      </c>
-      <c r="O22">
+      <c r="Q22" t="s">
+        <v>38</v>
+      </c>
+      <c r="R22">
         <v>41</v>
       </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1845,22 +2052,31 @@
         <v>21</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="M23">
+        <v>21</v>
+      </c>
+      <c r="N23">
+        <v>21</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>1734</v>
       </c>
-      <c r="N23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23">
+      <c r="Q23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23">
         <v>54</v>
       </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1895,22 +2111,31 @@
         <v>22</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M24">
+        <v>22</v>
+      </c>
+      <c r="N24">
+        <v>22</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
         <v>1878</v>
       </c>
-      <c r="N24" t="s">
-        <v>37</v>
-      </c>
-      <c r="O24">
+      <c r="Q24" t="s">
+        <v>40</v>
+      </c>
+      <c r="R24">
         <v>65</v>
       </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1945,22 +2170,31 @@
         <v>23</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M25">
+        <v>23</v>
+      </c>
+      <c r="N25">
+        <v>23</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
         <v>2009</v>
       </c>
-      <c r="N25" t="s">
-        <v>38</v>
-      </c>
-      <c r="O25">
+      <c r="Q25" t="s">
+        <v>41</v>
+      </c>
+      <c r="R25">
         <v>71</v>
       </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1995,22 +2229,31 @@
         <v>24</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M26">
+        <v>24</v>
+      </c>
+      <c r="N26">
+        <v>24</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
         <v>2144</v>
       </c>
-      <c r="N26" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26">
+      <c r="Q26" t="s">
+        <v>42</v>
+      </c>
+      <c r="R26">
         <v>75</v>
       </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2045,22 +2288,31 @@
         <v>25</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M27">
+        <v>25</v>
+      </c>
+      <c r="N27">
+        <v>25</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
         <v>2144</v>
       </c>
-      <c r="N27" t="s">
-        <v>40</v>
-      </c>
-      <c r="O27">
+      <c r="Q27" t="s">
+        <v>43</v>
+      </c>
+      <c r="R27">
         <v>75</v>
       </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2095,22 +2347,31 @@
         <v>26</v>
       </c>
       <c r="L28">
+        <v>26</v>
+      </c>
+      <c r="M28">
+        <v>26</v>
+      </c>
+      <c r="N28">
+        <v>26</v>
+      </c>
+      <c r="O28">
         <v>2224</v>
       </c>
-      <c r="M28">
+      <c r="P28">
         <v>2324</v>
       </c>
-      <c r="N28" t="s">
-        <v>41</v>
-      </c>
-      <c r="O28">
+      <c r="Q28" t="s">
+        <v>44</v>
+      </c>
+      <c r="R28">
         <v>100</v>
       </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2145,22 +2406,31 @@
         <v>27</v>
       </c>
       <c r="L29">
+        <v>27</v>
+      </c>
+      <c r="M29">
+        <v>27</v>
+      </c>
+      <c r="N29">
+        <v>27</v>
+      </c>
+      <c r="O29">
         <v>2343</v>
       </c>
-      <c r="M29">
+      <c r="P29">
         <v>2444</v>
       </c>
-      <c r="N29" t="s">
-        <v>42</v>
-      </c>
-      <c r="O29">
+      <c r="Q29" t="s">
+        <v>45</v>
+      </c>
+      <c r="R29">
         <v>101</v>
       </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2195,22 +2465,31 @@
         <v>28</v>
       </c>
       <c r="L30">
+        <v>28</v>
+      </c>
+      <c r="M30">
+        <v>28</v>
+      </c>
+      <c r="N30">
+        <v>28</v>
+      </c>
+      <c r="O30">
         <v>2403</v>
       </c>
-      <c r="M30">
+      <c r="P30">
         <v>2509</v>
       </c>
-      <c r="N30" t="s">
-        <v>43</v>
-      </c>
-      <c r="O30">
+      <c r="Q30" t="s">
+        <v>46</v>
+      </c>
+      <c r="R30">
         <v>106</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2245,22 +2524,31 @@
         <v>29</v>
       </c>
       <c r="L31">
+        <v>29</v>
+      </c>
+      <c r="M31">
+        <v>29</v>
+      </c>
+      <c r="N31">
+        <v>29</v>
+      </c>
+      <c r="O31">
         <v>2444</v>
       </c>
-      <c r="M31">
+      <c r="P31">
         <v>2559</v>
       </c>
-      <c r="N31" t="s">
-        <v>44</v>
-      </c>
-      <c r="O31">
+      <c r="Q31" t="s">
+        <v>47</v>
+      </c>
+      <c r="R31">
         <v>115</v>
       </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="S31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2295,22 +2583,31 @@
         <v>30</v>
       </c>
       <c r="L32">
+        <v>30</v>
+      </c>
+      <c r="M32">
+        <v>30</v>
+      </c>
+      <c r="N32">
+        <v>30</v>
+      </c>
+      <c r="O32">
         <v>2444</v>
       </c>
-      <c r="M32">
+      <c r="P32">
         <v>2559</v>
       </c>
-      <c r="N32" t="s">
-        <v>45</v>
-      </c>
-      <c r="O32">
+      <c r="Q32" t="s">
+        <v>48</v>
+      </c>
+      <c r="R32">
         <v>115</v>
       </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="S32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2345,22 +2642,31 @@
         <v>31</v>
       </c>
       <c r="L33">
+        <v>31</v>
+      </c>
+      <c r="M33">
+        <v>31</v>
+      </c>
+      <c r="N33">
+        <v>31</v>
+      </c>
+      <c r="O33">
         <v>2614</v>
       </c>
-      <c r="M33">
+      <c r="P33">
         <v>2738</v>
       </c>
-      <c r="N33" t="s">
-        <v>46</v>
-      </c>
-      <c r="O33">
+      <c r="Q33" t="s">
+        <v>49</v>
+      </c>
+      <c r="R33">
         <v>124</v>
       </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2395,22 +2701,31 @@
         <v>32</v>
       </c>
       <c r="L34">
+        <v>32</v>
+      </c>
+      <c r="M34">
+        <v>32</v>
+      </c>
+      <c r="N34">
+        <v>32</v>
+      </c>
+      <c r="O34">
         <v>2749</v>
       </c>
-      <c r="M34">
+      <c r="P34">
         <v>2882</v>
       </c>
-      <c r="N34" t="s">
-        <v>47</v>
-      </c>
-      <c r="O34">
+      <c r="Q34" t="s">
+        <v>50</v>
+      </c>
+      <c r="R34">
         <v>133</v>
       </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2445,22 +2760,31 @@
         <v>33</v>
       </c>
       <c r="L35">
+        <v>33</v>
+      </c>
+      <c r="M35">
+        <v>33</v>
+      </c>
+      <c r="N35">
+        <v>33</v>
+      </c>
+      <c r="O35">
         <v>2803</v>
       </c>
-      <c r="M35">
+      <c r="P35">
         <v>2940</v>
       </c>
-      <c r="N35" t="s">
-        <v>48</v>
-      </c>
-      <c r="O35">
+      <c r="Q35" t="s">
+        <v>51</v>
+      </c>
+      <c r="R35">
         <v>137</v>
       </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2495,22 +2819,31 @@
         <v>34</v>
       </c>
       <c r="L36">
+        <v>34</v>
+      </c>
+      <c r="M36">
+        <v>34</v>
+      </c>
+      <c r="N36">
+        <v>34</v>
+      </c>
+      <c r="O36">
         <v>2861</v>
       </c>
-      <c r="M36">
+      <c r="P36">
         <v>2998</v>
       </c>
-      <c r="N36" t="s">
-        <v>49</v>
-      </c>
-      <c r="O36">
+      <c r="Q36" t="s">
+        <v>52</v>
+      </c>
+      <c r="R36">
         <v>137</v>
       </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="S36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2545,22 +2878,31 @@
         <v>35</v>
       </c>
       <c r="L37">
+        <v>35</v>
+      </c>
+      <c r="M37">
+        <v>35</v>
+      </c>
+      <c r="N37">
+        <v>35</v>
+      </c>
+      <c r="O37">
         <v>2958</v>
       </c>
-      <c r="M37">
+      <c r="P37">
         <v>3099</v>
       </c>
-      <c r="N37" t="s">
-        <v>50</v>
-      </c>
-      <c r="O37">
+      <c r="Q37" t="s">
+        <v>53</v>
+      </c>
+      <c r="R37">
         <v>141</v>
       </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="S37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2595,22 +2937,31 @@
         <v>36</v>
       </c>
       <c r="L38">
+        <v>36</v>
+      </c>
+      <c r="M38">
+        <v>36</v>
+      </c>
+      <c r="N38">
+        <v>36</v>
+      </c>
+      <c r="O38">
         <v>3068</v>
       </c>
-      <c r="M38">
+      <c r="P38">
         <v>3218</v>
       </c>
-      <c r="N38" t="s">
-        <v>51</v>
-      </c>
-      <c r="O38">
+      <c r="Q38" t="s">
+        <v>54</v>
+      </c>
+      <c r="R38">
         <v>150</v>
       </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="S38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2645,22 +2996,31 @@
         <v>37</v>
       </c>
       <c r="L39">
+        <v>37</v>
+      </c>
+      <c r="M39">
+        <v>37</v>
+      </c>
+      <c r="N39">
+        <v>37</v>
+      </c>
+      <c r="O39">
         <v>3151</v>
       </c>
-      <c r="M39">
+      <c r="P39">
         <v>3314</v>
       </c>
-      <c r="N39" t="s">
-        <v>52</v>
-      </c>
-      <c r="O39">
+      <c r="Q39" t="s">
+        <v>55</v>
+      </c>
+      <c r="R39">
         <v>163</v>
       </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2695,22 +3055,31 @@
         <v>38</v>
       </c>
       <c r="L40">
+        <v>38</v>
+      </c>
+      <c r="M40">
+        <v>38</v>
+      </c>
+      <c r="N40">
+        <v>38</v>
+      </c>
+      <c r="O40">
         <v>3275</v>
       </c>
-      <c r="M40">
+      <c r="P40">
         <v>3443</v>
       </c>
-      <c r="N40" t="s">
-        <v>53</v>
-      </c>
-      <c r="O40">
+      <c r="Q40" t="s">
+        <v>56</v>
+      </c>
+      <c r="R40">
         <v>168</v>
       </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="S40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2745,22 +3114,31 @@
         <v>39</v>
       </c>
       <c r="L41">
+        <v>39</v>
+      </c>
+      <c r="M41">
+        <v>39</v>
+      </c>
+      <c r="N41">
+        <v>39</v>
+      </c>
+      <c r="O41">
         <v>3396</v>
       </c>
-      <c r="M41">
+      <c r="P41">
         <v>3570</v>
       </c>
-      <c r="N41" t="s">
-        <v>54</v>
-      </c>
-      <c r="O41">
+      <c r="Q41" t="s">
+        <v>57</v>
+      </c>
+      <c r="R41">
         <v>174</v>
       </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="S41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2795,22 +3173,31 @@
         <v>40</v>
       </c>
       <c r="L42">
+        <v>40</v>
+      </c>
+      <c r="M42">
+        <v>40</v>
+      </c>
+      <c r="N42">
+        <v>40</v>
+      </c>
+      <c r="O42">
         <v>3491</v>
       </c>
-      <c r="M42">
+      <c r="P42">
         <v>3665</v>
       </c>
-      <c r="N42" t="s">
-        <v>55</v>
-      </c>
-      <c r="O42">
+      <c r="Q42" t="s">
+        <v>58</v>
+      </c>
+      <c r="R42">
         <v>174</v>
       </c>
-      <c r="P42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="S42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2845,22 +3232,31 @@
         <v>41</v>
       </c>
       <c r="L43">
+        <v>41</v>
+      </c>
+      <c r="M43">
+        <v>41</v>
+      </c>
+      <c r="N43">
+        <v>41</v>
+      </c>
+      <c r="O43">
         <v>3543</v>
       </c>
-      <c r="M43">
+      <c r="P43">
         <v>3717</v>
       </c>
-      <c r="N43" t="s">
-        <v>56</v>
-      </c>
-      <c r="O43">
+      <c r="Q43" t="s">
+        <v>59</v>
+      </c>
+      <c r="R43">
         <v>174</v>
       </c>
-      <c r="P43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="S43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2895,22 +3291,31 @@
         <v>42</v>
       </c>
       <c r="L44">
+        <v>42</v>
+      </c>
+      <c r="M44">
+        <v>42</v>
+      </c>
+      <c r="N44">
+        <v>42</v>
+      </c>
+      <c r="O44">
         <v>3607</v>
       </c>
-      <c r="M44">
+      <c r="P44">
         <v>3793</v>
       </c>
-      <c r="N44" t="s">
-        <v>57</v>
-      </c>
-      <c r="O44">
+      <c r="Q44" t="s">
+        <v>60</v>
+      </c>
+      <c r="R44">
         <v>186</v>
       </c>
-      <c r="P44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="S44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2945,22 +3350,31 @@
         <v>43</v>
       </c>
       <c r="L45">
+        <v>43</v>
+      </c>
+      <c r="M45">
+        <v>43</v>
+      </c>
+      <c r="N45">
+        <v>43</v>
+      </c>
+      <c r="O45">
         <v>3695</v>
       </c>
-      <c r="M45">
+      <c r="P45">
         <v>3891</v>
       </c>
-      <c r="N45" t="s">
-        <v>58</v>
-      </c>
-      <c r="O45">
+      <c r="Q45" t="s">
+        <v>61</v>
+      </c>
+      <c r="R45">
         <v>196</v>
       </c>
-      <c r="P45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="S45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2995,22 +3409,31 @@
         <v>44</v>
       </c>
       <c r="L46">
+        <v>44</v>
+      </c>
+      <c r="M46">
+        <v>44</v>
+      </c>
+      <c r="N46">
+        <v>44</v>
+      </c>
+      <c r="O46">
         <v>3777</v>
       </c>
-      <c r="M46">
+      <c r="P46">
         <v>3979</v>
       </c>
-      <c r="N46" t="s">
-        <v>59</v>
-      </c>
-      <c r="O46">
+      <c r="Q46" t="s">
+        <v>62</v>
+      </c>
+      <c r="R46">
         <v>202</v>
       </c>
-      <c r="P46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="S46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3045,22 +3468,31 @@
         <v>45</v>
       </c>
       <c r="L47">
+        <v>45</v>
+      </c>
+      <c r="M47">
+        <v>45</v>
+      </c>
+      <c r="N47">
+        <v>45</v>
+      </c>
+      <c r="O47">
         <v>3912</v>
       </c>
-      <c r="M47">
+      <c r="P47">
         <v>4118</v>
       </c>
-      <c r="N47" t="s">
-        <v>60</v>
-      </c>
-      <c r="O47">
+      <c r="Q47" t="s">
+        <v>63</v>
+      </c>
+      <c r="R47">
         <v>206</v>
       </c>
-      <c r="P47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="S47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3095,22 +3527,31 @@
         <v>46</v>
       </c>
       <c r="L48">
+        <v>46</v>
+      </c>
+      <c r="M48">
+        <v>46</v>
+      </c>
+      <c r="N48">
+        <v>46</v>
+      </c>
+      <c r="O48">
         <v>4010</v>
       </c>
-      <c r="M48">
+      <c r="P48">
         <v>4225</v>
       </c>
-      <c r="N48" t="s">
-        <v>61</v>
-      </c>
-      <c r="O48">
+      <c r="Q48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R48">
         <v>215</v>
       </c>
-      <c r="P48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="S48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3145,22 +3586,31 @@
         <v>47</v>
       </c>
       <c r="L49">
+        <v>47</v>
+      </c>
+      <c r="M49">
+        <v>47</v>
+      </c>
+      <c r="N49">
+        <v>47</v>
+      </c>
+      <c r="O49">
         <v>4056</v>
       </c>
-      <c r="M49">
+      <c r="P49">
         <v>4274</v>
       </c>
-      <c r="N49" t="s">
-        <v>62</v>
-      </c>
-      <c r="O49">
+      <c r="Q49" t="s">
+        <v>65</v>
+      </c>
+      <c r="R49">
         <v>218</v>
       </c>
-      <c r="P49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
+      <c r="S49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3195,22 +3645,31 @@
         <v>48</v>
       </c>
       <c r="L50">
+        <v>48</v>
+      </c>
+      <c r="M50">
+        <v>48</v>
+      </c>
+      <c r="N50">
+        <v>48</v>
+      </c>
+      <c r="O50">
         <v>4188</v>
       </c>
-      <c r="M50">
+      <c r="P50">
         <v>4411</v>
       </c>
-      <c r="N50" t="s">
-        <v>63</v>
-      </c>
-      <c r="O50">
+      <c r="Q50" t="s">
+        <v>66</v>
+      </c>
+      <c r="R50">
         <v>223</v>
       </c>
-      <c r="P50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="S50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3245,22 +3704,31 @@
         <v>49</v>
       </c>
       <c r="L51">
+        <v>49</v>
+      </c>
+      <c r="M51">
+        <v>49</v>
+      </c>
+      <c r="N51">
+        <v>49</v>
+      </c>
+      <c r="O51">
         <v>4182</v>
       </c>
-      <c r="M51">
+      <c r="P51">
         <v>4408</v>
       </c>
-      <c r="N51" t="s">
-        <v>64</v>
-      </c>
-      <c r="O51">
+      <c r="Q51" t="s">
+        <v>67</v>
+      </c>
+      <c r="R51">
         <v>226</v>
       </c>
-      <c r="P51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="S51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3295,22 +3763,31 @@
         <v>50</v>
       </c>
       <c r="L52">
+        <v>50</v>
+      </c>
+      <c r="M52">
+        <v>50</v>
+      </c>
+      <c r="N52">
+        <v>50</v>
+      </c>
+      <c r="O52">
         <v>4235</v>
       </c>
-      <c r="M52">
+      <c r="P52">
         <v>4473</v>
       </c>
-      <c r="N52" t="s">
-        <v>65</v>
-      </c>
-      <c r="O52">
+      <c r="Q52" t="s">
+        <v>68</v>
+      </c>
+      <c r="R52">
         <v>238</v>
       </c>
-      <c r="P52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="S52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3345,22 +3822,31 @@
         <v>51</v>
       </c>
       <c r="L53">
+        <v>51</v>
+      </c>
+      <c r="M53">
+        <v>51</v>
+      </c>
+      <c r="N53">
+        <v>51</v>
+      </c>
+      <c r="O53">
         <v>4328</v>
       </c>
-      <c r="M53">
+      <c r="P53">
         <v>4573</v>
       </c>
-      <c r="N53" t="s">
-        <v>66</v>
-      </c>
-      <c r="O53">
+      <c r="Q53" t="s">
+        <v>69</v>
+      </c>
+      <c r="R53">
         <v>245</v>
       </c>
-      <c r="P53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
+      <c r="S53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3395,22 +3881,31 @@
         <v>52</v>
       </c>
       <c r="L54">
+        <v>52</v>
+      </c>
+      <c r="M54">
+        <v>52</v>
+      </c>
+      <c r="N54">
+        <v>52</v>
+      </c>
+      <c r="O54">
         <v>4328</v>
       </c>
-      <c r="M54">
+      <c r="P54">
         <v>4573</v>
       </c>
-      <c r="N54" t="s">
-        <v>67</v>
-      </c>
-      <c r="O54">
+      <c r="Q54" t="s">
+        <v>70</v>
+      </c>
+      <c r="R54">
         <v>245</v>
       </c>
-      <c r="P54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16">
+      <c r="S54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3445,22 +3940,31 @@
         <v>53</v>
       </c>
       <c r="L55">
+        <v>53</v>
+      </c>
+      <c r="M55">
+        <v>53</v>
+      </c>
+      <c r="N55">
+        <v>53</v>
+      </c>
+      <c r="O55">
         <v>4448</v>
       </c>
-      <c r="M55">
+      <c r="P55">
         <v>4704</v>
       </c>
-      <c r="N55" t="s">
-        <v>68</v>
-      </c>
-      <c r="O55">
+      <c r="Q55" t="s">
+        <v>71</v>
+      </c>
+      <c r="R55">
         <v>256</v>
       </c>
-      <c r="P55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16">
+      <c r="S55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3495,22 +3999,31 @@
         <v>54</v>
       </c>
       <c r="L56">
+        <v>54</v>
+      </c>
+      <c r="M56">
+        <v>54</v>
+      </c>
+      <c r="N56">
+        <v>54</v>
+      </c>
+      <c r="O56">
         <v>4490</v>
       </c>
-      <c r="M56">
+      <c r="P56">
         <v>4750</v>
       </c>
-      <c r="N56" t="s">
-        <v>69</v>
-      </c>
-      <c r="O56">
+      <c r="Q56" t="s">
+        <v>72</v>
+      </c>
+      <c r="R56">
         <v>260</v>
       </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="S56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3545,22 +4058,31 @@
         <v>55</v>
       </c>
       <c r="L57">
+        <v>55</v>
+      </c>
+      <c r="M57">
+        <v>55</v>
+      </c>
+      <c r="N57">
+        <v>55</v>
+      </c>
+      <c r="O57">
         <v>4502</v>
       </c>
-      <c r="M57">
+      <c r="P57">
         <v>4762</v>
       </c>
-      <c r="N57" t="s">
-        <v>70</v>
-      </c>
-      <c r="O57">
+      <c r="Q57" t="s">
+        <v>73</v>
+      </c>
+      <c r="R57">
         <v>260</v>
       </c>
-      <c r="P57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="S57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3595,22 +4117,31 @@
         <v>56</v>
       </c>
       <c r="L58">
+        <v>56</v>
+      </c>
+      <c r="M58">
+        <v>56</v>
+      </c>
+      <c r="N58">
+        <v>56</v>
+      </c>
+      <c r="O58">
         <v>4602</v>
       </c>
-      <c r="M58">
+      <c r="P58">
         <v>4869</v>
       </c>
-      <c r="N58" t="s">
-        <v>71</v>
-      </c>
-      <c r="O58">
+      <c r="Q58" t="s">
+        <v>74</v>
+      </c>
+      <c r="R58">
         <v>267</v>
       </c>
-      <c r="P58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="S58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3645,22 +4176,31 @@
         <v>57</v>
       </c>
       <c r="L59">
+        <v>57</v>
+      </c>
+      <c r="M59">
+        <v>57</v>
+      </c>
+      <c r="N59">
+        <v>57</v>
+      </c>
+      <c r="O59">
         <v>4770</v>
       </c>
-      <c r="M59">
+      <c r="P59">
         <v>5045</v>
       </c>
-      <c r="N59" t="s">
-        <v>72</v>
-      </c>
-      <c r="O59">
+      <c r="Q59" t="s">
+        <v>75</v>
+      </c>
+      <c r="R59">
         <v>275</v>
       </c>
-      <c r="P59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="S59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3695,22 +4235,31 @@
         <v>58</v>
       </c>
       <c r="L60">
+        <v>58</v>
+      </c>
+      <c r="M60">
+        <v>58</v>
+      </c>
+      <c r="N60">
+        <v>58</v>
+      </c>
+      <c r="O60">
         <v>4770</v>
       </c>
-      <c r="M60">
+      <c r="P60">
         <v>5045</v>
       </c>
-      <c r="N60" t="s">
-        <v>73</v>
-      </c>
-      <c r="O60">
+      <c r="Q60" t="s">
+        <v>76</v>
+      </c>
+      <c r="R60">
         <v>275</v>
       </c>
-      <c r="P60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="S60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3745,22 +4294,31 @@
         <v>59</v>
       </c>
       <c r="L61">
+        <v>59</v>
+      </c>
+      <c r="M61">
+        <v>59</v>
+      </c>
+      <c r="N61">
+        <v>59</v>
+      </c>
+      <c r="O61">
         <v>4944</v>
       </c>
-      <c r="M61">
+      <c r="P61">
         <v>5235</v>
       </c>
-      <c r="N61" t="s">
-        <v>74</v>
-      </c>
-      <c r="O61">
+      <c r="Q61" t="s">
+        <v>77</v>
+      </c>
+      <c r="R61">
         <v>291</v>
       </c>
-      <c r="P61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="S61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3795,22 +4353,31 @@
         <v>60</v>
       </c>
       <c r="L62">
+        <v>60</v>
+      </c>
+      <c r="M62">
+        <v>60</v>
+      </c>
+      <c r="N62">
+        <v>60</v>
+      </c>
+      <c r="O62">
         <v>5005</v>
       </c>
-      <c r="M62">
+      <c r="P62">
         <v>5298</v>
       </c>
-      <c r="N62" t="s">
-        <v>75</v>
-      </c>
-      <c r="O62">
+      <c r="Q62" t="s">
+        <v>78</v>
+      </c>
+      <c r="R62">
         <v>293</v>
       </c>
-      <c r="P62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="S62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3845,22 +4412,31 @@
         <v>61</v>
       </c>
       <c r="L63">
+        <v>61</v>
+      </c>
+      <c r="M63">
+        <v>61</v>
+      </c>
+      <c r="N63">
+        <v>61</v>
+      </c>
+      <c r="O63">
         <v>5070</v>
       </c>
-      <c r="M63">
+      <c r="P63">
         <v>5366</v>
       </c>
-      <c r="N63" t="s">
-        <v>76</v>
-      </c>
-      <c r="O63">
+      <c r="Q63" t="s">
+        <v>79</v>
+      </c>
+      <c r="R63">
         <v>296</v>
       </c>
-      <c r="P63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="S63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3895,22 +4471,31 @@
         <v>62</v>
       </c>
       <c r="L64">
+        <v>62</v>
+      </c>
+      <c r="M64">
+        <v>62</v>
+      </c>
+      <c r="N64">
+        <v>62</v>
+      </c>
+      <c r="O64">
         <v>5167</v>
       </c>
-      <c r="M64">
+      <c r="P64">
         <v>5463</v>
       </c>
-      <c r="N64" t="s">
-        <v>77</v>
-      </c>
-      <c r="O64">
+      <c r="Q64" t="s">
+        <v>80</v>
+      </c>
+      <c r="R64">
         <v>296</v>
       </c>
-      <c r="P64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="S64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3945,22 +4530,31 @@
         <v>63</v>
       </c>
       <c r="L65">
+        <v>63</v>
+      </c>
+      <c r="M65">
+        <v>63</v>
+      </c>
+      <c r="N65">
+        <v>63</v>
+      </c>
+      <c r="O65">
         <v>5167</v>
       </c>
-      <c r="M65">
+      <c r="P65">
         <v>5463</v>
       </c>
-      <c r="N65" t="s">
-        <v>78</v>
-      </c>
-      <c r="O65">
+      <c r="Q65" t="s">
+        <v>81</v>
+      </c>
+      <c r="R65">
         <v>296</v>
       </c>
-      <c r="P65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="S65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3995,22 +4589,31 @@
         <v>64</v>
       </c>
       <c r="L66">
+        <v>64</v>
+      </c>
+      <c r="M66">
+        <v>64</v>
+      </c>
+      <c r="N66">
+        <v>64</v>
+      </c>
+      <c r="O66">
         <v>5336</v>
       </c>
-      <c r="M66">
+      <c r="P66">
         <v>5650</v>
       </c>
-      <c r="N66" t="s">
-        <v>79</v>
-      </c>
-      <c r="O66">
+      <c r="Q66" t="s">
+        <v>82</v>
+      </c>
+      <c r="R66">
         <v>314</v>
       </c>
-      <c r="P66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="S66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4045,22 +4648,31 @@
         <v>65</v>
       </c>
       <c r="L67">
+        <v>65</v>
+      </c>
+      <c r="M67">
+        <v>65</v>
+      </c>
+      <c r="N67">
+        <v>65</v>
+      </c>
+      <c r="O67">
         <v>5414</v>
       </c>
-      <c r="M67">
+      <c r="P67">
         <v>5734</v>
       </c>
-      <c r="N67" t="s">
-        <v>80</v>
-      </c>
-      <c r="O67">
+      <c r="Q67" t="s">
+        <v>83</v>
+      </c>
+      <c r="R67">
         <v>320</v>
       </c>
-      <c r="P67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16">
+      <c r="S67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4095,22 +4707,31 @@
         <v>66</v>
       </c>
       <c r="L68">
+        <v>66</v>
+      </c>
+      <c r="M68">
+        <v>66</v>
+      </c>
+      <c r="N68">
+        <v>66</v>
+      </c>
+      <c r="O68">
         <v>5493</v>
       </c>
-      <c r="M68">
+      <c r="P68">
         <v>5815</v>
       </c>
-      <c r="N68" t="s">
-        <v>81</v>
-      </c>
-      <c r="O68">
+      <c r="Q68" t="s">
+        <v>84</v>
+      </c>
+      <c r="R68">
         <v>322</v>
       </c>
-      <c r="P68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16">
+      <c r="S68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4145,22 +4766,31 @@
         <v>67</v>
       </c>
       <c r="L69">
+        <v>67</v>
+      </c>
+      <c r="M69">
+        <v>67</v>
+      </c>
+      <c r="N69">
+        <v>67</v>
+      </c>
+      <c r="O69">
         <v>5493</v>
       </c>
-      <c r="M69">
+      <c r="P69">
         <v>5815</v>
       </c>
-      <c r="N69" t="s">
-        <v>82</v>
-      </c>
-      <c r="O69">
+      <c r="Q69" t="s">
+        <v>85</v>
+      </c>
+      <c r="R69">
         <v>322</v>
       </c>
-      <c r="P69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16">
+      <c r="S69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4195,22 +4825,31 @@
         <v>68</v>
       </c>
       <c r="L70">
+        <v>68</v>
+      </c>
+      <c r="M70">
+        <v>68</v>
+      </c>
+      <c r="N70">
+        <v>68</v>
+      </c>
+      <c r="O70">
         <v>5818</v>
       </c>
-      <c r="M70">
+      <c r="P70">
         <v>6140</v>
       </c>
-      <c r="N70" t="s">
-        <v>83</v>
-      </c>
-      <c r="O70">
+      <c r="Q70" t="s">
+        <v>86</v>
+      </c>
+      <c r="R70">
         <v>322</v>
       </c>
-      <c r="P70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16">
+      <c r="S70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4245,22 +4884,31 @@
         <v>69</v>
       </c>
       <c r="L71">
+        <v>69</v>
+      </c>
+      <c r="M71">
+        <v>69</v>
+      </c>
+      <c r="N71">
+        <v>69</v>
+      </c>
+      <c r="O71">
         <v>5853</v>
       </c>
-      <c r="M71">
+      <c r="P71">
         <v>6182</v>
       </c>
-      <c r="N71" t="s">
-        <v>84</v>
-      </c>
-      <c r="O71">
+      <c r="Q71" t="s">
+        <v>87</v>
+      </c>
+      <c r="R71">
         <v>329</v>
       </c>
-      <c r="P71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
+      <c r="S71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4295,22 +4943,31 @@
         <v>70</v>
       </c>
       <c r="L72">
+        <v>70</v>
+      </c>
+      <c r="M72">
+        <v>70</v>
+      </c>
+      <c r="N72">
+        <v>70</v>
+      </c>
+      <c r="O72">
         <v>5897</v>
       </c>
-      <c r="M72">
+      <c r="P72">
         <v>6226</v>
       </c>
-      <c r="N72" t="s">
-        <v>85</v>
-      </c>
-      <c r="O72">
+      <c r="Q72" t="s">
+        <v>88</v>
+      </c>
+      <c r="R72">
         <v>329</v>
       </c>
-      <c r="P72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16">
+      <c r="S72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4345,22 +5002,31 @@
         <v>71</v>
       </c>
       <c r="L73">
+        <v>71</v>
+      </c>
+      <c r="M73">
+        <v>71</v>
+      </c>
+      <c r="N73">
+        <v>71</v>
+      </c>
+      <c r="O73">
         <v>5956</v>
       </c>
-      <c r="M73">
+      <c r="P73">
         <v>6287</v>
       </c>
-      <c r="N73" t="s">
-        <v>86</v>
-      </c>
-      <c r="O73">
+      <c r="Q73" t="s">
+        <v>89</v>
+      </c>
+      <c r="R73">
         <v>331</v>
       </c>
-      <c r="P73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16">
+      <c r="S73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4395,22 +5061,31 @@
         <v>72</v>
       </c>
       <c r="L74">
+        <v>72</v>
+      </c>
+      <c r="M74">
+        <v>72</v>
+      </c>
+      <c r="N74">
+        <v>72</v>
+      </c>
+      <c r="O74">
         <v>6013</v>
       </c>
-      <c r="M74">
+      <c r="P74">
         <v>6352</v>
       </c>
-      <c r="N74" t="s">
-        <v>87</v>
-      </c>
-      <c r="O74">
+      <c r="Q74" t="s">
+        <v>90</v>
+      </c>
+      <c r="R74">
         <v>339</v>
       </c>
-      <c r="P74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="S74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4445,22 +5120,31 @@
         <v>73</v>
       </c>
       <c r="L75">
+        <v>73</v>
+      </c>
+      <c r="M75">
+        <v>73</v>
+      </c>
+      <c r="N75">
+        <v>73</v>
+      </c>
+      <c r="O75">
         <v>6118</v>
       </c>
-      <c r="M75">
+      <c r="P75">
         <v>6457</v>
       </c>
-      <c r="N75" t="s">
-        <v>88</v>
-      </c>
-      <c r="O75">
+      <c r="Q75" t="s">
+        <v>91</v>
+      </c>
+      <c r="R75">
         <v>339</v>
       </c>
-      <c r="P75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="S75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4495,22 +5179,31 @@
         <v>74</v>
       </c>
       <c r="L76">
+        <v>74</v>
+      </c>
+      <c r="M76">
+        <v>74</v>
+      </c>
+      <c r="N76">
+        <v>74</v>
+      </c>
+      <c r="O76">
         <v>6236</v>
       </c>
-      <c r="M76">
+      <c r="P76">
         <v>6579</v>
       </c>
-      <c r="N76" t="s">
-        <v>89</v>
-      </c>
-      <c r="O76">
+      <c r="Q76" t="s">
+        <v>92</v>
+      </c>
+      <c r="R76">
         <v>343</v>
       </c>
-      <c r="P76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16">
+      <c r="S76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4545,22 +5238,31 @@
         <v>75</v>
       </c>
       <c r="L77">
+        <v>75</v>
+      </c>
+      <c r="M77">
+        <v>75</v>
+      </c>
+      <c r="N77">
+        <v>75</v>
+      </c>
+      <c r="O77">
         <v>6314</v>
       </c>
-      <c r="M77">
+      <c r="P77">
         <v>6657</v>
       </c>
-      <c r="N77" t="s">
-        <v>90</v>
-      </c>
-      <c r="O77">
+      <c r="Q77" t="s">
+        <v>93</v>
+      </c>
+      <c r="R77">
         <v>343</v>
       </c>
-      <c r="P77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="S77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4595,22 +5297,31 @@
         <v>76</v>
       </c>
       <c r="L78">
+        <v>76</v>
+      </c>
+      <c r="M78">
+        <v>76</v>
+      </c>
+      <c r="N78">
+        <v>76</v>
+      </c>
+      <c r="O78">
         <v>6376</v>
       </c>
-      <c r="M78">
+      <c r="P78">
         <v>6719</v>
       </c>
-      <c r="N78" t="s">
-        <v>91</v>
-      </c>
-      <c r="O78">
+      <c r="Q78" t="s">
+        <v>94</v>
+      </c>
+      <c r="R78">
         <v>343</v>
       </c>
-      <c r="P78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16">
+      <c r="S78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4645,22 +5356,31 @@
         <v>77</v>
       </c>
       <c r="L79">
+        <v>77</v>
+      </c>
+      <c r="M79">
+        <v>77</v>
+      </c>
+      <c r="N79">
+        <v>77</v>
+      </c>
+      <c r="O79">
         <v>6502</v>
       </c>
-      <c r="M79">
+      <c r="P79">
         <v>6845</v>
       </c>
-      <c r="N79" t="s">
-        <v>92</v>
-      </c>
-      <c r="O79">
+      <c r="Q79" t="s">
+        <v>95</v>
+      </c>
+      <c r="R79">
         <v>343</v>
       </c>
-      <c r="P79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="S79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4695,22 +5415,31 @@
         <v>78</v>
       </c>
       <c r="L80">
+        <v>78</v>
+      </c>
+      <c r="M80">
+        <v>78</v>
+      </c>
+      <c r="N80">
+        <v>78</v>
+      </c>
+      <c r="O80">
         <v>6568</v>
       </c>
-      <c r="M80">
+      <c r="P80">
         <v>6923</v>
       </c>
-      <c r="N80" t="s">
-        <v>93</v>
-      </c>
-      <c r="O80">
+      <c r="Q80" t="s">
+        <v>96</v>
+      </c>
+      <c r="R80">
         <v>355</v>
       </c>
-      <c r="P80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="S80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4745,22 +5474,31 @@
         <v>79</v>
       </c>
       <c r="L81">
+        <v>79</v>
+      </c>
+      <c r="M81">
+        <v>79</v>
+      </c>
+      <c r="N81">
+        <v>79</v>
+      </c>
+      <c r="O81">
         <v>6701</v>
       </c>
-      <c r="M81">
+      <c r="P81">
         <v>7056</v>
       </c>
-      <c r="N81" t="s">
-        <v>94</v>
-      </c>
-      <c r="O81">
+      <c r="Q81" t="s">
+        <v>97</v>
+      </c>
+      <c r="R81">
         <v>355</v>
       </c>
-      <c r="P81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="S81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4795,22 +5533,31 @@
         <v>80</v>
       </c>
       <c r="L82">
+        <v>80</v>
+      </c>
+      <c r="M82">
+        <v>80</v>
+      </c>
+      <c r="N82">
+        <v>80</v>
+      </c>
+      <c r="O82">
         <v>6829</v>
       </c>
-      <c r="M82">
+      <c r="P82">
         <v>7186</v>
       </c>
-      <c r="N82" t="s">
-        <v>95</v>
-      </c>
-      <c r="O82">
+      <c r="Q82" t="s">
+        <v>98</v>
+      </c>
+      <c r="R82">
         <v>357</v>
       </c>
-      <c r="P82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16">
+      <c r="S82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4845,22 +5592,31 @@
         <v>81</v>
       </c>
       <c r="L83">
+        <v>81</v>
+      </c>
+      <c r="M83">
+        <v>81</v>
+      </c>
+      <c r="N83">
+        <v>81</v>
+      </c>
+      <c r="O83">
         <v>6973</v>
       </c>
-      <c r="M83">
+      <c r="P83">
         <v>7331</v>
       </c>
-      <c r="N83" t="s">
-        <v>96</v>
-      </c>
-      <c r="O83">
+      <c r="Q83" t="s">
+        <v>99</v>
+      </c>
+      <c r="R83">
         <v>358</v>
       </c>
-      <c r="P83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16">
+      <c r="S83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4895,22 +5651,31 @@
         <v>82</v>
       </c>
       <c r="L84">
+        <v>82</v>
+      </c>
+      <c r="M84">
+        <v>82</v>
+      </c>
+      <c r="N84">
+        <v>82</v>
+      </c>
+      <c r="O84">
         <v>7124</v>
       </c>
-      <c r="M84">
+      <c r="P84">
         <v>7483</v>
       </c>
-      <c r="N84" t="s">
-        <v>97</v>
-      </c>
-      <c r="O84">
+      <c r="Q84" t="s">
+        <v>100</v>
+      </c>
+      <c r="R84">
         <v>359</v>
       </c>
-      <c r="P84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16">
+      <c r="S84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4945,22 +5710,31 @@
         <v>83</v>
       </c>
       <c r="L85">
+        <v>83</v>
+      </c>
+      <c r="M85">
+        <v>83</v>
+      </c>
+      <c r="N85">
+        <v>83</v>
+      </c>
+      <c r="O85">
         <v>7229</v>
       </c>
-      <c r="M85">
+      <c r="P85">
         <v>7592</v>
       </c>
-      <c r="N85" t="s">
-        <v>98</v>
-      </c>
-      <c r="O85">
+      <c r="Q85" t="s">
+        <v>101</v>
+      </c>
+      <c r="R85">
         <v>363</v>
       </c>
-      <c r="P85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16">
+      <c r="S85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4995,22 +5769,31 @@
         <v>84</v>
       </c>
       <c r="L86">
+        <v>84</v>
+      </c>
+      <c r="M86">
+        <v>84</v>
+      </c>
+      <c r="N86">
+        <v>84</v>
+      </c>
+      <c r="O86">
         <v>7434</v>
       </c>
-      <c r="M86">
+      <c r="P86">
         <v>7799</v>
       </c>
-      <c r="N86" t="s">
-        <v>99</v>
-      </c>
-      <c r="O86">
+      <c r="Q86" t="s">
+        <v>102</v>
+      </c>
+      <c r="R86">
         <v>365</v>
       </c>
-      <c r="P86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16">
+      <c r="S86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5045,22 +5828,31 @@
         <v>85</v>
       </c>
       <c r="L87">
+        <v>85</v>
+      </c>
+      <c r="M87">
+        <v>85</v>
+      </c>
+      <c r="N87">
+        <v>85</v>
+      </c>
+      <c r="O87">
         <v>7548</v>
       </c>
-      <c r="M87">
+      <c r="P87">
         <v>7915</v>
       </c>
-      <c r="N87" t="s">
-        <v>100</v>
-      </c>
-      <c r="O87">
+      <c r="Q87" t="s">
+        <v>103</v>
+      </c>
+      <c r="R87">
         <v>367</v>
       </c>
-      <c r="P87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16">
+      <c r="S87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5095,22 +5887,31 @@
         <v>86</v>
       </c>
       <c r="L88">
+        <v>86</v>
+      </c>
+      <c r="M88">
+        <v>86</v>
+      </c>
+      <c r="N88">
+        <v>86</v>
+      </c>
+      <c r="O88">
         <v>7725</v>
       </c>
-      <c r="M88">
+      <c r="P88">
         <v>8100</v>
       </c>
-      <c r="N88" t="s">
-        <v>101</v>
-      </c>
-      <c r="O88">
+      <c r="Q88" t="s">
+        <v>104</v>
+      </c>
+      <c r="R88">
         <v>375</v>
       </c>
-      <c r="P88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16">
+      <c r="S88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5145,22 +5946,31 @@
         <v>87</v>
       </c>
       <c r="L89">
+        <v>87</v>
+      </c>
+      <c r="M89">
+        <v>87</v>
+      </c>
+      <c r="N89">
+        <v>87</v>
+      </c>
+      <c r="O89">
         <v>7937</v>
       </c>
-      <c r="M89">
+      <c r="P89">
         <v>8314</v>
       </c>
-      <c r="N89" t="s">
-        <v>102</v>
-      </c>
-      <c r="O89">
+      <c r="Q89" t="s">
+        <v>105</v>
+      </c>
+      <c r="R89">
         <v>377</v>
       </c>
-      <c r="P89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16">
+      <c r="S89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5195,22 +6005,31 @@
         <v>88</v>
       </c>
       <c r="L90">
+        <v>88</v>
+      </c>
+      <c r="M90">
+        <v>88</v>
+      </c>
+      <c r="N90">
+        <v>88</v>
+      </c>
+      <c r="O90">
         <v>8179</v>
       </c>
-      <c r="M90">
+      <c r="P90">
         <v>8556</v>
       </c>
-      <c r="N90" t="s">
-        <v>103</v>
-      </c>
-      <c r="O90">
+      <c r="Q90" t="s">
+        <v>106</v>
+      </c>
+      <c r="R90">
         <v>377</v>
       </c>
-      <c r="P90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16">
+      <c r="S90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5226,23 +6045,32 @@
       <c r="E91">
         <v>89</v>
       </c>
-      <c r="L91">
+      <c r="F91">
+        <v>89</v>
+      </c>
+      <c r="G91">
+        <v>89</v>
+      </c>
+      <c r="H91">
+        <v>89</v>
+      </c>
+      <c r="O91">
         <v>8357</v>
       </c>
-      <c r="M91">
+      <c r="P91">
         <v>8735</v>
       </c>
-      <c r="N91" t="s">
-        <v>104</v>
-      </c>
-      <c r="O91">
+      <c r="Q91" t="s">
+        <v>107</v>
+      </c>
+      <c r="R91">
         <v>378</v>
       </c>
-      <c r="P91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16">
+      <c r="S91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5255,23 +6083,32 @@
       <c r="D92">
         <v>90</v>
       </c>
-      <c r="L92">
+      <c r="E92">
+        <v>90</v>
+      </c>
+      <c r="F92">
+        <v>90</v>
+      </c>
+      <c r="G92">
+        <v>90</v>
+      </c>
+      <c r="O92">
         <v>8436</v>
       </c>
-      <c r="M92">
+      <c r="P92">
         <v>8815</v>
       </c>
-      <c r="N92" t="s">
-        <v>105</v>
-      </c>
-      <c r="O92">
+      <c r="Q92" t="s">
+        <v>108</v>
+      </c>
+      <c r="R92">
         <v>379</v>
       </c>
-      <c r="P92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16">
+      <c r="S92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5284,23 +6121,32 @@
       <c r="D93">
         <v>91</v>
       </c>
-      <c r="L93">
+      <c r="E93">
+        <v>91</v>
+      </c>
+      <c r="F93">
+        <v>91</v>
+      </c>
+      <c r="G93">
+        <v>91</v>
+      </c>
+      <c r="O93">
         <v>8777</v>
       </c>
-      <c r="M93">
+      <c r="P93">
         <v>9157</v>
       </c>
-      <c r="N93" t="s">
-        <v>106</v>
-      </c>
-      <c r="O93">
+      <c r="Q93" t="s">
+        <v>109</v>
+      </c>
+      <c r="R93">
         <v>380</v>
       </c>
-      <c r="P93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16">
+      <c r="S93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5310,111 +6156,156 @@
       <c r="C94">
         <v>92</v>
       </c>
-      <c r="L94">
+      <c r="D94">
+        <v>92</v>
+      </c>
+      <c r="E94">
+        <v>92</v>
+      </c>
+      <c r="F94">
+        <v>92</v>
+      </c>
+      <c r="O94">
         <v>8932</v>
       </c>
-      <c r="M94">
+      <c r="P94">
         <v>9318</v>
       </c>
-      <c r="N94" t="s">
-        <v>107</v>
-      </c>
-      <c r="O94">
+      <c r="Q94" t="s">
+        <v>110</v>
+      </c>
+      <c r="R94">
         <v>386</v>
       </c>
-      <c r="P94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16">
+      <c r="S94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95">
         <v>93</v>
       </c>
-      <c r="L95">
+      <c r="C95">
+        <v>93</v>
+      </c>
+      <c r="D95">
+        <v>93</v>
+      </c>
+      <c r="E95">
+        <v>93</v>
+      </c>
+      <c r="O95">
         <v>9148</v>
       </c>
-      <c r="M95">
+      <c r="P95">
         <v>9535</v>
       </c>
-      <c r="N95" t="s">
-        <v>108</v>
-      </c>
-      <c r="O95">
+      <c r="Q95" t="s">
+        <v>111</v>
+      </c>
+      <c r="R95">
         <v>387</v>
       </c>
-      <c r="P95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16">
+      <c r="S95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96">
         <v>94</v>
       </c>
-      <c r="L96">
+      <c r="C96">
+        <v>94</v>
+      </c>
+      <c r="D96">
+        <v>94</v>
+      </c>
+      <c r="E96">
+        <v>94</v>
+      </c>
+      <c r="O96">
         <v>9462</v>
       </c>
-      <c r="M96">
+      <c r="P96">
         <v>9852</v>
       </c>
-      <c r="N96" t="s">
-        <v>109</v>
-      </c>
-      <c r="O96">
+      <c r="Q96" t="s">
+        <v>112</v>
+      </c>
+      <c r="R96">
         <v>390</v>
       </c>
-      <c r="P96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16">
+      <c r="S96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97">
         <v>95</v>
       </c>
-      <c r="L97">
+      <c r="C97">
+        <v>95</v>
+      </c>
+      <c r="D97">
+        <v>95</v>
+      </c>
+      <c r="E97">
+        <v>95</v>
+      </c>
+      <c r="O97">
         <v>9862</v>
       </c>
-      <c r="M97">
+      <c r="P97">
         <v>10259</v>
       </c>
-      <c r="N97" t="s">
-        <v>110</v>
-      </c>
-      <c r="O97">
+      <c r="Q97" t="s">
+        <v>113</v>
+      </c>
+      <c r="R97">
         <v>397</v>
       </c>
-      <c r="P97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16">
+      <c r="S97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98">
         <v>96</v>
       </c>
-      <c r="L98">
+      <c r="C98">
+        <v>96</v>
+      </c>
+      <c r="D98">
+        <v>96</v>
+      </c>
+      <c r="E98">
+        <v>96</v>
+      </c>
+      <c r="O98">
         <v>10088</v>
       </c>
-      <c r="M98">
+      <c r="P98">
         <v>10486</v>
       </c>
-      <c r="N98" t="s">
-        <v>111</v>
-      </c>
-      <c r="O98">
+      <c r="Q98" t="s">
+        <v>114</v>
+      </c>
+      <c r="R98">
         <v>398</v>
       </c>
-      <c r="P98">
+      <c r="S98">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating plotting code so that days without reported data don't cause the trend to go negative
</commit_message>
<xml_diff>
--- a/Clark_Data.xlsx
+++ b/Clark_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Active</t>
@@ -728,13 +734,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,8 +801,14 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -849,19 +861,25 @@
         <v>0</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="U2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -911,22 +929,28 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
-        <v>21</v>
+      <c r="S3">
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -976,22 +1000,28 @@
         <v>2</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>1</v>
       </c>
-      <c r="S4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="U4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1041,22 +1071,28 @@
         <v>3</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>2</v>
       </c>
-      <c r="S5" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="U5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1106,22 +1142,28 @@
         <v>4</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>2</v>
       </c>
-      <c r="S6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="U6" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1171,22 +1213,28 @@
         <v>5</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>126</v>
       </c>
-      <c r="S7" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7">
+      <c r="U7" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7">
         <v>2</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1236,22 +1284,28 @@
         <v>6</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>126</v>
       </c>
-      <c r="S8" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8">
+      <c r="U8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V8">
         <v>4</v>
       </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1301,22 +1355,28 @@
         <v>7</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
         <v>212</v>
       </c>
-      <c r="S9" t="s">
-        <v>27</v>
-      </c>
-      <c r="T9">
+      <c r="U9" t="s">
+        <v>29</v>
+      </c>
+      <c r="V9">
         <v>4</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1366,22 +1426,28 @@
         <v>8</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R10">
+        <v>8</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
         <v>249</v>
       </c>
-      <c r="S10" t="s">
-        <v>28</v>
-      </c>
-      <c r="T10">
+      <c r="U10" t="s">
+        <v>30</v>
+      </c>
+      <c r="V10">
         <v>6</v>
       </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1431,22 +1497,28 @@
         <v>9</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="R11">
+        <v>9</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>350</v>
       </c>
-      <c r="S11" t="s">
-        <v>29</v>
-      </c>
-      <c r="T11">
+      <c r="U11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V11">
         <v>6</v>
       </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1496,22 +1568,28 @@
         <v>10</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R12">
+        <v>10</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
         <v>443</v>
       </c>
-      <c r="S12" t="s">
-        <v>30</v>
-      </c>
-      <c r="T12">
+      <c r="U12" t="s">
+        <v>32</v>
+      </c>
+      <c r="V12">
         <v>10</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1561,22 +1639,28 @@
         <v>11</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="R13">
+        <v>11</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
         <v>443</v>
       </c>
-      <c r="S13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T13">
+      <c r="U13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V13">
         <v>10</v>
       </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1626,22 +1710,28 @@
         <v>12</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R14">
+        <v>12</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
         <v>528</v>
       </c>
-      <c r="S14" t="s">
-        <v>32</v>
-      </c>
-      <c r="T14">
+      <c r="U14" t="s">
+        <v>34</v>
+      </c>
+      <c r="V14">
         <v>14</v>
       </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1691,22 +1781,28 @@
         <v>13</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="R15">
+        <v>13</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
         <v>753</v>
       </c>
-      <c r="S15" t="s">
-        <v>33</v>
-      </c>
-      <c r="T15">
+      <c r="U15" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15">
         <v>14</v>
       </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1756,22 +1852,28 @@
         <v>14</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="R16">
+        <v>14</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
         <v>869</v>
       </c>
-      <c r="S16" t="s">
-        <v>34</v>
-      </c>
-      <c r="T16">
+      <c r="U16" t="s">
+        <v>36</v>
+      </c>
+      <c r="V16">
         <v>23</v>
       </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1821,22 +1923,28 @@
         <v>15</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R17">
+        <v>15</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
         <v>961</v>
       </c>
-      <c r="S17" t="s">
-        <v>35</v>
-      </c>
-      <c r="T17">
+      <c r="U17" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17">
         <v>28</v>
       </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1886,22 +1994,28 @@
         <v>16</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R18">
+        <v>16</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
         <v>1125</v>
       </c>
-      <c r="S18" t="s">
-        <v>36</v>
-      </c>
-      <c r="T18">
+      <c r="U18" t="s">
+        <v>38</v>
+      </c>
+      <c r="V18">
         <v>34</v>
       </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1951,22 +2065,28 @@
         <v>17</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="R19">
+        <v>17</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
         <v>1279</v>
       </c>
-      <c r="S19" t="s">
-        <v>37</v>
-      </c>
-      <c r="T19">
+      <c r="U19" t="s">
         <v>39</v>
       </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="V19">
+        <v>39</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2016,22 +2136,28 @@
         <v>18</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R20">
+        <v>18</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>1418</v>
       </c>
-      <c r="S20" t="s">
-        <v>38</v>
-      </c>
-      <c r="T20">
+      <c r="U20" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20">
         <v>41</v>
       </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="W20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2081,22 +2207,28 @@
         <v>19</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="R21">
+        <v>19</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
         <v>1519</v>
       </c>
-      <c r="S21" t="s">
-        <v>39</v>
-      </c>
-      <c r="T21">
+      <c r="U21" t="s">
         <v>41</v>
       </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="V21">
+        <v>41</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2146,22 +2278,28 @@
         <v>20</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="R22">
+        <v>20</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
         <v>1608</v>
       </c>
-      <c r="S22" t="s">
-        <v>40</v>
-      </c>
-      <c r="T22">
+      <c r="U22" t="s">
+        <v>42</v>
+      </c>
+      <c r="V22">
         <v>41</v>
       </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2211,22 +2349,28 @@
         <v>21</v>
       </c>
       <c r="Q23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="R23">
+        <v>21</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
         <v>1734</v>
       </c>
-      <c r="S23" t="s">
-        <v>41</v>
-      </c>
-      <c r="T23">
+      <c r="U23" t="s">
+        <v>43</v>
+      </c>
+      <c r="V23">
         <v>54</v>
       </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="W23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2276,22 +2420,28 @@
         <v>22</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="R24">
+        <v>22</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
         <v>1878</v>
       </c>
-      <c r="S24" t="s">
-        <v>42</v>
-      </c>
-      <c r="T24">
+      <c r="U24" t="s">
+        <v>44</v>
+      </c>
+      <c r="V24">
         <v>65</v>
       </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="W24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2341,22 +2491,28 @@
         <v>23</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R25">
+        <v>23</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
         <v>2009</v>
       </c>
-      <c r="S25" t="s">
-        <v>43</v>
-      </c>
-      <c r="T25">
+      <c r="U25" t="s">
+        <v>45</v>
+      </c>
+      <c r="V25">
         <v>71</v>
       </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="W25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2406,22 +2562,28 @@
         <v>24</v>
       </c>
       <c r="Q26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="R26">
+        <v>24</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
         <v>2144</v>
       </c>
-      <c r="S26" t="s">
-        <v>44</v>
-      </c>
-      <c r="T26">
+      <c r="U26" t="s">
+        <v>46</v>
+      </c>
+      <c r="V26">
         <v>75</v>
       </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="W26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2471,22 +2633,28 @@
         <v>25</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="R27">
+        <v>25</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
         <v>2144</v>
       </c>
-      <c r="S27" t="s">
-        <v>45</v>
-      </c>
-      <c r="T27">
+      <c r="U27" t="s">
+        <v>47</v>
+      </c>
+      <c r="V27">
         <v>75</v>
       </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2536,22 +2704,28 @@
         <v>26</v>
       </c>
       <c r="Q28">
+        <v>26</v>
+      </c>
+      <c r="R28">
+        <v>26</v>
+      </c>
+      <c r="S28">
         <v>2224</v>
       </c>
-      <c r="R28">
+      <c r="T28">
         <v>2324</v>
       </c>
-      <c r="S28" t="s">
-        <v>46</v>
-      </c>
-      <c r="T28">
+      <c r="U28" t="s">
+        <v>48</v>
+      </c>
+      <c r="V28">
         <v>100</v>
       </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="W28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2601,22 +2775,28 @@
         <v>27</v>
       </c>
       <c r="Q29">
+        <v>27</v>
+      </c>
+      <c r="R29">
+        <v>27</v>
+      </c>
+      <c r="S29">
         <v>2343</v>
       </c>
-      <c r="R29">
+      <c r="T29">
         <v>2444</v>
       </c>
-      <c r="S29" t="s">
-        <v>47</v>
-      </c>
-      <c r="T29">
+      <c r="U29" t="s">
+        <v>49</v>
+      </c>
+      <c r="V29">
         <v>101</v>
       </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="W29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2666,22 +2846,28 @@
         <v>28</v>
       </c>
       <c r="Q30">
+        <v>28</v>
+      </c>
+      <c r="R30">
+        <v>28</v>
+      </c>
+      <c r="S30">
         <v>2403</v>
       </c>
-      <c r="R30">
+      <c r="T30">
         <v>2509</v>
       </c>
-      <c r="S30" t="s">
-        <v>48</v>
-      </c>
-      <c r="T30">
+      <c r="U30" t="s">
+        <v>50</v>
+      </c>
+      <c r="V30">
         <v>106</v>
       </c>
-      <c r="U30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
+      <c r="W30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2731,22 +2917,28 @@
         <v>29</v>
       </c>
       <c r="Q31">
+        <v>29</v>
+      </c>
+      <c r="R31">
+        <v>29</v>
+      </c>
+      <c r="S31">
         <v>2444</v>
       </c>
-      <c r="R31">
+      <c r="T31">
         <v>2559</v>
       </c>
-      <c r="S31" t="s">
-        <v>49</v>
-      </c>
-      <c r="T31">
+      <c r="U31" t="s">
+        <v>51</v>
+      </c>
+      <c r="V31">
         <v>115</v>
       </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="W31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2796,22 +2988,28 @@
         <v>30</v>
       </c>
       <c r="Q32">
+        <v>30</v>
+      </c>
+      <c r="R32">
+        <v>30</v>
+      </c>
+      <c r="S32">
         <v>2444</v>
       </c>
-      <c r="R32">
+      <c r="T32">
         <v>2559</v>
       </c>
-      <c r="S32" t="s">
-        <v>50</v>
-      </c>
-      <c r="T32">
+      <c r="U32" t="s">
+        <v>52</v>
+      </c>
+      <c r="V32">
         <v>115</v>
       </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="W32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2861,22 +3059,28 @@
         <v>31</v>
       </c>
       <c r="Q33">
+        <v>31</v>
+      </c>
+      <c r="R33">
+        <v>31</v>
+      </c>
+      <c r="S33">
         <v>2614</v>
       </c>
-      <c r="R33">
+      <c r="T33">
         <v>2738</v>
       </c>
-      <c r="S33" t="s">
-        <v>51</v>
-      </c>
-      <c r="T33">
+      <c r="U33" t="s">
+        <v>53</v>
+      </c>
+      <c r="V33">
         <v>124</v>
       </c>
-      <c r="U33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="W33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2926,22 +3130,28 @@
         <v>32</v>
       </c>
       <c r="Q34">
+        <v>32</v>
+      </c>
+      <c r="R34">
+        <v>32</v>
+      </c>
+      <c r="S34">
         <v>2749</v>
       </c>
-      <c r="R34">
+      <c r="T34">
         <v>2882</v>
       </c>
-      <c r="S34" t="s">
-        <v>52</v>
-      </c>
-      <c r="T34">
+      <c r="U34" t="s">
+        <v>54</v>
+      </c>
+      <c r="V34">
         <v>133</v>
       </c>
-      <c r="U34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="W34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2991,22 +3201,28 @@
         <v>33</v>
       </c>
       <c r="Q35">
+        <v>33</v>
+      </c>
+      <c r="R35">
+        <v>33</v>
+      </c>
+      <c r="S35">
         <v>2803</v>
       </c>
-      <c r="R35">
+      <c r="T35">
         <v>2940</v>
       </c>
-      <c r="S35" t="s">
-        <v>53</v>
-      </c>
-      <c r="T35">
+      <c r="U35" t="s">
+        <v>55</v>
+      </c>
+      <c r="V35">
         <v>137</v>
       </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="W35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3056,22 +3272,28 @@
         <v>34</v>
       </c>
       <c r="Q36">
+        <v>34</v>
+      </c>
+      <c r="R36">
+        <v>34</v>
+      </c>
+      <c r="S36">
         <v>2861</v>
       </c>
-      <c r="R36">
+      <c r="T36">
         <v>2998</v>
       </c>
-      <c r="S36" t="s">
-        <v>54</v>
-      </c>
-      <c r="T36">
+      <c r="U36" t="s">
+        <v>56</v>
+      </c>
+      <c r="V36">
         <v>137</v>
       </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="W36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3121,22 +3343,28 @@
         <v>35</v>
       </c>
       <c r="Q37">
+        <v>35</v>
+      </c>
+      <c r="R37">
+        <v>35</v>
+      </c>
+      <c r="S37">
         <v>2958</v>
       </c>
-      <c r="R37">
+      <c r="T37">
         <v>3099</v>
       </c>
-      <c r="S37" t="s">
-        <v>55</v>
-      </c>
-      <c r="T37">
+      <c r="U37" t="s">
+        <v>57</v>
+      </c>
+      <c r="V37">
         <v>141</v>
       </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
+      <c r="W37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3186,22 +3414,28 @@
         <v>36</v>
       </c>
       <c r="Q38">
+        <v>36</v>
+      </c>
+      <c r="R38">
+        <v>36</v>
+      </c>
+      <c r="S38">
         <v>3068</v>
       </c>
-      <c r="R38">
+      <c r="T38">
         <v>3218</v>
       </c>
-      <c r="S38" t="s">
-        <v>56</v>
-      </c>
-      <c r="T38">
+      <c r="U38" t="s">
+        <v>58</v>
+      </c>
+      <c r="V38">
         <v>150</v>
       </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
+      <c r="W38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3251,22 +3485,28 @@
         <v>37</v>
       </c>
       <c r="Q39">
+        <v>37</v>
+      </c>
+      <c r="R39">
+        <v>37</v>
+      </c>
+      <c r="S39">
         <v>3151</v>
       </c>
-      <c r="R39">
+      <c r="T39">
         <v>3314</v>
       </c>
-      <c r="S39" t="s">
-        <v>57</v>
-      </c>
-      <c r="T39">
+      <c r="U39" t="s">
+        <v>59</v>
+      </c>
+      <c r="V39">
         <v>163</v>
       </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="W39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3316,22 +3556,28 @@
         <v>38</v>
       </c>
       <c r="Q40">
+        <v>38</v>
+      </c>
+      <c r="R40">
+        <v>38</v>
+      </c>
+      <c r="S40">
         <v>3275</v>
       </c>
-      <c r="R40">
+      <c r="T40">
         <v>3443</v>
       </c>
-      <c r="S40" t="s">
-        <v>58</v>
-      </c>
-      <c r="T40">
+      <c r="U40" t="s">
+        <v>60</v>
+      </c>
+      <c r="V40">
         <v>168</v>
       </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="W40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3381,22 +3627,28 @@
         <v>39</v>
       </c>
       <c r="Q41">
+        <v>39</v>
+      </c>
+      <c r="R41">
+        <v>39</v>
+      </c>
+      <c r="S41">
         <v>3396</v>
       </c>
-      <c r="R41">
+      <c r="T41">
         <v>3570</v>
       </c>
-      <c r="S41" t="s">
-        <v>59</v>
-      </c>
-      <c r="T41">
+      <c r="U41" t="s">
+        <v>61</v>
+      </c>
+      <c r="V41">
         <v>174</v>
       </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21">
+      <c r="W41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3446,22 +3698,28 @@
         <v>40</v>
       </c>
       <c r="Q42">
+        <v>40</v>
+      </c>
+      <c r="R42">
+        <v>40</v>
+      </c>
+      <c r="S42">
         <v>3491</v>
       </c>
-      <c r="R42">
+      <c r="T42">
         <v>3665</v>
       </c>
-      <c r="S42" t="s">
-        <v>60</v>
-      </c>
-      <c r="T42">
+      <c r="U42" t="s">
+        <v>62</v>
+      </c>
+      <c r="V42">
         <v>174</v>
       </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="W42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3511,22 +3769,28 @@
         <v>41</v>
       </c>
       <c r="Q43">
+        <v>41</v>
+      </c>
+      <c r="R43">
+        <v>41</v>
+      </c>
+      <c r="S43">
         <v>3543</v>
       </c>
-      <c r="R43">
+      <c r="T43">
         <v>3717</v>
       </c>
-      <c r="S43" t="s">
-        <v>61</v>
-      </c>
-      <c r="T43">
+      <c r="U43" t="s">
+        <v>63</v>
+      </c>
+      <c r="V43">
         <v>174</v>
       </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21">
+      <c r="W43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3576,22 +3840,28 @@
         <v>42</v>
       </c>
       <c r="Q44">
+        <v>42</v>
+      </c>
+      <c r="R44">
+        <v>42</v>
+      </c>
+      <c r="S44">
         <v>3607</v>
       </c>
-      <c r="R44">
+      <c r="T44">
         <v>3793</v>
       </c>
-      <c r="S44" t="s">
-        <v>62</v>
-      </c>
-      <c r="T44">
+      <c r="U44" t="s">
+        <v>64</v>
+      </c>
+      <c r="V44">
         <v>186</v>
       </c>
-      <c r="U44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
+      <c r="W44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3641,22 +3911,28 @@
         <v>43</v>
       </c>
       <c r="Q45">
+        <v>43</v>
+      </c>
+      <c r="R45">
+        <v>43</v>
+      </c>
+      <c r="S45">
         <v>3695</v>
       </c>
-      <c r="R45">
+      <c r="T45">
         <v>3891</v>
       </c>
-      <c r="S45" t="s">
-        <v>63</v>
-      </c>
-      <c r="T45">
+      <c r="U45" t="s">
+        <v>65</v>
+      </c>
+      <c r="V45">
         <v>196</v>
       </c>
-      <c r="U45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
+      <c r="W45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3706,22 +3982,28 @@
         <v>44</v>
       </c>
       <c r="Q46">
+        <v>44</v>
+      </c>
+      <c r="R46">
+        <v>44</v>
+      </c>
+      <c r="S46">
         <v>3777</v>
       </c>
-      <c r="R46">
+      <c r="T46">
         <v>3979</v>
       </c>
-      <c r="S46" t="s">
-        <v>64</v>
-      </c>
-      <c r="T46">
+      <c r="U46" t="s">
+        <v>66</v>
+      </c>
+      <c r="V46">
         <v>202</v>
       </c>
-      <c r="U46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
+      <c r="W46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3771,22 +4053,28 @@
         <v>45</v>
       </c>
       <c r="Q47">
+        <v>45</v>
+      </c>
+      <c r="R47">
+        <v>45</v>
+      </c>
+      <c r="S47">
         <v>3912</v>
       </c>
-      <c r="R47">
+      <c r="T47">
         <v>4118</v>
       </c>
-      <c r="S47" t="s">
-        <v>65</v>
-      </c>
-      <c r="T47">
+      <c r="U47" t="s">
+        <v>67</v>
+      </c>
+      <c r="V47">
         <v>206</v>
       </c>
-      <c r="U47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
+      <c r="W47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3836,22 +4124,28 @@
         <v>46</v>
       </c>
       <c r="Q48">
+        <v>46</v>
+      </c>
+      <c r="R48">
+        <v>46</v>
+      </c>
+      <c r="S48">
         <v>4010</v>
       </c>
-      <c r="R48">
+      <c r="T48">
         <v>4225</v>
       </c>
-      <c r="S48" t="s">
-        <v>66</v>
-      </c>
-      <c r="T48">
+      <c r="U48" t="s">
+        <v>68</v>
+      </c>
+      <c r="V48">
         <v>215</v>
       </c>
-      <c r="U48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21">
+      <c r="W48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3901,22 +4195,28 @@
         <v>47</v>
       </c>
       <c r="Q49">
+        <v>47</v>
+      </c>
+      <c r="R49">
+        <v>47</v>
+      </c>
+      <c r="S49">
         <v>4056</v>
       </c>
-      <c r="R49">
+      <c r="T49">
         <v>4274</v>
       </c>
-      <c r="S49" t="s">
-        <v>67</v>
-      </c>
-      <c r="T49">
+      <c r="U49" t="s">
+        <v>69</v>
+      </c>
+      <c r="V49">
         <v>218</v>
       </c>
-      <c r="U49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
+      <c r="W49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3966,22 +4266,28 @@
         <v>48</v>
       </c>
       <c r="Q50">
+        <v>48</v>
+      </c>
+      <c r="R50">
+        <v>48</v>
+      </c>
+      <c r="S50">
         <v>4188</v>
       </c>
-      <c r="R50">
+      <c r="T50">
         <v>4411</v>
       </c>
-      <c r="S50" t="s">
-        <v>68</v>
-      </c>
-      <c r="T50">
+      <c r="U50" t="s">
+        <v>70</v>
+      </c>
+      <c r="V50">
         <v>223</v>
       </c>
-      <c r="U50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
+      <c r="W50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4031,22 +4337,28 @@
         <v>49</v>
       </c>
       <c r="Q51">
+        <v>49</v>
+      </c>
+      <c r="R51">
+        <v>49</v>
+      </c>
+      <c r="S51">
         <v>4182</v>
       </c>
-      <c r="R51">
+      <c r="T51">
         <v>4408</v>
       </c>
-      <c r="S51" t="s">
-        <v>69</v>
-      </c>
-      <c r="T51">
+      <c r="U51" t="s">
+        <v>71</v>
+      </c>
+      <c r="V51">
         <v>226</v>
       </c>
-      <c r="U51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
+      <c r="W51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4096,22 +4408,28 @@
         <v>50</v>
       </c>
       <c r="Q52">
+        <v>50</v>
+      </c>
+      <c r="R52">
+        <v>50</v>
+      </c>
+      <c r="S52">
         <v>4235</v>
       </c>
-      <c r="R52">
+      <c r="T52">
         <v>4473</v>
       </c>
-      <c r="S52" t="s">
-        <v>70</v>
-      </c>
-      <c r="T52">
+      <c r="U52" t="s">
+        <v>72</v>
+      </c>
+      <c r="V52">
         <v>238</v>
       </c>
-      <c r="U52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
+      <c r="W52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4161,22 +4479,28 @@
         <v>51</v>
       </c>
       <c r="Q53">
+        <v>51</v>
+      </c>
+      <c r="R53">
+        <v>51</v>
+      </c>
+      <c r="S53">
         <v>4328</v>
       </c>
-      <c r="R53">
+      <c r="T53">
         <v>4573</v>
       </c>
-      <c r="S53" t="s">
-        <v>71</v>
-      </c>
-      <c r="T53">
+      <c r="U53" t="s">
+        <v>73</v>
+      </c>
+      <c r="V53">
         <v>245</v>
       </c>
-      <c r="U53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21">
+      <c r="W53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4226,22 +4550,28 @@
         <v>52</v>
       </c>
       <c r="Q54">
+        <v>52</v>
+      </c>
+      <c r="R54">
+        <v>52</v>
+      </c>
+      <c r="S54">
         <v>4328</v>
       </c>
-      <c r="R54">
+      <c r="T54">
         <v>4573</v>
       </c>
-      <c r="S54" t="s">
-        <v>72</v>
-      </c>
-      <c r="T54">
+      <c r="U54" t="s">
+        <v>74</v>
+      </c>
+      <c r="V54">
         <v>245</v>
       </c>
-      <c r="U54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21">
+      <c r="W54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4291,22 +4621,28 @@
         <v>53</v>
       </c>
       <c r="Q55">
+        <v>53</v>
+      </c>
+      <c r="R55">
+        <v>53</v>
+      </c>
+      <c r="S55">
         <v>4448</v>
       </c>
-      <c r="R55">
+      <c r="T55">
         <v>4704</v>
       </c>
-      <c r="S55" t="s">
-        <v>73</v>
-      </c>
-      <c r="T55">
+      <c r="U55" t="s">
+        <v>75</v>
+      </c>
+      <c r="V55">
         <v>256</v>
       </c>
-      <c r="U55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
+      <c r="W55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4356,22 +4692,28 @@
         <v>54</v>
       </c>
       <c r="Q56">
+        <v>54</v>
+      </c>
+      <c r="R56">
+        <v>54</v>
+      </c>
+      <c r="S56">
         <v>4490</v>
       </c>
-      <c r="R56">
+      <c r="T56">
         <v>4750</v>
       </c>
-      <c r="S56" t="s">
-        <v>74</v>
-      </c>
-      <c r="T56">
+      <c r="U56" t="s">
+        <v>76</v>
+      </c>
+      <c r="V56">
         <v>260</v>
       </c>
-      <c r="U56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21">
+      <c r="W56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4421,22 +4763,28 @@
         <v>55</v>
       </c>
       <c r="Q57">
+        <v>55</v>
+      </c>
+      <c r="R57">
+        <v>55</v>
+      </c>
+      <c r="S57">
         <v>4502</v>
       </c>
-      <c r="R57">
+      <c r="T57">
         <v>4762</v>
       </c>
-      <c r="S57" t="s">
-        <v>75</v>
-      </c>
-      <c r="T57">
+      <c r="U57" t="s">
+        <v>77</v>
+      </c>
+      <c r="V57">
         <v>260</v>
       </c>
-      <c r="U57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
+      <c r="W57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4486,22 +4834,28 @@
         <v>56</v>
       </c>
       <c r="Q58">
+        <v>56</v>
+      </c>
+      <c r="R58">
+        <v>56</v>
+      </c>
+      <c r="S58">
         <v>4602</v>
       </c>
-      <c r="R58">
+      <c r="T58">
         <v>4869</v>
       </c>
-      <c r="S58" t="s">
-        <v>76</v>
-      </c>
-      <c r="T58">
+      <c r="U58" t="s">
+        <v>78</v>
+      </c>
+      <c r="V58">
         <v>267</v>
       </c>
-      <c r="U58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21">
+      <c r="W58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4551,22 +4905,28 @@
         <v>57</v>
       </c>
       <c r="Q59">
+        <v>57</v>
+      </c>
+      <c r="R59">
+        <v>57</v>
+      </c>
+      <c r="S59">
         <v>4770</v>
       </c>
-      <c r="R59">
+      <c r="T59">
         <v>5045</v>
       </c>
-      <c r="S59" t="s">
-        <v>77</v>
-      </c>
-      <c r="T59">
+      <c r="U59" t="s">
+        <v>79</v>
+      </c>
+      <c r="V59">
         <v>275</v>
       </c>
-      <c r="U59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21">
+      <c r="W59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4616,22 +4976,28 @@
         <v>58</v>
       </c>
       <c r="Q60">
+        <v>58</v>
+      </c>
+      <c r="R60">
+        <v>58</v>
+      </c>
+      <c r="S60">
         <v>4770</v>
       </c>
-      <c r="R60">
+      <c r="T60">
         <v>5045</v>
       </c>
-      <c r="S60" t="s">
-        <v>78</v>
-      </c>
-      <c r="T60">
+      <c r="U60" t="s">
+        <v>80</v>
+      </c>
+      <c r="V60">
         <v>275</v>
       </c>
-      <c r="U60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21">
+      <c r="W60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4681,22 +5047,28 @@
         <v>59</v>
       </c>
       <c r="Q61">
+        <v>59</v>
+      </c>
+      <c r="R61">
+        <v>59</v>
+      </c>
+      <c r="S61">
         <v>4944</v>
       </c>
-      <c r="R61">
+      <c r="T61">
         <v>5235</v>
       </c>
-      <c r="S61" t="s">
-        <v>79</v>
-      </c>
-      <c r="T61">
+      <c r="U61" t="s">
+        <v>81</v>
+      </c>
+      <c r="V61">
         <v>291</v>
       </c>
-      <c r="U61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21">
+      <c r="W61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4746,22 +5118,28 @@
         <v>60</v>
       </c>
       <c r="Q62">
+        <v>60</v>
+      </c>
+      <c r="R62">
+        <v>60</v>
+      </c>
+      <c r="S62">
         <v>5005</v>
       </c>
-      <c r="R62">
+      <c r="T62">
         <v>5298</v>
       </c>
-      <c r="S62" t="s">
-        <v>80</v>
-      </c>
-      <c r="T62">
+      <c r="U62" t="s">
+        <v>82</v>
+      </c>
+      <c r="V62">
         <v>293</v>
       </c>
-      <c r="U62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21">
+      <c r="W62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4811,22 +5189,28 @@
         <v>61</v>
       </c>
       <c r="Q63">
+        <v>61</v>
+      </c>
+      <c r="R63">
+        <v>61</v>
+      </c>
+      <c r="S63">
         <v>5070</v>
       </c>
-      <c r="R63">
+      <c r="T63">
         <v>5366</v>
       </c>
-      <c r="S63" t="s">
-        <v>81</v>
-      </c>
-      <c r="T63">
+      <c r="U63" t="s">
+        <v>83</v>
+      </c>
+      <c r="V63">
         <v>296</v>
       </c>
-      <c r="U63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21">
+      <c r="W63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4876,22 +5260,28 @@
         <v>62</v>
       </c>
       <c r="Q64">
+        <v>62</v>
+      </c>
+      <c r="R64">
+        <v>62</v>
+      </c>
+      <c r="S64">
         <v>5167</v>
       </c>
-      <c r="R64">
+      <c r="T64">
         <v>5463</v>
       </c>
-      <c r="S64" t="s">
-        <v>82</v>
-      </c>
-      <c r="T64">
+      <c r="U64" t="s">
+        <v>84</v>
+      </c>
+      <c r="V64">
         <v>296</v>
       </c>
-      <c r="U64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21">
+      <c r="W64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4941,22 +5331,28 @@
         <v>63</v>
       </c>
       <c r="Q65">
+        <v>63</v>
+      </c>
+      <c r="R65">
+        <v>63</v>
+      </c>
+      <c r="S65">
         <v>5167</v>
       </c>
-      <c r="R65">
+      <c r="T65">
         <v>5463</v>
       </c>
-      <c r="S65" t="s">
-        <v>83</v>
-      </c>
-      <c r="T65">
+      <c r="U65" t="s">
+        <v>85</v>
+      </c>
+      <c r="V65">
         <v>296</v>
       </c>
-      <c r="U65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21">
+      <c r="W65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5006,22 +5402,28 @@
         <v>64</v>
       </c>
       <c r="Q66">
+        <v>64</v>
+      </c>
+      <c r="R66">
+        <v>64</v>
+      </c>
+      <c r="S66">
         <v>5336</v>
       </c>
-      <c r="R66">
+      <c r="T66">
         <v>5650</v>
       </c>
-      <c r="S66" t="s">
-        <v>84</v>
-      </c>
-      <c r="T66">
+      <c r="U66" t="s">
+        <v>86</v>
+      </c>
+      <c r="V66">
         <v>314</v>
       </c>
-      <c r="U66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21">
+      <c r="W66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5071,22 +5473,28 @@
         <v>65</v>
       </c>
       <c r="Q67">
+        <v>65</v>
+      </c>
+      <c r="R67">
+        <v>65</v>
+      </c>
+      <c r="S67">
         <v>5414</v>
       </c>
-      <c r="R67">
+      <c r="T67">
         <v>5734</v>
       </c>
-      <c r="S67" t="s">
-        <v>85</v>
-      </c>
-      <c r="T67">
+      <c r="U67" t="s">
+        <v>87</v>
+      </c>
+      <c r="V67">
         <v>320</v>
       </c>
-      <c r="U67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21">
+      <c r="W67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5136,22 +5544,28 @@
         <v>66</v>
       </c>
       <c r="Q68">
+        <v>66</v>
+      </c>
+      <c r="R68">
+        <v>66</v>
+      </c>
+      <c r="S68">
         <v>5493</v>
       </c>
-      <c r="R68">
+      <c r="T68">
         <v>5815</v>
       </c>
-      <c r="S68" t="s">
-        <v>86</v>
-      </c>
-      <c r="T68">
+      <c r="U68" t="s">
+        <v>88</v>
+      </c>
+      <c r="V68">
         <v>322</v>
       </c>
-      <c r="U68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21">
+      <c r="W68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5201,22 +5615,28 @@
         <v>67</v>
       </c>
       <c r="Q69">
+        <v>67</v>
+      </c>
+      <c r="R69">
+        <v>67</v>
+      </c>
+      <c r="S69">
         <v>5493</v>
       </c>
-      <c r="R69">
+      <c r="T69">
         <v>5815</v>
       </c>
-      <c r="S69" t="s">
-        <v>87</v>
-      </c>
-      <c r="T69">
+      <c r="U69" t="s">
+        <v>89</v>
+      </c>
+      <c r="V69">
         <v>322</v>
       </c>
-      <c r="U69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21">
+      <c r="W69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5266,22 +5686,28 @@
         <v>68</v>
       </c>
       <c r="Q70">
+        <v>68</v>
+      </c>
+      <c r="R70">
+        <v>68</v>
+      </c>
+      <c r="S70">
         <v>5818</v>
       </c>
-      <c r="R70">
+      <c r="T70">
         <v>6140</v>
       </c>
-      <c r="S70" t="s">
-        <v>88</v>
-      </c>
-      <c r="T70">
+      <c r="U70" t="s">
+        <v>90</v>
+      </c>
+      <c r="V70">
         <v>322</v>
       </c>
-      <c r="U70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21">
+      <c r="W70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5331,22 +5757,28 @@
         <v>69</v>
       </c>
       <c r="Q71">
+        <v>69</v>
+      </c>
+      <c r="R71">
+        <v>69</v>
+      </c>
+      <c r="S71">
         <v>5853</v>
       </c>
-      <c r="R71">
+      <c r="T71">
         <v>6182</v>
       </c>
-      <c r="S71" t="s">
-        <v>89</v>
-      </c>
-      <c r="T71">
+      <c r="U71" t="s">
+        <v>91</v>
+      </c>
+      <c r="V71">
         <v>329</v>
       </c>
-      <c r="U71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21">
+      <c r="W71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5396,22 +5828,28 @@
         <v>70</v>
       </c>
       <c r="Q72">
+        <v>70</v>
+      </c>
+      <c r="R72">
+        <v>70</v>
+      </c>
+      <c r="S72">
         <v>5897</v>
       </c>
-      <c r="R72">
+      <c r="T72">
         <v>6226</v>
       </c>
-      <c r="S72" t="s">
-        <v>90</v>
-      </c>
-      <c r="T72">
+      <c r="U72" t="s">
+        <v>92</v>
+      </c>
+      <c r="V72">
         <v>329</v>
       </c>
-      <c r="U72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21">
+      <c r="W72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5461,22 +5899,28 @@
         <v>71</v>
       </c>
       <c r="Q73">
+        <v>71</v>
+      </c>
+      <c r="R73">
+        <v>71</v>
+      </c>
+      <c r="S73">
         <v>5956</v>
       </c>
-      <c r="R73">
+      <c r="T73">
         <v>6287</v>
       </c>
-      <c r="S73" t="s">
-        <v>91</v>
-      </c>
-      <c r="T73">
+      <c r="U73" t="s">
+        <v>93</v>
+      </c>
+      <c r="V73">
         <v>331</v>
       </c>
-      <c r="U73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21">
+      <c r="W73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5526,22 +5970,28 @@
         <v>72</v>
       </c>
       <c r="Q74">
+        <v>72</v>
+      </c>
+      <c r="R74">
+        <v>72</v>
+      </c>
+      <c r="S74">
         <v>6013</v>
       </c>
-      <c r="R74">
+      <c r="T74">
         <v>6352</v>
       </c>
-      <c r="S74" t="s">
-        <v>92</v>
-      </c>
-      <c r="T74">
+      <c r="U74" t="s">
+        <v>94</v>
+      </c>
+      <c r="V74">
         <v>339</v>
       </c>
-      <c r="U74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21">
+      <c r="W74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5591,22 +6041,28 @@
         <v>73</v>
       </c>
       <c r="Q75">
+        <v>73</v>
+      </c>
+      <c r="R75">
+        <v>73</v>
+      </c>
+      <c r="S75">
         <v>6118</v>
       </c>
-      <c r="R75">
+      <c r="T75">
         <v>6457</v>
       </c>
-      <c r="S75" t="s">
-        <v>93</v>
-      </c>
-      <c r="T75">
+      <c r="U75" t="s">
+        <v>95</v>
+      </c>
+      <c r="V75">
         <v>339</v>
       </c>
-      <c r="U75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21">
+      <c r="W75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5656,22 +6112,28 @@
         <v>74</v>
       </c>
       <c r="Q76">
+        <v>74</v>
+      </c>
+      <c r="R76">
+        <v>74</v>
+      </c>
+      <c r="S76">
         <v>6236</v>
       </c>
-      <c r="R76">
+      <c r="T76">
         <v>6579</v>
       </c>
-      <c r="S76" t="s">
-        <v>94</v>
-      </c>
-      <c r="T76">
+      <c r="U76" t="s">
+        <v>96</v>
+      </c>
+      <c r="V76">
         <v>343</v>
       </c>
-      <c r="U76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21">
+      <c r="W76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5721,22 +6183,28 @@
         <v>75</v>
       </c>
       <c r="Q77">
+        <v>75</v>
+      </c>
+      <c r="R77">
+        <v>75</v>
+      </c>
+      <c r="S77">
         <v>6314</v>
       </c>
-      <c r="R77">
+      <c r="T77">
         <v>6657</v>
       </c>
-      <c r="S77" t="s">
-        <v>95</v>
-      </c>
-      <c r="T77">
+      <c r="U77" t="s">
+        <v>97</v>
+      </c>
+      <c r="V77">
         <v>343</v>
       </c>
-      <c r="U77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21">
+      <c r="W77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5786,22 +6254,28 @@
         <v>76</v>
       </c>
       <c r="Q78">
+        <v>76</v>
+      </c>
+      <c r="R78">
+        <v>76</v>
+      </c>
+      <c r="S78">
         <v>6376</v>
       </c>
-      <c r="R78">
+      <c r="T78">
         <v>6719</v>
       </c>
-      <c r="S78" t="s">
-        <v>96</v>
-      </c>
-      <c r="T78">
+      <c r="U78" t="s">
+        <v>98</v>
+      </c>
+      <c r="V78">
         <v>343</v>
       </c>
-      <c r="U78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21">
+      <c r="W78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5851,22 +6325,28 @@
         <v>77</v>
       </c>
       <c r="Q79">
+        <v>77</v>
+      </c>
+      <c r="R79">
+        <v>77</v>
+      </c>
+      <c r="S79">
         <v>6502</v>
       </c>
-      <c r="R79">
+      <c r="T79">
         <v>6845</v>
       </c>
-      <c r="S79" t="s">
-        <v>97</v>
-      </c>
-      <c r="T79">
+      <c r="U79" t="s">
+        <v>99</v>
+      </c>
+      <c r="V79">
         <v>343</v>
       </c>
-      <c r="U79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21">
+      <c r="W79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5916,22 +6396,28 @@
         <v>78</v>
       </c>
       <c r="Q80">
+        <v>78</v>
+      </c>
+      <c r="R80">
+        <v>78</v>
+      </c>
+      <c r="S80">
         <v>6568</v>
       </c>
-      <c r="R80">
+      <c r="T80">
         <v>6923</v>
       </c>
-      <c r="S80" t="s">
-        <v>98</v>
-      </c>
-      <c r="T80">
+      <c r="U80" t="s">
+        <v>100</v>
+      </c>
+      <c r="V80">
         <v>355</v>
       </c>
-      <c r="U80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21">
+      <c r="W80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5981,22 +6467,28 @@
         <v>79</v>
       </c>
       <c r="Q81">
+        <v>79</v>
+      </c>
+      <c r="R81">
+        <v>79</v>
+      </c>
+      <c r="S81">
         <v>6701</v>
       </c>
-      <c r="R81">
+      <c r="T81">
         <v>7056</v>
       </c>
-      <c r="S81" t="s">
-        <v>99</v>
-      </c>
-      <c r="T81">
+      <c r="U81" t="s">
+        <v>101</v>
+      </c>
+      <c r="V81">
         <v>355</v>
       </c>
-      <c r="U81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21">
+      <c r="W81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -6046,22 +6538,28 @@
         <v>80</v>
       </c>
       <c r="Q82">
+        <v>80</v>
+      </c>
+      <c r="R82">
+        <v>80</v>
+      </c>
+      <c r="S82">
         <v>6829</v>
       </c>
-      <c r="R82">
+      <c r="T82">
         <v>7186</v>
       </c>
-      <c r="S82" t="s">
-        <v>100</v>
-      </c>
-      <c r="T82">
+      <c r="U82" t="s">
+        <v>102</v>
+      </c>
+      <c r="V82">
         <v>357</v>
       </c>
-      <c r="U82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21">
+      <c r="W82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -6111,22 +6609,28 @@
         <v>81</v>
       </c>
       <c r="Q83">
+        <v>81</v>
+      </c>
+      <c r="R83">
+        <v>81</v>
+      </c>
+      <c r="S83">
         <v>6973</v>
       </c>
-      <c r="R83">
+      <c r="T83">
         <v>7331</v>
       </c>
-      <c r="S83" t="s">
-        <v>101</v>
-      </c>
-      <c r="T83">
+      <c r="U83" t="s">
+        <v>103</v>
+      </c>
+      <c r="V83">
         <v>358</v>
       </c>
-      <c r="U83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21">
+      <c r="W83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -6176,22 +6680,28 @@
         <v>82</v>
       </c>
       <c r="Q84">
+        <v>82</v>
+      </c>
+      <c r="R84">
+        <v>82</v>
+      </c>
+      <c r="S84">
         <v>7124</v>
       </c>
-      <c r="R84">
+      <c r="T84">
         <v>7483</v>
       </c>
-      <c r="S84" t="s">
-        <v>102</v>
-      </c>
-      <c r="T84">
+      <c r="U84" t="s">
+        <v>104</v>
+      </c>
+      <c r="V84">
         <v>359</v>
       </c>
-      <c r="U84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21">
+      <c r="W84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -6241,22 +6751,28 @@
         <v>83</v>
       </c>
       <c r="Q85">
+        <v>83</v>
+      </c>
+      <c r="R85">
+        <v>83</v>
+      </c>
+      <c r="S85">
         <v>7229</v>
       </c>
-      <c r="R85">
+      <c r="T85">
         <v>7592</v>
       </c>
-      <c r="S85" t="s">
-        <v>103</v>
-      </c>
-      <c r="T85">
+      <c r="U85" t="s">
+        <v>105</v>
+      </c>
+      <c r="V85">
         <v>363</v>
       </c>
-      <c r="U85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21">
+      <c r="W85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -6306,22 +6822,28 @@
         <v>84</v>
       </c>
       <c r="Q86">
+        <v>84</v>
+      </c>
+      <c r="R86">
+        <v>84</v>
+      </c>
+      <c r="S86">
         <v>7434</v>
       </c>
-      <c r="R86">
+      <c r="T86">
         <v>7799</v>
       </c>
-      <c r="S86" t="s">
-        <v>104</v>
-      </c>
-      <c r="T86">
+      <c r="U86" t="s">
+        <v>106</v>
+      </c>
+      <c r="V86">
         <v>365</v>
       </c>
-      <c r="U86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:21">
+      <c r="W86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -6371,22 +6893,28 @@
         <v>85</v>
       </c>
       <c r="Q87">
+        <v>85</v>
+      </c>
+      <c r="R87">
+        <v>85</v>
+      </c>
+      <c r="S87">
         <v>7548</v>
       </c>
-      <c r="R87">
+      <c r="T87">
         <v>7915</v>
       </c>
-      <c r="S87" t="s">
-        <v>105</v>
-      </c>
-      <c r="T87">
+      <c r="U87" t="s">
+        <v>107</v>
+      </c>
+      <c r="V87">
         <v>367</v>
       </c>
-      <c r="U87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:21">
+      <c r="W87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -6436,22 +6964,28 @@
         <v>86</v>
       </c>
       <c r="Q88">
+        <v>86</v>
+      </c>
+      <c r="R88">
+        <v>86</v>
+      </c>
+      <c r="S88">
         <v>7725</v>
       </c>
-      <c r="R88">
+      <c r="T88">
         <v>8100</v>
       </c>
-      <c r="S88" t="s">
-        <v>106</v>
-      </c>
-      <c r="T88">
+      <c r="U88" t="s">
+        <v>108</v>
+      </c>
+      <c r="V88">
         <v>375</v>
       </c>
-      <c r="U88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:21">
+      <c r="W88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -6501,22 +7035,28 @@
         <v>87</v>
       </c>
       <c r="Q89">
+        <v>87</v>
+      </c>
+      <c r="R89">
+        <v>87</v>
+      </c>
+      <c r="S89">
         <v>7937</v>
       </c>
-      <c r="R89">
+      <c r="T89">
         <v>8314</v>
       </c>
-      <c r="S89" t="s">
-        <v>107</v>
-      </c>
-      <c r="T89">
+      <c r="U89" t="s">
+        <v>109</v>
+      </c>
+      <c r="V89">
         <v>377</v>
       </c>
-      <c r="U89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:21">
+      <c r="W89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -6566,22 +7106,28 @@
         <v>88</v>
       </c>
       <c r="Q90">
+        <v>88</v>
+      </c>
+      <c r="R90">
+        <v>88</v>
+      </c>
+      <c r="S90">
         <v>8179</v>
       </c>
-      <c r="R90">
+      <c r="T90">
         <v>8556</v>
       </c>
-      <c r="S90" t="s">
-        <v>108</v>
-      </c>
-      <c r="T90">
+      <c r="U90" t="s">
+        <v>110</v>
+      </c>
+      <c r="V90">
         <v>377</v>
       </c>
-      <c r="U90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21">
+      <c r="W90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -6612,23 +7158,29 @@
       <c r="J91">
         <v>89</v>
       </c>
-      <c r="Q91">
+      <c r="K91">
+        <v>89</v>
+      </c>
+      <c r="L91">
+        <v>89</v>
+      </c>
+      <c r="S91">
         <v>8357</v>
       </c>
-      <c r="R91">
+      <c r="T91">
         <v>8735</v>
       </c>
-      <c r="S91" t="s">
-        <v>109</v>
-      </c>
-      <c r="T91">
+      <c r="U91" t="s">
+        <v>111</v>
+      </c>
+      <c r="V91">
         <v>378</v>
       </c>
-      <c r="U91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:21">
+      <c r="W91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -6656,23 +7208,29 @@
       <c r="I92">
         <v>90</v>
       </c>
-      <c r="Q92">
+      <c r="J92">
+        <v>90</v>
+      </c>
+      <c r="K92">
+        <v>90</v>
+      </c>
+      <c r="S92">
         <v>8436</v>
       </c>
-      <c r="R92">
+      <c r="T92">
         <v>8815</v>
       </c>
-      <c r="S92" t="s">
-        <v>110</v>
-      </c>
-      <c r="T92">
+      <c r="U92" t="s">
+        <v>112</v>
+      </c>
+      <c r="V92">
         <v>379</v>
       </c>
-      <c r="U92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21">
+      <c r="W92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -6700,23 +7258,29 @@
       <c r="I93">
         <v>91</v>
       </c>
-      <c r="Q93">
+      <c r="J93">
+        <v>91</v>
+      </c>
+      <c r="K93">
+        <v>91</v>
+      </c>
+      <c r="S93">
         <v>8777</v>
       </c>
-      <c r="R93">
+      <c r="T93">
         <v>9157</v>
       </c>
-      <c r="S93" t="s">
-        <v>111</v>
-      </c>
-      <c r="T93">
+      <c r="U93" t="s">
+        <v>113</v>
+      </c>
+      <c r="V93">
         <v>380</v>
       </c>
-      <c r="U93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:21">
+      <c r="W93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -6741,23 +7305,29 @@
       <c r="H94">
         <v>92</v>
       </c>
-      <c r="Q94">
+      <c r="I94">
+        <v>92</v>
+      </c>
+      <c r="J94">
+        <v>92</v>
+      </c>
+      <c r="S94">
         <v>8932</v>
       </c>
-      <c r="R94">
+      <c r="T94">
         <v>9318</v>
       </c>
-      <c r="S94" t="s">
-        <v>112</v>
-      </c>
-      <c r="T94">
+      <c r="U94" t="s">
+        <v>114</v>
+      </c>
+      <c r="V94">
         <v>386</v>
       </c>
-      <c r="U94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:21">
+      <c r="W94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -6779,23 +7349,29 @@
       <c r="G95">
         <v>93</v>
       </c>
-      <c r="Q95">
+      <c r="H95">
+        <v>93</v>
+      </c>
+      <c r="I95">
+        <v>93</v>
+      </c>
+      <c r="S95">
         <v>9148</v>
       </c>
-      <c r="R95">
+      <c r="T95">
         <v>9535</v>
       </c>
-      <c r="S95" t="s">
-        <v>113</v>
-      </c>
-      <c r="T95">
+      <c r="U95" t="s">
+        <v>115</v>
+      </c>
+      <c r="V95">
         <v>387</v>
       </c>
-      <c r="U95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:21">
+      <c r="W95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -6817,23 +7393,29 @@
       <c r="G96">
         <v>94</v>
       </c>
-      <c r="Q96">
+      <c r="H96">
+        <v>94</v>
+      </c>
+      <c r="I96">
+        <v>94</v>
+      </c>
+      <c r="S96">
         <v>9462</v>
       </c>
-      <c r="R96">
+      <c r="T96">
         <v>9852</v>
       </c>
-      <c r="S96" t="s">
-        <v>114</v>
-      </c>
-      <c r="T96">
+      <c r="U96" t="s">
+        <v>116</v>
+      </c>
+      <c r="V96">
         <v>390</v>
       </c>
-      <c r="U96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:21">
+      <c r="W96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -6855,23 +7437,29 @@
       <c r="G97">
         <v>95</v>
       </c>
-      <c r="Q97">
+      <c r="H97">
+        <v>95</v>
+      </c>
+      <c r="I97">
+        <v>95</v>
+      </c>
+      <c r="S97">
         <v>9862</v>
       </c>
-      <c r="R97">
+      <c r="T97">
         <v>10259</v>
       </c>
-      <c r="S97" t="s">
-        <v>115</v>
-      </c>
-      <c r="T97">
+      <c r="U97" t="s">
+        <v>117</v>
+      </c>
+      <c r="V97">
         <v>397</v>
       </c>
-      <c r="U97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:21">
+      <c r="W97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6893,62 +7481,80 @@
       <c r="G98">
         <v>96</v>
       </c>
-      <c r="Q98">
+      <c r="H98">
+        <v>96</v>
+      </c>
+      <c r="I98">
+        <v>96</v>
+      </c>
+      <c r="S98">
         <v>10088</v>
       </c>
-      <c r="R98">
+      <c r="T98">
         <v>10486</v>
       </c>
-      <c r="S98" t="s">
-        <v>116</v>
-      </c>
-      <c r="T98">
+      <c r="U98" t="s">
+        <v>118</v>
+      </c>
+      <c r="V98">
         <v>398</v>
       </c>
-      <c r="U98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:21">
+      <c r="W98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99">
         <v>97</v>
       </c>
-      <c r="Q99">
+      <c r="C99">
+        <v>97</v>
+      </c>
+      <c r="D99">
+        <v>97</v>
+      </c>
+      <c r="S99">
         <v>10374</v>
       </c>
-      <c r="R99">
+      <c r="T99">
         <v>10774</v>
       </c>
-      <c r="S99" t="s">
-        <v>117</v>
-      </c>
-      <c r="T99">
+      <c r="U99" t="s">
+        <v>119</v>
+      </c>
+      <c r="V99">
         <v>400</v>
       </c>
-      <c r="U99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:21">
+      <c r="W99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23">
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="Q100">
+      <c r="B100">
+        <v>98</v>
+      </c>
+      <c r="C100">
+        <v>98</v>
+      </c>
+      <c r="S100">
         <v>10374</v>
       </c>
-      <c r="R100">
+      <c r="T100">
         <v>10774</v>
       </c>
-      <c r="S100" t="s">
-        <v>118</v>
-      </c>
-      <c r="T100">
+      <c r="U100" t="s">
+        <v>120</v>
+      </c>
+      <c r="V100">
         <v>400</v>
       </c>
-      <c r="U100">
+      <c r="W100">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manual update after code edits.
</commit_message>
<xml_diff>
--- a/Clark_Data.xlsx
+++ b/Clark_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -70,6 +70,9 @@
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
@@ -383,6 +386,24 @@
   </si>
   <si>
     <t>06-24-2020</t>
+  </si>
+  <si>
+    <t>06-25-2020</t>
+  </si>
+  <si>
+    <t>06-26-2020</t>
+  </si>
+  <si>
+    <t>06-27-2020</t>
+  </si>
+  <si>
+    <t>06-28-2020</t>
+  </si>
+  <si>
+    <t>06-29-2020</t>
+  </si>
+  <si>
+    <t>06-30-2020</t>
   </si>
 </sst>
 </file>
@@ -740,13 +761,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X101"/>
+  <dimension ref="A1:Y107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,8 +837,11 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:24">
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -879,19 +903,22 @@
         <v>0</v>
       </c>
       <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
         <v>1</v>
       </c>
-      <c r="V2" t="s">
-        <v>23</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
+      <c r="W2" t="s">
+        <v>24</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -950,22 +977,25 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
         <v>1</v>
       </c>
-      <c r="V3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
+      <c r="W3" t="s">
+        <v>25</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1024,22 +1054,25 @@
         <v>2</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>1</v>
       </c>
-      <c r="V4" t="s">
-        <v>25</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
+      <c r="W4" t="s">
+        <v>26</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1098,22 +1131,25 @@
         <v>3</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
         <v>2</v>
       </c>
-      <c r="V5" t="s">
-        <v>26</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
+      <c r="W5" t="s">
+        <v>27</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1172,22 +1208,25 @@
         <v>4</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>2</v>
       </c>
-      <c r="V6" t="s">
-        <v>27</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
+      <c r="W6" t="s">
+        <v>28</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1246,22 +1285,25 @@
         <v>5</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>126</v>
       </c>
-      <c r="V7" t="s">
-        <v>28</v>
-      </c>
-      <c r="W7">
+      <c r="W7" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7">
         <v>2</v>
       </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Y7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1320,22 +1362,25 @@
         <v>6</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
         <v>126</v>
       </c>
-      <c r="V8" t="s">
-        <v>29</v>
-      </c>
-      <c r="W8">
+      <c r="W8" t="s">
+        <v>30</v>
+      </c>
+      <c r="X8">
         <v>4</v>
       </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Y8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1394,22 +1439,25 @@
         <v>7</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
         <v>212</v>
       </c>
-      <c r="V9" t="s">
-        <v>30</v>
-      </c>
-      <c r="W9">
+      <c r="W9" t="s">
+        <v>31</v>
+      </c>
+      <c r="X9">
         <v>4</v>
       </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1468,22 +1516,25 @@
         <v>8</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
         <v>249</v>
       </c>
-      <c r="V10" t="s">
-        <v>31</v>
-      </c>
-      <c r="W10">
+      <c r="W10" t="s">
+        <v>32</v>
+      </c>
+      <c r="X10">
         <v>6</v>
       </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Y10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1542,22 +1593,25 @@
         <v>9</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
         <v>350</v>
       </c>
-      <c r="V11" t="s">
-        <v>32</v>
-      </c>
-      <c r="W11">
+      <c r="W11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X11">
         <v>6</v>
       </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="Y11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1616,22 +1670,25 @@
         <v>10</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
         <v>443</v>
       </c>
-      <c r="V12" t="s">
-        <v>33</v>
-      </c>
-      <c r="W12">
+      <c r="W12" t="s">
+        <v>34</v>
+      </c>
+      <c r="X12">
         <v>10</v>
       </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1690,22 +1747,25 @@
         <v>11</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
         <v>443</v>
       </c>
-      <c r="V13" t="s">
-        <v>34</v>
-      </c>
-      <c r="W13">
+      <c r="W13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X13">
         <v>10</v>
       </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Y13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1764,22 +1824,25 @@
         <v>12</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
         <v>528</v>
       </c>
-      <c r="V14" t="s">
-        <v>35</v>
-      </c>
-      <c r="W14">
+      <c r="W14" t="s">
+        <v>36</v>
+      </c>
+      <c r="X14">
         <v>14</v>
       </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="Y14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1838,22 +1901,25 @@
         <v>13</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
         <v>753</v>
       </c>
-      <c r="V15" t="s">
-        <v>36</v>
-      </c>
-      <c r="W15">
+      <c r="W15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X15">
         <v>14</v>
       </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Y15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1912,22 +1978,25 @@
         <v>14</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
         <v>869</v>
       </c>
-      <c r="V16" t="s">
-        <v>37</v>
-      </c>
-      <c r="W16">
+      <c r="W16" t="s">
+        <v>38</v>
+      </c>
+      <c r="X16">
         <v>23</v>
       </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
+      <c r="Y16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1986,22 +2055,25 @@
         <v>15</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>961</v>
       </c>
-      <c r="V17" t="s">
-        <v>38</v>
-      </c>
-      <c r="W17">
+      <c r="W17" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17">
         <v>28</v>
       </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2060,22 +2132,25 @@
         <v>16</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
         <v>1125</v>
       </c>
-      <c r="V18" t="s">
-        <v>39</v>
-      </c>
-      <c r="W18">
+      <c r="W18" t="s">
+        <v>40</v>
+      </c>
+      <c r="X18">
         <v>34</v>
       </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2134,22 +2209,25 @@
         <v>17</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
         <v>1279</v>
       </c>
-      <c r="V19" t="s">
-        <v>40</v>
-      </c>
-      <c r="W19">
+      <c r="W19" t="s">
+        <v>41</v>
+      </c>
+      <c r="X19">
         <v>39</v>
       </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2208,22 +2286,25 @@
         <v>18</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
         <v>1418</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
+        <v>42</v>
+      </c>
+      <c r="X20">
         <v>41</v>
       </c>
-      <c r="W20">
-        <v>41</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2282,22 +2363,25 @@
         <v>19</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
         <v>1519</v>
       </c>
-      <c r="V21" t="s">
-        <v>42</v>
-      </c>
-      <c r="W21">
+      <c r="W21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X21">
         <v>41</v>
       </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
+      <c r="Y21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2356,22 +2440,25 @@
         <v>20</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
         <v>1608</v>
       </c>
-      <c r="V22" t="s">
-        <v>43</v>
-      </c>
-      <c r="W22">
+      <c r="W22" t="s">
+        <v>44</v>
+      </c>
+      <c r="X22">
         <v>41</v>
       </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="Y22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2430,22 +2517,25 @@
         <v>21</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
         <v>1734</v>
       </c>
-      <c r="V23" t="s">
-        <v>44</v>
-      </c>
-      <c r="W23">
+      <c r="W23" t="s">
+        <v>45</v>
+      </c>
+      <c r="X23">
         <v>54</v>
       </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24">
+      <c r="Y23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2504,22 +2594,25 @@
         <v>22</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
         <v>1878</v>
       </c>
-      <c r="V24" t="s">
-        <v>45</v>
-      </c>
-      <c r="W24">
+      <c r="W24" t="s">
+        <v>46</v>
+      </c>
+      <c r="X24">
         <v>65</v>
       </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Y24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2578,22 +2671,25 @@
         <v>23</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
         <v>2009</v>
       </c>
-      <c r="V25" t="s">
-        <v>46</v>
-      </c>
-      <c r="W25">
+      <c r="W25" t="s">
+        <v>47</v>
+      </c>
+      <c r="X25">
         <v>71</v>
       </c>
-      <c r="X25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="Y25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2652,22 +2748,25 @@
         <v>24</v>
       </c>
       <c r="T26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
         <v>2144</v>
       </c>
-      <c r="V26" t="s">
-        <v>47</v>
-      </c>
-      <c r="W26">
+      <c r="W26" t="s">
+        <v>48</v>
+      </c>
+      <c r="X26">
         <v>75</v>
       </c>
-      <c r="X26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="Y26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2726,22 +2825,25 @@
         <v>25</v>
       </c>
       <c r="T27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
         <v>2144</v>
       </c>
-      <c r="V27" t="s">
-        <v>48</v>
-      </c>
-      <c r="W27">
+      <c r="W27" t="s">
+        <v>49</v>
+      </c>
+      <c r="X27">
         <v>75</v>
       </c>
-      <c r="X27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="Y27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2800,22 +2902,25 @@
         <v>26</v>
       </c>
       <c r="T28">
+        <v>26</v>
+      </c>
+      <c r="U28">
         <v>2224</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>2324</v>
       </c>
-      <c r="V28" t="s">
-        <v>49</v>
-      </c>
-      <c r="W28">
+      <c r="W28" t="s">
+        <v>50</v>
+      </c>
+      <c r="X28">
         <v>100</v>
       </c>
-      <c r="X28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="Y28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2874,22 +2979,25 @@
         <v>27</v>
       </c>
       <c r="T29">
+        <v>27</v>
+      </c>
+      <c r="U29">
         <v>2343</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>2444</v>
       </c>
-      <c r="V29" t="s">
-        <v>50</v>
-      </c>
-      <c r="W29">
+      <c r="W29" t="s">
+        <v>51</v>
+      </c>
+      <c r="X29">
         <v>101</v>
       </c>
-      <c r="X29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="Y29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2948,22 +3056,25 @@
         <v>28</v>
       </c>
       <c r="T30">
+        <v>28</v>
+      </c>
+      <c r="U30">
         <v>2403</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>2509</v>
       </c>
-      <c r="V30" t="s">
-        <v>51</v>
-      </c>
-      <c r="W30">
+      <c r="W30" t="s">
+        <v>52</v>
+      </c>
+      <c r="X30">
         <v>106</v>
       </c>
-      <c r="X30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="Y30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3022,22 +3133,25 @@
         <v>29</v>
       </c>
       <c r="T31">
+        <v>29</v>
+      </c>
+      <c r="U31">
         <v>2444</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <v>2559</v>
       </c>
-      <c r="V31" t="s">
-        <v>52</v>
-      </c>
-      <c r="W31">
+      <c r="W31" t="s">
+        <v>53</v>
+      </c>
+      <c r="X31">
         <v>115</v>
       </c>
-      <c r="X31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="Y31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3096,22 +3210,25 @@
         <v>30</v>
       </c>
       <c r="T32">
+        <v>30</v>
+      </c>
+      <c r="U32">
         <v>2444</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <v>2559</v>
       </c>
-      <c r="V32" t="s">
-        <v>53</v>
-      </c>
-      <c r="W32">
+      <c r="W32" t="s">
+        <v>54</v>
+      </c>
+      <c r="X32">
         <v>115</v>
       </c>
-      <c r="X32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="Y32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3170,22 +3287,25 @@
         <v>31</v>
       </c>
       <c r="T33">
+        <v>31</v>
+      </c>
+      <c r="U33">
         <v>2614</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <v>2738</v>
       </c>
-      <c r="V33" t="s">
-        <v>54</v>
-      </c>
-      <c r="W33">
+      <c r="W33" t="s">
+        <v>55</v>
+      </c>
+      <c r="X33">
         <v>124</v>
       </c>
-      <c r="X33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="Y33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3244,22 +3364,25 @@
         <v>32</v>
       </c>
       <c r="T34">
+        <v>32</v>
+      </c>
+      <c r="U34">
         <v>2749</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <v>2882</v>
       </c>
-      <c r="V34" t="s">
-        <v>55</v>
-      </c>
-      <c r="W34">
+      <c r="W34" t="s">
+        <v>56</v>
+      </c>
+      <c r="X34">
         <v>133</v>
       </c>
-      <c r="X34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="Y34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3318,22 +3441,25 @@
         <v>33</v>
       </c>
       <c r="T35">
+        <v>33</v>
+      </c>
+      <c r="U35">
         <v>2803</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <v>2940</v>
       </c>
-      <c r="V35" t="s">
-        <v>56</v>
-      </c>
-      <c r="W35">
+      <c r="W35" t="s">
+        <v>57</v>
+      </c>
+      <c r="X35">
         <v>137</v>
       </c>
-      <c r="X35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24">
+      <c r="Y35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3392,22 +3518,25 @@
         <v>34</v>
       </c>
       <c r="T36">
+        <v>34</v>
+      </c>
+      <c r="U36">
         <v>2861</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <v>2998</v>
       </c>
-      <c r="V36" t="s">
-        <v>57</v>
-      </c>
-      <c r="W36">
+      <c r="W36" t="s">
+        <v>58</v>
+      </c>
+      <c r="X36">
         <v>137</v>
       </c>
-      <c r="X36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24">
+      <c r="Y36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3466,22 +3595,25 @@
         <v>35</v>
       </c>
       <c r="T37">
+        <v>35</v>
+      </c>
+      <c r="U37">
         <v>2958</v>
       </c>
-      <c r="U37">
+      <c r="V37">
         <v>3099</v>
       </c>
-      <c r="V37" t="s">
-        <v>58</v>
-      </c>
-      <c r="W37">
+      <c r="W37" t="s">
+        <v>59</v>
+      </c>
+      <c r="X37">
         <v>141</v>
       </c>
-      <c r="X37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="Y37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3540,22 +3672,25 @@
         <v>36</v>
       </c>
       <c r="T38">
+        <v>36</v>
+      </c>
+      <c r="U38">
         <v>3068</v>
       </c>
-      <c r="U38">
+      <c r="V38">
         <v>3218</v>
       </c>
-      <c r="V38" t="s">
-        <v>59</v>
-      </c>
-      <c r="W38">
+      <c r="W38" t="s">
+        <v>60</v>
+      </c>
+      <c r="X38">
         <v>150</v>
       </c>
-      <c r="X38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24">
+      <c r="Y38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3614,22 +3749,25 @@
         <v>37</v>
       </c>
       <c r="T39">
+        <v>37</v>
+      </c>
+      <c r="U39">
         <v>3151</v>
       </c>
-      <c r="U39">
+      <c r="V39">
         <v>3314</v>
       </c>
-      <c r="V39" t="s">
-        <v>60</v>
-      </c>
-      <c r="W39">
+      <c r="W39" t="s">
+        <v>61</v>
+      </c>
+      <c r="X39">
         <v>163</v>
       </c>
-      <c r="X39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24">
+      <c r="Y39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3688,22 +3826,25 @@
         <v>38</v>
       </c>
       <c r="T40">
+        <v>38</v>
+      </c>
+      <c r="U40">
         <v>3275</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>3443</v>
       </c>
-      <c r="V40" t="s">
-        <v>61</v>
-      </c>
-      <c r="W40">
+      <c r="W40" t="s">
+        <v>62</v>
+      </c>
+      <c r="X40">
         <v>168</v>
       </c>
-      <c r="X40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="Y40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3762,22 +3903,25 @@
         <v>39</v>
       </c>
       <c r="T41">
+        <v>39</v>
+      </c>
+      <c r="U41">
         <v>3396</v>
       </c>
-      <c r="U41">
+      <c r="V41">
         <v>3570</v>
       </c>
-      <c r="V41" t="s">
-        <v>62</v>
-      </c>
-      <c r="W41">
+      <c r="W41" t="s">
+        <v>63</v>
+      </c>
+      <c r="X41">
         <v>174</v>
       </c>
-      <c r="X41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24">
+      <c r="Y41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3836,22 +3980,25 @@
         <v>40</v>
       </c>
       <c r="T42">
+        <v>40</v>
+      </c>
+      <c r="U42">
         <v>3491</v>
       </c>
-      <c r="U42">
+      <c r="V42">
         <v>3665</v>
       </c>
-      <c r="V42" t="s">
-        <v>63</v>
-      </c>
-      <c r="W42">
+      <c r="W42" t="s">
+        <v>64</v>
+      </c>
+      <c r="X42">
         <v>174</v>
       </c>
-      <c r="X42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24">
+      <c r="Y42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3910,22 +4057,25 @@
         <v>41</v>
       </c>
       <c r="T43">
+        <v>41</v>
+      </c>
+      <c r="U43">
         <v>3543</v>
       </c>
-      <c r="U43">
+      <c r="V43">
         <v>3717</v>
       </c>
-      <c r="V43" t="s">
-        <v>64</v>
-      </c>
-      <c r="W43">
+      <c r="W43" t="s">
+        <v>65</v>
+      </c>
+      <c r="X43">
         <v>174</v>
       </c>
-      <c r="X43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24">
+      <c r="Y43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3984,22 +4134,25 @@
         <v>42</v>
       </c>
       <c r="T44">
+        <v>42</v>
+      </c>
+      <c r="U44">
         <v>3607</v>
       </c>
-      <c r="U44">
+      <c r="V44">
         <v>3793</v>
       </c>
-      <c r="V44" t="s">
-        <v>65</v>
-      </c>
-      <c r="W44">
+      <c r="W44" t="s">
+        <v>66</v>
+      </c>
+      <c r="X44">
         <v>186</v>
       </c>
-      <c r="X44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="Y44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4058,22 +4211,25 @@
         <v>43</v>
       </c>
       <c r="T45">
+        <v>43</v>
+      </c>
+      <c r="U45">
         <v>3695</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <v>3891</v>
       </c>
-      <c r="V45" t="s">
-        <v>66</v>
-      </c>
-      <c r="W45">
+      <c r="W45" t="s">
+        <v>67</v>
+      </c>
+      <c r="X45">
         <v>196</v>
       </c>
-      <c r="X45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24">
+      <c r="Y45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4132,22 +4288,25 @@
         <v>44</v>
       </c>
       <c r="T46">
+        <v>44</v>
+      </c>
+      <c r="U46">
         <v>3777</v>
       </c>
-      <c r="U46">
+      <c r="V46">
         <v>3979</v>
       </c>
-      <c r="V46" t="s">
-        <v>67</v>
-      </c>
-      <c r="W46">
+      <c r="W46" t="s">
+        <v>68</v>
+      </c>
+      <c r="X46">
         <v>202</v>
       </c>
-      <c r="X46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24">
+      <c r="Y46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4206,22 +4365,25 @@
         <v>45</v>
       </c>
       <c r="T47">
+        <v>45</v>
+      </c>
+      <c r="U47">
         <v>3912</v>
       </c>
-      <c r="U47">
+      <c r="V47">
         <v>4118</v>
       </c>
-      <c r="V47" t="s">
-        <v>68</v>
-      </c>
-      <c r="W47">
+      <c r="W47" t="s">
+        <v>69</v>
+      </c>
+      <c r="X47">
         <v>206</v>
       </c>
-      <c r="X47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24">
+      <c r="Y47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4280,22 +4442,25 @@
         <v>46</v>
       </c>
       <c r="T48">
+        <v>46</v>
+      </c>
+      <c r="U48">
         <v>4010</v>
       </c>
-      <c r="U48">
+      <c r="V48">
         <v>4225</v>
       </c>
-      <c r="V48" t="s">
-        <v>69</v>
-      </c>
-      <c r="W48">
+      <c r="W48" t="s">
+        <v>70</v>
+      </c>
+      <c r="X48">
         <v>215</v>
       </c>
-      <c r="X48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24">
+      <c r="Y48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4354,22 +4519,25 @@
         <v>47</v>
       </c>
       <c r="T49">
+        <v>47</v>
+      </c>
+      <c r="U49">
         <v>4056</v>
       </c>
-      <c r="U49">
+      <c r="V49">
         <v>4274</v>
       </c>
-      <c r="V49" t="s">
-        <v>70</v>
-      </c>
-      <c r="W49">
+      <c r="W49" t="s">
+        <v>71</v>
+      </c>
+      <c r="X49">
         <v>218</v>
       </c>
-      <c r="X49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24">
+      <c r="Y49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4428,22 +4596,25 @@
         <v>48</v>
       </c>
       <c r="T50">
+        <v>48</v>
+      </c>
+      <c r="U50">
         <v>4188</v>
       </c>
-      <c r="U50">
+      <c r="V50">
         <v>4411</v>
       </c>
-      <c r="V50" t="s">
-        <v>71</v>
-      </c>
-      <c r="W50">
+      <c r="W50" t="s">
+        <v>72</v>
+      </c>
+      <c r="X50">
         <v>223</v>
       </c>
-      <c r="X50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
+      <c r="Y50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4502,22 +4673,25 @@
         <v>49</v>
       </c>
       <c r="T51">
+        <v>49</v>
+      </c>
+      <c r="U51">
         <v>4182</v>
       </c>
-      <c r="U51">
+      <c r="V51">
         <v>4408</v>
       </c>
-      <c r="V51" t="s">
-        <v>72</v>
-      </c>
-      <c r="W51">
+      <c r="W51" t="s">
+        <v>73</v>
+      </c>
+      <c r="X51">
         <v>226</v>
       </c>
-      <c r="X51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24">
+      <c r="Y51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4576,22 +4750,25 @@
         <v>50</v>
       </c>
       <c r="T52">
+        <v>50</v>
+      </c>
+      <c r="U52">
         <v>4235</v>
       </c>
-      <c r="U52">
+      <c r="V52">
         <v>4473</v>
       </c>
-      <c r="V52" t="s">
-        <v>73</v>
-      </c>
-      <c r="W52">
+      <c r="W52" t="s">
+        <v>74</v>
+      </c>
+      <c r="X52">
         <v>238</v>
       </c>
-      <c r="X52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24">
+      <c r="Y52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4650,22 +4827,25 @@
         <v>51</v>
       </c>
       <c r="T53">
+        <v>51</v>
+      </c>
+      <c r="U53">
         <v>4328</v>
       </c>
-      <c r="U53">
+      <c r="V53">
         <v>4573</v>
       </c>
-      <c r="V53" t="s">
-        <v>74</v>
-      </c>
-      <c r="W53">
+      <c r="W53" t="s">
+        <v>75</v>
+      </c>
+      <c r="X53">
         <v>245</v>
       </c>
-      <c r="X53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24">
+      <c r="Y53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4724,22 +4904,25 @@
         <v>52</v>
       </c>
       <c r="T54">
+        <v>52</v>
+      </c>
+      <c r="U54">
         <v>4328</v>
       </c>
-      <c r="U54">
+      <c r="V54">
         <v>4573</v>
       </c>
-      <c r="V54" t="s">
-        <v>75</v>
-      </c>
-      <c r="W54">
+      <c r="W54" t="s">
+        <v>76</v>
+      </c>
+      <c r="X54">
         <v>245</v>
       </c>
-      <c r="X54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24">
+      <c r="Y54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4798,22 +4981,25 @@
         <v>53</v>
       </c>
       <c r="T55">
+        <v>53</v>
+      </c>
+      <c r="U55">
         <v>4448</v>
       </c>
-      <c r="U55">
+      <c r="V55">
         <v>4704</v>
       </c>
-      <c r="V55" t="s">
-        <v>76</v>
-      </c>
-      <c r="W55">
+      <c r="W55" t="s">
+        <v>77</v>
+      </c>
+      <c r="X55">
         <v>256</v>
       </c>
-      <c r="X55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24">
+      <c r="Y55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4872,22 +5058,25 @@
         <v>54</v>
       </c>
       <c r="T56">
+        <v>54</v>
+      </c>
+      <c r="U56">
         <v>4490</v>
       </c>
-      <c r="U56">
+      <c r="V56">
         <v>4750</v>
       </c>
-      <c r="V56" t="s">
-        <v>77</v>
-      </c>
-      <c r="W56">
+      <c r="W56" t="s">
+        <v>78</v>
+      </c>
+      <c r="X56">
         <v>260</v>
       </c>
-      <c r="X56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24">
+      <c r="Y56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4946,22 +5135,25 @@
         <v>55</v>
       </c>
       <c r="T57">
+        <v>55</v>
+      </c>
+      <c r="U57">
         <v>4502</v>
       </c>
-      <c r="U57">
+      <c r="V57">
         <v>4762</v>
       </c>
-      <c r="V57" t="s">
-        <v>78</v>
-      </c>
-      <c r="W57">
+      <c r="W57" t="s">
+        <v>79</v>
+      </c>
+      <c r="X57">
         <v>260</v>
       </c>
-      <c r="X57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24">
+      <c r="Y57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5020,22 +5212,25 @@
         <v>56</v>
       </c>
       <c r="T58">
+        <v>56</v>
+      </c>
+      <c r="U58">
         <v>4602</v>
       </c>
-      <c r="U58">
+      <c r="V58">
         <v>4869</v>
       </c>
-      <c r="V58" t="s">
-        <v>79</v>
-      </c>
-      <c r="W58">
+      <c r="W58" t="s">
+        <v>80</v>
+      </c>
+      <c r="X58">
         <v>267</v>
       </c>
-      <c r="X58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24">
+      <c r="Y58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5094,22 +5289,25 @@
         <v>57</v>
       </c>
       <c r="T59">
+        <v>57</v>
+      </c>
+      <c r="U59">
         <v>4770</v>
       </c>
-      <c r="U59">
+      <c r="V59">
         <v>5045</v>
       </c>
-      <c r="V59" t="s">
-        <v>80</v>
-      </c>
-      <c r="W59">
+      <c r="W59" t="s">
+        <v>81</v>
+      </c>
+      <c r="X59">
         <v>275</v>
       </c>
-      <c r="X59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24">
+      <c r="Y59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5168,22 +5366,25 @@
         <v>58</v>
       </c>
       <c r="T60">
+        <v>58</v>
+      </c>
+      <c r="U60">
         <v>4770</v>
       </c>
-      <c r="U60">
+      <c r="V60">
         <v>5045</v>
       </c>
-      <c r="V60" t="s">
-        <v>81</v>
-      </c>
-      <c r="W60">
+      <c r="W60" t="s">
+        <v>82</v>
+      </c>
+      <c r="X60">
         <v>275</v>
       </c>
-      <c r="X60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24">
+      <c r="Y60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5242,22 +5443,25 @@
         <v>59</v>
       </c>
       <c r="T61">
+        <v>59</v>
+      </c>
+      <c r="U61">
         <v>4944</v>
       </c>
-      <c r="U61">
+      <c r="V61">
         <v>5235</v>
       </c>
-      <c r="V61" t="s">
-        <v>82</v>
-      </c>
-      <c r="W61">
+      <c r="W61" t="s">
+        <v>83</v>
+      </c>
+      <c r="X61">
         <v>291</v>
       </c>
-      <c r="X61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24">
+      <c r="Y61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5316,22 +5520,25 @@
         <v>60</v>
       </c>
       <c r="T62">
+        <v>60</v>
+      </c>
+      <c r="U62">
         <v>5005</v>
       </c>
-      <c r="U62">
+      <c r="V62">
         <v>5298</v>
       </c>
-      <c r="V62" t="s">
-        <v>83</v>
-      </c>
-      <c r="W62">
+      <c r="W62" t="s">
+        <v>84</v>
+      </c>
+      <c r="X62">
         <v>293</v>
       </c>
-      <c r="X62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24">
+      <c r="Y62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5390,22 +5597,25 @@
         <v>61</v>
       </c>
       <c r="T63">
+        <v>61</v>
+      </c>
+      <c r="U63">
         <v>5070</v>
       </c>
-      <c r="U63">
+      <c r="V63">
         <v>5366</v>
       </c>
-      <c r="V63" t="s">
-        <v>84</v>
-      </c>
-      <c r="W63">
+      <c r="W63" t="s">
+        <v>85</v>
+      </c>
+      <c r="X63">
         <v>296</v>
       </c>
-      <c r="X63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24">
+      <c r="Y63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5464,22 +5674,25 @@
         <v>62</v>
       </c>
       <c r="T64">
+        <v>62</v>
+      </c>
+      <c r="U64">
         <v>5167</v>
       </c>
-      <c r="U64">
+      <c r="V64">
         <v>5463</v>
       </c>
-      <c r="V64" t="s">
-        <v>85</v>
-      </c>
-      <c r="W64">
+      <c r="W64" t="s">
+        <v>86</v>
+      </c>
+      <c r="X64">
         <v>296</v>
       </c>
-      <c r="X64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24">
+      <c r="Y64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5538,22 +5751,25 @@
         <v>63</v>
       </c>
       <c r="T65">
+        <v>63</v>
+      </c>
+      <c r="U65">
         <v>5167</v>
       </c>
-      <c r="U65">
+      <c r="V65">
         <v>5463</v>
       </c>
-      <c r="V65" t="s">
-        <v>86</v>
-      </c>
-      <c r="W65">
+      <c r="W65" t="s">
+        <v>87</v>
+      </c>
+      <c r="X65">
         <v>296</v>
       </c>
-      <c r="X65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24">
+      <c r="Y65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5612,22 +5828,25 @@
         <v>64</v>
       </c>
       <c r="T66">
+        <v>64</v>
+      </c>
+      <c r="U66">
         <v>5336</v>
       </c>
-      <c r="U66">
+      <c r="V66">
         <v>5650</v>
       </c>
-      <c r="V66" t="s">
-        <v>87</v>
-      </c>
-      <c r="W66">
+      <c r="W66" t="s">
+        <v>88</v>
+      </c>
+      <c r="X66">
         <v>314</v>
       </c>
-      <c r="X66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24">
+      <c r="Y66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5686,22 +5905,25 @@
         <v>65</v>
       </c>
       <c r="T67">
+        <v>65</v>
+      </c>
+      <c r="U67">
         <v>5414</v>
       </c>
-      <c r="U67">
+      <c r="V67">
         <v>5734</v>
       </c>
-      <c r="V67" t="s">
-        <v>88</v>
-      </c>
-      <c r="W67">
+      <c r="W67" t="s">
+        <v>89</v>
+      </c>
+      <c r="X67">
         <v>320</v>
       </c>
-      <c r="X67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24">
+      <c r="Y67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5760,22 +5982,25 @@
         <v>66</v>
       </c>
       <c r="T68">
+        <v>66</v>
+      </c>
+      <c r="U68">
         <v>5493</v>
       </c>
-      <c r="U68">
+      <c r="V68">
         <v>5815</v>
       </c>
-      <c r="V68" t="s">
-        <v>89</v>
-      </c>
-      <c r="W68">
+      <c r="W68" t="s">
+        <v>90</v>
+      </c>
+      <c r="X68">
         <v>322</v>
       </c>
-      <c r="X68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24">
+      <c r="Y68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5834,22 +6059,25 @@
         <v>67</v>
       </c>
       <c r="T69">
+        <v>67</v>
+      </c>
+      <c r="U69">
         <v>5493</v>
       </c>
-      <c r="U69">
+      <c r="V69">
         <v>5815</v>
       </c>
-      <c r="V69" t="s">
-        <v>90</v>
-      </c>
-      <c r="W69">
+      <c r="W69" t="s">
+        <v>91</v>
+      </c>
+      <c r="X69">
         <v>322</v>
       </c>
-      <c r="X69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24">
+      <c r="Y69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5908,22 +6136,25 @@
         <v>68</v>
       </c>
       <c r="T70">
+        <v>68</v>
+      </c>
+      <c r="U70">
         <v>5818</v>
       </c>
-      <c r="U70">
+      <c r="V70">
         <v>6140</v>
       </c>
-      <c r="V70" t="s">
-        <v>91</v>
-      </c>
-      <c r="W70">
+      <c r="W70" t="s">
+        <v>92</v>
+      </c>
+      <c r="X70">
         <v>322</v>
       </c>
-      <c r="X70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24">
+      <c r="Y70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5982,22 +6213,25 @@
         <v>69</v>
       </c>
       <c r="T71">
+        <v>69</v>
+      </c>
+      <c r="U71">
         <v>5853</v>
       </c>
-      <c r="U71">
+      <c r="V71">
         <v>6182</v>
       </c>
-      <c r="V71" t="s">
-        <v>92</v>
-      </c>
-      <c r="W71">
+      <c r="W71" t="s">
+        <v>93</v>
+      </c>
+      <c r="X71">
         <v>329</v>
       </c>
-      <c r="X71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24">
+      <c r="Y71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -6056,22 +6290,25 @@
         <v>70</v>
       </c>
       <c r="T72">
+        <v>70</v>
+      </c>
+      <c r="U72">
         <v>5897</v>
       </c>
-      <c r="U72">
+      <c r="V72">
         <v>6226</v>
       </c>
-      <c r="V72" t="s">
-        <v>93</v>
-      </c>
-      <c r="W72">
+      <c r="W72" t="s">
+        <v>94</v>
+      </c>
+      <c r="X72">
         <v>329</v>
       </c>
-      <c r="X72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24">
+      <c r="Y72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -6130,22 +6367,25 @@
         <v>71</v>
       </c>
       <c r="T73">
+        <v>71</v>
+      </c>
+      <c r="U73">
         <v>5956</v>
       </c>
-      <c r="U73">
+      <c r="V73">
         <v>6287</v>
       </c>
-      <c r="V73" t="s">
-        <v>94</v>
-      </c>
-      <c r="W73">
+      <c r="W73" t="s">
+        <v>95</v>
+      </c>
+      <c r="X73">
         <v>331</v>
       </c>
-      <c r="X73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24">
+      <c r="Y73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -6204,22 +6444,25 @@
         <v>72</v>
       </c>
       <c r="T74">
+        <v>72</v>
+      </c>
+      <c r="U74">
         <v>6013</v>
       </c>
-      <c r="U74">
+      <c r="V74">
         <v>6352</v>
       </c>
-      <c r="V74" t="s">
-        <v>95</v>
-      </c>
-      <c r="W74">
+      <c r="W74" t="s">
+        <v>96</v>
+      </c>
+      <c r="X74">
         <v>339</v>
       </c>
-      <c r="X74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24">
+      <c r="Y74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -6278,22 +6521,25 @@
         <v>73</v>
       </c>
       <c r="T75">
+        <v>73</v>
+      </c>
+      <c r="U75">
         <v>6118</v>
       </c>
-      <c r="U75">
+      <c r="V75">
         <v>6457</v>
       </c>
-      <c r="V75" t="s">
-        <v>96</v>
-      </c>
-      <c r="W75">
+      <c r="W75" t="s">
+        <v>97</v>
+      </c>
+      <c r="X75">
         <v>339</v>
       </c>
-      <c r="X75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24">
+      <c r="Y75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -6352,22 +6598,25 @@
         <v>74</v>
       </c>
       <c r="T76">
+        <v>74</v>
+      </c>
+      <c r="U76">
         <v>6236</v>
       </c>
-      <c r="U76">
+      <c r="V76">
         <v>6579</v>
       </c>
-      <c r="V76" t="s">
-        <v>97</v>
-      </c>
-      <c r="W76">
+      <c r="W76" t="s">
+        <v>98</v>
+      </c>
+      <c r="X76">
         <v>343</v>
       </c>
-      <c r="X76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24">
+      <c r="Y76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -6426,22 +6675,25 @@
         <v>75</v>
       </c>
       <c r="T77">
+        <v>75</v>
+      </c>
+      <c r="U77">
         <v>6314</v>
       </c>
-      <c r="U77">
+      <c r="V77">
         <v>6657</v>
       </c>
-      <c r="V77" t="s">
-        <v>98</v>
-      </c>
-      <c r="W77">
+      <c r="W77" t="s">
+        <v>99</v>
+      </c>
+      <c r="X77">
         <v>343</v>
       </c>
-      <c r="X77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24">
+      <c r="Y77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -6500,22 +6752,25 @@
         <v>76</v>
       </c>
       <c r="T78">
+        <v>76</v>
+      </c>
+      <c r="U78">
         <v>6376</v>
       </c>
-      <c r="U78">
+      <c r="V78">
         <v>6719</v>
       </c>
-      <c r="V78" t="s">
-        <v>99</v>
-      </c>
-      <c r="W78">
+      <c r="W78" t="s">
+        <v>100</v>
+      </c>
+      <c r="X78">
         <v>343</v>
       </c>
-      <c r="X78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:24">
+      <c r="Y78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -6574,22 +6829,25 @@
         <v>77</v>
       </c>
       <c r="T79">
+        <v>77</v>
+      </c>
+      <c r="U79">
         <v>6502</v>
       </c>
-      <c r="U79">
+      <c r="V79">
         <v>6845</v>
       </c>
-      <c r="V79" t="s">
-        <v>100</v>
-      </c>
-      <c r="W79">
+      <c r="W79" t="s">
+        <v>101</v>
+      </c>
+      <c r="X79">
         <v>343</v>
       </c>
-      <c r="X79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:24">
+      <c r="Y79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -6648,22 +6906,25 @@
         <v>78</v>
       </c>
       <c r="T80">
+        <v>78</v>
+      </c>
+      <c r="U80">
         <v>6568</v>
       </c>
-      <c r="U80">
+      <c r="V80">
         <v>6923</v>
       </c>
-      <c r="V80" t="s">
-        <v>101</v>
-      </c>
-      <c r="W80">
+      <c r="W80" t="s">
+        <v>102</v>
+      </c>
+      <c r="X80">
         <v>355</v>
       </c>
-      <c r="X80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:24">
+      <c r="Y80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -6722,22 +6983,25 @@
         <v>79</v>
       </c>
       <c r="T81">
+        <v>79</v>
+      </c>
+      <c r="U81">
         <v>6701</v>
       </c>
-      <c r="U81">
+      <c r="V81">
         <v>7056</v>
       </c>
-      <c r="V81" t="s">
-        <v>102</v>
-      </c>
-      <c r="W81">
+      <c r="W81" t="s">
+        <v>103</v>
+      </c>
+      <c r="X81">
         <v>355</v>
       </c>
-      <c r="X81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:24">
+      <c r="Y81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -6796,22 +7060,25 @@
         <v>80</v>
       </c>
       <c r="T82">
+        <v>80</v>
+      </c>
+      <c r="U82">
         <v>6829</v>
       </c>
-      <c r="U82">
+      <c r="V82">
         <v>7186</v>
       </c>
-      <c r="V82" t="s">
-        <v>103</v>
-      </c>
-      <c r="W82">
+      <c r="W82" t="s">
+        <v>104</v>
+      </c>
+      <c r="X82">
         <v>357</v>
       </c>
-      <c r="X82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:24">
+      <c r="Y82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -6870,22 +7137,25 @@
         <v>81</v>
       </c>
       <c r="T83">
+        <v>81</v>
+      </c>
+      <c r="U83">
         <v>6973</v>
       </c>
-      <c r="U83">
+      <c r="V83">
         <v>7331</v>
       </c>
-      <c r="V83" t="s">
-        <v>104</v>
-      </c>
-      <c r="W83">
+      <c r="W83" t="s">
+        <v>105</v>
+      </c>
+      <c r="X83">
         <v>358</v>
       </c>
-      <c r="X83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:24">
+      <c r="Y83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -6944,22 +7214,25 @@
         <v>82</v>
       </c>
       <c r="T84">
+        <v>82</v>
+      </c>
+      <c r="U84">
         <v>7124</v>
       </c>
-      <c r="U84">
+      <c r="V84">
         <v>7483</v>
       </c>
-      <c r="V84" t="s">
-        <v>105</v>
-      </c>
-      <c r="W84">
+      <c r="W84" t="s">
+        <v>106</v>
+      </c>
+      <c r="X84">
         <v>359</v>
       </c>
-      <c r="X84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:24">
+      <c r="Y84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -7018,22 +7291,25 @@
         <v>83</v>
       </c>
       <c r="T85">
+        <v>83</v>
+      </c>
+      <c r="U85">
         <v>7229</v>
       </c>
-      <c r="U85">
+      <c r="V85">
         <v>7592</v>
       </c>
-      <c r="V85" t="s">
-        <v>106</v>
-      </c>
-      <c r="W85">
+      <c r="W85" t="s">
+        <v>107</v>
+      </c>
+      <c r="X85">
         <v>363</v>
       </c>
-      <c r="X85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24">
+      <c r="Y85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -7092,22 +7368,25 @@
         <v>84</v>
       </c>
       <c r="T86">
+        <v>84</v>
+      </c>
+      <c r="U86">
         <v>7434</v>
       </c>
-      <c r="U86">
+      <c r="V86">
         <v>7799</v>
       </c>
-      <c r="V86" t="s">
-        <v>107</v>
-      </c>
-      <c r="W86">
+      <c r="W86" t="s">
+        <v>108</v>
+      </c>
+      <c r="X86">
         <v>365</v>
       </c>
-      <c r="X86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:24">
+      <c r="Y86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -7166,22 +7445,25 @@
         <v>85</v>
       </c>
       <c r="T87">
+        <v>85</v>
+      </c>
+      <c r="U87">
         <v>7548</v>
       </c>
-      <c r="U87">
+      <c r="V87">
         <v>7915</v>
       </c>
-      <c r="V87" t="s">
-        <v>108</v>
-      </c>
-      <c r="W87">
+      <c r="W87" t="s">
+        <v>109</v>
+      </c>
+      <c r="X87">
         <v>367</v>
       </c>
-      <c r="X87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24">
+      <c r="Y87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -7240,22 +7522,25 @@
         <v>86</v>
       </c>
       <c r="T88">
+        <v>86</v>
+      </c>
+      <c r="U88">
         <v>7725</v>
       </c>
-      <c r="U88">
+      <c r="V88">
         <v>8100</v>
       </c>
-      <c r="V88" t="s">
-        <v>109</v>
-      </c>
-      <c r="W88">
+      <c r="W88" t="s">
+        <v>110</v>
+      </c>
+      <c r="X88">
         <v>375</v>
       </c>
-      <c r="X88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24">
+      <c r="Y88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -7314,22 +7599,25 @@
         <v>87</v>
       </c>
       <c r="T89">
+        <v>87</v>
+      </c>
+      <c r="U89">
         <v>7937</v>
       </c>
-      <c r="U89">
+      <c r="V89">
         <v>8314</v>
       </c>
-      <c r="V89" t="s">
-        <v>110</v>
-      </c>
-      <c r="W89">
+      <c r="W89" t="s">
+        <v>111</v>
+      </c>
+      <c r="X89">
         <v>377</v>
       </c>
-      <c r="X89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24">
+      <c r="Y89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -7388,22 +7676,25 @@
         <v>88</v>
       </c>
       <c r="T90">
+        <v>88</v>
+      </c>
+      <c r="U90">
         <v>8179</v>
       </c>
-      <c r="U90">
+      <c r="V90">
         <v>8556</v>
       </c>
-      <c r="V90" t="s">
-        <v>111</v>
-      </c>
-      <c r="W90">
+      <c r="W90" t="s">
+        <v>112</v>
+      </c>
+      <c r="X90">
         <v>377</v>
       </c>
-      <c r="X90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:24">
+      <c r="Y90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -7443,23 +7734,26 @@
       <c r="M91">
         <v>89</v>
       </c>
-      <c r="T91">
+      <c r="N91">
+        <v>89</v>
+      </c>
+      <c r="U91">
         <v>8357</v>
       </c>
-      <c r="U91">
+      <c r="V91">
         <v>8735</v>
       </c>
-      <c r="V91" t="s">
-        <v>112</v>
-      </c>
-      <c r="W91">
+      <c r="W91" t="s">
+        <v>113</v>
+      </c>
+      <c r="X91">
         <v>378</v>
       </c>
-      <c r="X91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:24">
+      <c r="Y91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -7496,23 +7790,26 @@
       <c r="L92">
         <v>90</v>
       </c>
-      <c r="T92">
+      <c r="M92">
+        <v>90</v>
+      </c>
+      <c r="U92">
         <v>8436</v>
       </c>
-      <c r="U92">
+      <c r="V92">
         <v>8815</v>
       </c>
-      <c r="V92" t="s">
-        <v>113</v>
-      </c>
-      <c r="W92">
+      <c r="W92" t="s">
+        <v>114</v>
+      </c>
+      <c r="X92">
         <v>379</v>
       </c>
-      <c r="X92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24">
+      <c r="Y92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -7549,23 +7846,26 @@
       <c r="L93">
         <v>91</v>
       </c>
-      <c r="T93">
+      <c r="M93">
+        <v>91</v>
+      </c>
+      <c r="U93">
         <v>8777</v>
       </c>
-      <c r="U93">
+      <c r="V93">
         <v>9157</v>
       </c>
-      <c r="V93" t="s">
-        <v>114</v>
-      </c>
-      <c r="W93">
+      <c r="W93" t="s">
+        <v>115</v>
+      </c>
+      <c r="X93">
         <v>380</v>
       </c>
-      <c r="X93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:24">
+      <c r="Y93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -7599,23 +7899,26 @@
       <c r="K94">
         <v>92</v>
       </c>
-      <c r="T94">
+      <c r="L94">
+        <v>92</v>
+      </c>
+      <c r="U94">
         <v>8932</v>
       </c>
-      <c r="U94">
+      <c r="V94">
         <v>9318</v>
       </c>
-      <c r="V94" t="s">
-        <v>115</v>
-      </c>
-      <c r="W94">
+      <c r="W94" t="s">
+        <v>116</v>
+      </c>
+      <c r="X94">
         <v>386</v>
       </c>
-      <c r="X94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24">
+      <c r="Y94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -7646,23 +7949,26 @@
       <c r="J95">
         <v>93</v>
       </c>
-      <c r="T95">
+      <c r="K95">
+        <v>93</v>
+      </c>
+      <c r="U95">
         <v>9148</v>
       </c>
-      <c r="U95">
+      <c r="V95">
         <v>9535</v>
       </c>
-      <c r="V95" t="s">
-        <v>116</v>
-      </c>
-      <c r="W95">
+      <c r="W95" t="s">
+        <v>117</v>
+      </c>
+      <c r="X95">
         <v>387</v>
       </c>
-      <c r="X95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:24">
+      <c r="Y95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -7693,23 +7999,26 @@
       <c r="J96">
         <v>94</v>
       </c>
-      <c r="T96">
+      <c r="K96">
+        <v>94</v>
+      </c>
+      <c r="U96">
         <v>9462</v>
       </c>
-      <c r="U96">
+      <c r="V96">
         <v>9852</v>
       </c>
-      <c r="V96" t="s">
-        <v>117</v>
-      </c>
-      <c r="W96">
+      <c r="W96" t="s">
+        <v>118</v>
+      </c>
+      <c r="X96">
         <v>390</v>
       </c>
-      <c r="X96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:24">
+      <c r="Y96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -7740,23 +8049,26 @@
       <c r="J97">
         <v>95</v>
       </c>
-      <c r="T97">
+      <c r="K97">
+        <v>95</v>
+      </c>
+      <c r="U97">
         <v>9862</v>
       </c>
-      <c r="U97">
+      <c r="V97">
         <v>10259</v>
       </c>
-      <c r="V97" t="s">
-        <v>118</v>
-      </c>
-      <c r="W97">
+      <c r="W97" t="s">
+        <v>119</v>
+      </c>
+      <c r="X97">
         <v>397</v>
       </c>
-      <c r="X97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:24">
+      <c r="Y97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -7787,23 +8099,26 @@
       <c r="J98">
         <v>96</v>
       </c>
-      <c r="T98">
+      <c r="K98">
+        <v>96</v>
+      </c>
+      <c r="U98">
         <v>10088</v>
       </c>
-      <c r="U98">
+      <c r="V98">
         <v>10486</v>
       </c>
-      <c r="V98" t="s">
-        <v>119</v>
-      </c>
-      <c r="W98">
+      <c r="W98" t="s">
+        <v>120</v>
+      </c>
+      <c r="X98">
         <v>398</v>
       </c>
-      <c r="X98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:24">
+      <c r="Y98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -7819,23 +8134,26 @@
       <c r="E99">
         <v>97</v>
       </c>
-      <c r="T99">
+      <c r="F99">
+        <v>97</v>
+      </c>
+      <c r="U99">
         <v>10374</v>
       </c>
-      <c r="U99">
+      <c r="V99">
         <v>10774</v>
       </c>
-      <c r="V99" t="s">
-        <v>120</v>
-      </c>
-      <c r="W99">
+      <c r="W99" t="s">
+        <v>121</v>
+      </c>
+      <c r="X99">
         <v>400</v>
       </c>
-      <c r="X99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:24">
+      <c r="Y99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -7848,39 +8166,165 @@
       <c r="D100">
         <v>98</v>
       </c>
-      <c r="T100">
+      <c r="E100">
+        <v>98</v>
+      </c>
+      <c r="U100">
         <v>10374</v>
       </c>
-      <c r="U100">
+      <c r="V100">
         <v>10774</v>
       </c>
-      <c r="V100" t="s">
-        <v>121</v>
-      </c>
-      <c r="W100">
+      <c r="W100" t="s">
+        <v>122</v>
+      </c>
+      <c r="X100">
         <v>400</v>
       </c>
-      <c r="X100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:24">
+      <c r="Y100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="T101">
+      <c r="B101">
+        <v>99</v>
+      </c>
+      <c r="U101">
         <v>10374</v>
       </c>
-      <c r="U101">
+      <c r="V101">
         <v>10774</v>
       </c>
-      <c r="V101" t="s">
-        <v>122</v>
-      </c>
-      <c r="W101">
+      <c r="W101" t="s">
+        <v>123</v>
+      </c>
+      <c r="X101">
         <v>400</v>
       </c>
-      <c r="X101">
+      <c r="Y101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="U102">
+        <v>11473</v>
+      </c>
+      <c r="V102">
+        <v>11878</v>
+      </c>
+      <c r="W102" t="s">
+        <v>124</v>
+      </c>
+      <c r="X102">
+        <v>405</v>
+      </c>
+      <c r="Y102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="U103">
+        <v>11796</v>
+      </c>
+      <c r="V103">
+        <v>12204</v>
+      </c>
+      <c r="W103" t="s">
+        <v>125</v>
+      </c>
+      <c r="X103">
+        <v>408</v>
+      </c>
+      <c r="Y103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="U104">
+        <v>12764</v>
+      </c>
+      <c r="V104">
+        <v>13174</v>
+      </c>
+      <c r="W104" t="s">
+        <v>126</v>
+      </c>
+      <c r="X104">
+        <v>410</v>
+      </c>
+      <c r="Y104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="U105">
+        <v>13500</v>
+      </c>
+      <c r="V105">
+        <v>13910</v>
+      </c>
+      <c r="W105" t="s">
+        <v>127</v>
+      </c>
+      <c r="X105">
+        <v>410</v>
+      </c>
+      <c r="Y105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="U106">
+        <v>14193</v>
+      </c>
+      <c r="V106">
+        <v>14607</v>
+      </c>
+      <c r="W106" t="s">
+        <v>128</v>
+      </c>
+      <c r="X106">
+        <v>414</v>
+      </c>
+      <c r="Y106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:25">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="U107">
+        <v>14679</v>
+      </c>
+      <c r="V107">
+        <v>15095</v>
+      </c>
+      <c r="W107" t="s">
+        <v>129</v>
+      </c>
+      <c r="X107">
+        <v>416</v>
+      </c>
+      <c r="Y107">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add second plot to per capita page (without Westchester)
</commit_message>
<xml_diff>
--- a/Clark_Data.xlsx
+++ b/Clark_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Active</t>
@@ -761,13 +773,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y107"/>
+  <dimension ref="A1:AC107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:29">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,8 +852,20 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -906,19 +930,31 @@
         <v>0</v>
       </c>
       <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="AA2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -980,22 +1016,34 @@
         <v>1</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
-      <c r="W3" t="s">
-        <v>25</v>
+      <c r="W3">
+        <v>1</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:25">
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1057,22 +1105,34 @@
         <v>2</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
         <v>1</v>
       </c>
-      <c r="W4" t="s">
-        <v>26</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="AA4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1134,22 +1194,34 @@
         <v>3</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
         <v>2</v>
       </c>
-      <c r="W5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="AA5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1211,22 +1283,34 @@
         <v>4</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V6">
+        <v>4</v>
+      </c>
+      <c r="W6">
+        <v>4</v>
+      </c>
+      <c r="X6">
+        <v>4</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
         <v>2</v>
       </c>
-      <c r="W6" t="s">
-        <v>28</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="AA6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1288,22 +1372,34 @@
         <v>5</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V7">
+        <v>5</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>5</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
         <v>126</v>
       </c>
-      <c r="W7" t="s">
-        <v>29</v>
-      </c>
-      <c r="X7">
+      <c r="AA7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB7">
         <v>2</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1365,22 +1461,34 @@
         <v>6</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V8">
+        <v>6</v>
+      </c>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8">
+        <v>6</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
         <v>126</v>
       </c>
-      <c r="W8" t="s">
-        <v>30</v>
-      </c>
-      <c r="X8">
+      <c r="AA8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB8">
         <v>4</v>
       </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="AC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1442,22 +1550,34 @@
         <v>7</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="V9">
+        <v>7</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9">
+        <v>7</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
         <v>212</v>
       </c>
-      <c r="W9" t="s">
-        <v>31</v>
-      </c>
-      <c r="X9">
+      <c r="AA9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB9">
         <v>4</v>
       </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+      <c r="AC9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1519,22 +1639,34 @@
         <v>8</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V10">
+        <v>8</v>
+      </c>
+      <c r="W10">
+        <v>8</v>
+      </c>
+      <c r="X10">
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
         <v>249</v>
       </c>
-      <c r="W10" t="s">
-        <v>32</v>
-      </c>
-      <c r="X10">
+      <c r="AA10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10">
         <v>6</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+      <c r="AC10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1596,22 +1728,34 @@
         <v>9</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V11">
+        <v>9</v>
+      </c>
+      <c r="W11">
+        <v>9</v>
+      </c>
+      <c r="X11">
+        <v>9</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
         <v>350</v>
       </c>
-      <c r="W11" t="s">
-        <v>33</v>
-      </c>
-      <c r="X11">
+      <c r="AA11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB11">
         <v>6</v>
       </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="AC11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1673,13 +1817,13 @@
         <v>10</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V12">
-        <v>443</v>
-      </c>
-      <c r="W12" t="s">
-        <v>34</v>
+        <v>10</v>
+      </c>
+      <c r="W12">
+        <v>10</v>
       </c>
       <c r="X12">
         <v>10</v>
@@ -1687,8 +1831,20 @@
       <c r="Y12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:25">
+      <c r="Z12">
+        <v>443</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB12">
+        <v>10</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1750,22 +1906,34 @@
         <v>11</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="V13">
+        <v>11</v>
+      </c>
+      <c r="W13">
+        <v>11</v>
+      </c>
+      <c r="X13">
+        <v>11</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
         <v>443</v>
       </c>
-      <c r="W13" t="s">
-        <v>35</v>
-      </c>
-      <c r="X13">
+      <c r="AA13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB13">
         <v>10</v>
       </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="AC13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1827,22 +1995,34 @@
         <v>12</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="V14">
+        <v>12</v>
+      </c>
+      <c r="W14">
+        <v>12</v>
+      </c>
+      <c r="X14">
+        <v>12</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
         <v>528</v>
       </c>
-      <c r="W14" t="s">
-        <v>36</v>
-      </c>
-      <c r="X14">
+      <c r="AA14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB14">
         <v>14</v>
       </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="AC14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1904,22 +2084,34 @@
         <v>13</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="V15">
+        <v>13</v>
+      </c>
+      <c r="W15">
+        <v>13</v>
+      </c>
+      <c r="X15">
+        <v>13</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
         <v>753</v>
       </c>
-      <c r="W15" t="s">
-        <v>37</v>
-      </c>
-      <c r="X15">
+      <c r="AA15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB15">
         <v>14</v>
       </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="AC15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1981,22 +2173,34 @@
         <v>14</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="V16">
+        <v>14</v>
+      </c>
+      <c r="W16">
+        <v>14</v>
+      </c>
+      <c r="X16">
+        <v>14</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
         <v>869</v>
       </c>
-      <c r="W16" t="s">
-        <v>38</v>
-      </c>
-      <c r="X16">
+      <c r="AA16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB16">
         <v>23</v>
       </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="AC16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2058,22 +2262,34 @@
         <v>15</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V17">
+        <v>15</v>
+      </c>
+      <c r="W17">
+        <v>15</v>
+      </c>
+      <c r="X17">
+        <v>15</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
         <v>961</v>
       </c>
-      <c r="W17" t="s">
-        <v>39</v>
-      </c>
-      <c r="X17">
+      <c r="AA17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB17">
         <v>28</v>
       </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25">
+      <c r="AC17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2135,22 +2351,34 @@
         <v>16</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V18">
+        <v>16</v>
+      </c>
+      <c r="W18">
+        <v>16</v>
+      </c>
+      <c r="X18">
+        <v>16</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
         <v>1125</v>
       </c>
-      <c r="W18" t="s">
-        <v>40</v>
-      </c>
-      <c r="X18">
+      <c r="AA18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB18">
         <v>34</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25">
+      <c r="AC18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2212,22 +2440,34 @@
         <v>17</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="V19">
+        <v>17</v>
+      </c>
+      <c r="W19">
+        <v>17</v>
+      </c>
+      <c r="X19">
+        <v>17</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
         <v>1279</v>
       </c>
-      <c r="W19" t="s">
-        <v>41</v>
-      </c>
-      <c r="X19">
+      <c r="AA19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB19">
         <v>39</v>
       </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
+      <c r="AC19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2289,22 +2529,34 @@
         <v>18</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="V20">
+        <v>18</v>
+      </c>
+      <c r="W20">
+        <v>18</v>
+      </c>
+      <c r="X20">
+        <v>18</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
         <v>1418</v>
       </c>
-      <c r="W20" t="s">
-        <v>42</v>
-      </c>
-      <c r="X20">
+      <c r="AA20" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB20">
         <v>41</v>
       </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
+      <c r="AC20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2366,22 +2618,34 @@
         <v>19</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V21">
+        <v>19</v>
+      </c>
+      <c r="W21">
+        <v>19</v>
+      </c>
+      <c r="X21">
+        <v>19</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
         <v>1519</v>
       </c>
-      <c r="W21" t="s">
-        <v>43</v>
-      </c>
-      <c r="X21">
+      <c r="AA21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB21">
         <v>41</v>
       </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="AC21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2443,22 +2707,34 @@
         <v>20</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="V22">
+        <v>20</v>
+      </c>
+      <c r="W22">
+        <v>20</v>
+      </c>
+      <c r="X22">
+        <v>20</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
         <v>1608</v>
       </c>
-      <c r="W22" t="s">
-        <v>44</v>
-      </c>
-      <c r="X22">
+      <c r="AA22" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB22">
         <v>41</v>
       </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25">
+      <c r="AC22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2520,22 +2796,34 @@
         <v>21</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="V23">
+        <v>21</v>
+      </c>
+      <c r="W23">
+        <v>21</v>
+      </c>
+      <c r="X23">
+        <v>21</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
         <v>1734</v>
       </c>
-      <c r="W23" t="s">
-        <v>45</v>
-      </c>
-      <c r="X23">
+      <c r="AA23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB23">
         <v>54</v>
       </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
+      <c r="AC23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2597,22 +2885,34 @@
         <v>22</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="V24">
+        <v>22</v>
+      </c>
+      <c r="W24">
+        <v>22</v>
+      </c>
+      <c r="X24">
+        <v>22</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <v>1878</v>
       </c>
-      <c r="W24" t="s">
-        <v>46</v>
-      </c>
-      <c r="X24">
+      <c r="AA24" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB24">
         <v>65</v>
       </c>
-      <c r="Y24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="AC24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2674,22 +2974,34 @@
         <v>23</v>
       </c>
       <c r="U25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="V25">
+        <v>23</v>
+      </c>
+      <c r="W25">
+        <v>23</v>
+      </c>
+      <c r="X25">
+        <v>23</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <v>2009</v>
       </c>
-      <c r="W25" t="s">
-        <v>47</v>
-      </c>
-      <c r="X25">
+      <c r="AA25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB25">
         <v>71</v>
       </c>
-      <c r="Y25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
+      <c r="AC25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2751,22 +3063,34 @@
         <v>24</v>
       </c>
       <c r="U26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="V26">
+        <v>24</v>
+      </c>
+      <c r="W26">
+        <v>24</v>
+      </c>
+      <c r="X26">
+        <v>24</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
         <v>2144</v>
       </c>
-      <c r="W26" t="s">
-        <v>48</v>
-      </c>
-      <c r="X26">
+      <c r="AA26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB26">
         <v>75</v>
       </c>
-      <c r="Y26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
+      <c r="AC26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2828,22 +3152,34 @@
         <v>25</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="V27">
+        <v>25</v>
+      </c>
+      <c r="W27">
+        <v>25</v>
+      </c>
+      <c r="X27">
+        <v>25</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
         <v>2144</v>
       </c>
-      <c r="W27" t="s">
-        <v>49</v>
-      </c>
-      <c r="X27">
+      <c r="AA27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB27">
         <v>75</v>
       </c>
-      <c r="Y27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
+      <c r="AC27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2905,22 +3241,34 @@
         <v>26</v>
       </c>
       <c r="U28">
+        <v>26</v>
+      </c>
+      <c r="V28">
+        <v>26</v>
+      </c>
+      <c r="W28">
+        <v>26</v>
+      </c>
+      <c r="X28">
+        <v>26</v>
+      </c>
+      <c r="Y28">
         <v>2224</v>
       </c>
-      <c r="V28">
+      <c r="Z28">
         <v>2324</v>
       </c>
-      <c r="W28" t="s">
-        <v>50</v>
-      </c>
-      <c r="X28">
+      <c r="AA28" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB28">
         <v>100</v>
       </c>
-      <c r="Y28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
+      <c r="AC28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2982,22 +3330,34 @@
         <v>27</v>
       </c>
       <c r="U29">
+        <v>27</v>
+      </c>
+      <c r="V29">
+        <v>27</v>
+      </c>
+      <c r="W29">
+        <v>27</v>
+      </c>
+      <c r="X29">
+        <v>27</v>
+      </c>
+      <c r="Y29">
         <v>2343</v>
       </c>
-      <c r="V29">
+      <c r="Z29">
         <v>2444</v>
       </c>
-      <c r="W29" t="s">
-        <v>51</v>
-      </c>
-      <c r="X29">
+      <c r="AA29" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB29">
         <v>101</v>
       </c>
-      <c r="Y29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
+      <c r="AC29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3059,22 +3419,34 @@
         <v>28</v>
       </c>
       <c r="U30">
+        <v>28</v>
+      </c>
+      <c r="V30">
+        <v>28</v>
+      </c>
+      <c r="W30">
+        <v>28</v>
+      </c>
+      <c r="X30">
+        <v>28</v>
+      </c>
+      <c r="Y30">
         <v>2403</v>
       </c>
-      <c r="V30">
+      <c r="Z30">
         <v>2509</v>
       </c>
-      <c r="W30" t="s">
-        <v>52</v>
-      </c>
-      <c r="X30">
+      <c r="AA30" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB30">
         <v>106</v>
       </c>
-      <c r="Y30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
+      <c r="AC30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3136,22 +3508,34 @@
         <v>29</v>
       </c>
       <c r="U31">
+        <v>29</v>
+      </c>
+      <c r="V31">
+        <v>29</v>
+      </c>
+      <c r="W31">
+        <v>29</v>
+      </c>
+      <c r="X31">
+        <v>29</v>
+      </c>
+      <c r="Y31">
         <v>2444</v>
       </c>
-      <c r="V31">
+      <c r="Z31">
         <v>2559</v>
       </c>
-      <c r="W31" t="s">
-        <v>53</v>
-      </c>
-      <c r="X31">
+      <c r="AA31" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB31">
         <v>115</v>
       </c>
-      <c r="Y31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="AC31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3213,22 +3597,34 @@
         <v>30</v>
       </c>
       <c r="U32">
+        <v>30</v>
+      </c>
+      <c r="V32">
+        <v>30</v>
+      </c>
+      <c r="W32">
+        <v>30</v>
+      </c>
+      <c r="X32">
+        <v>30</v>
+      </c>
+      <c r="Y32">
         <v>2444</v>
       </c>
-      <c r="V32">
+      <c r="Z32">
         <v>2559</v>
       </c>
-      <c r="W32" t="s">
-        <v>54</v>
-      </c>
-      <c r="X32">
+      <c r="AA32" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB32">
         <v>115</v>
       </c>
-      <c r="Y32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25">
+      <c r="AC32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3290,22 +3686,34 @@
         <v>31</v>
       </c>
       <c r="U33">
+        <v>31</v>
+      </c>
+      <c r="V33">
+        <v>31</v>
+      </c>
+      <c r="W33">
+        <v>31</v>
+      </c>
+      <c r="X33">
+        <v>31</v>
+      </c>
+      <c r="Y33">
         <v>2614</v>
       </c>
-      <c r="V33">
+      <c r="Z33">
         <v>2738</v>
       </c>
-      <c r="W33" t="s">
-        <v>55</v>
-      </c>
-      <c r="X33">
+      <c r="AA33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB33">
         <v>124</v>
       </c>
-      <c r="Y33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="AC33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3367,22 +3775,34 @@
         <v>32</v>
       </c>
       <c r="U34">
+        <v>32</v>
+      </c>
+      <c r="V34">
+        <v>32</v>
+      </c>
+      <c r="W34">
+        <v>32</v>
+      </c>
+      <c r="X34">
+        <v>32</v>
+      </c>
+      <c r="Y34">
         <v>2749</v>
       </c>
-      <c r="V34">
+      <c r="Z34">
         <v>2882</v>
       </c>
-      <c r="W34" t="s">
-        <v>56</v>
-      </c>
-      <c r="X34">
+      <c r="AA34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB34">
         <v>133</v>
       </c>
-      <c r="Y34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25">
+      <c r="AC34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3444,22 +3864,34 @@
         <v>33</v>
       </c>
       <c r="U35">
+        <v>33</v>
+      </c>
+      <c r="V35">
+        <v>33</v>
+      </c>
+      <c r="W35">
+        <v>33</v>
+      </c>
+      <c r="X35">
+        <v>33</v>
+      </c>
+      <c r="Y35">
         <v>2803</v>
       </c>
-      <c r="V35">
+      <c r="Z35">
         <v>2940</v>
       </c>
-      <c r="W35" t="s">
-        <v>57</v>
-      </c>
-      <c r="X35">
+      <c r="AA35" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB35">
         <v>137</v>
       </c>
-      <c r="Y35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25">
+      <c r="AC35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3521,22 +3953,34 @@
         <v>34</v>
       </c>
       <c r="U36">
+        <v>34</v>
+      </c>
+      <c r="V36">
+        <v>34</v>
+      </c>
+      <c r="W36">
+        <v>34</v>
+      </c>
+      <c r="X36">
+        <v>34</v>
+      </c>
+      <c r="Y36">
         <v>2861</v>
       </c>
-      <c r="V36">
+      <c r="Z36">
         <v>2998</v>
       </c>
-      <c r="W36" t="s">
-        <v>58</v>
-      </c>
-      <c r="X36">
+      <c r="AA36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB36">
         <v>137</v>
       </c>
-      <c r="Y36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25">
+      <c r="AC36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3598,22 +4042,34 @@
         <v>35</v>
       </c>
       <c r="U37">
+        <v>35</v>
+      </c>
+      <c r="V37">
+        <v>35</v>
+      </c>
+      <c r="W37">
+        <v>35</v>
+      </c>
+      <c r="X37">
+        <v>35</v>
+      </c>
+      <c r="Y37">
         <v>2958</v>
       </c>
-      <c r="V37">
+      <c r="Z37">
         <v>3099</v>
       </c>
-      <c r="W37" t="s">
-        <v>59</v>
-      </c>
-      <c r="X37">
+      <c r="AA37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB37">
         <v>141</v>
       </c>
-      <c r="Y37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25">
+      <c r="AC37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3675,22 +4131,34 @@
         <v>36</v>
       </c>
       <c r="U38">
+        <v>36</v>
+      </c>
+      <c r="V38">
+        <v>36</v>
+      </c>
+      <c r="W38">
+        <v>36</v>
+      </c>
+      <c r="X38">
+        <v>36</v>
+      </c>
+      <c r="Y38">
         <v>3068</v>
       </c>
-      <c r="V38">
+      <c r="Z38">
         <v>3218</v>
       </c>
-      <c r="W38" t="s">
-        <v>60</v>
-      </c>
-      <c r="X38">
+      <c r="AA38" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB38">
         <v>150</v>
       </c>
-      <c r="Y38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25">
+      <c r="AC38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3752,22 +4220,34 @@
         <v>37</v>
       </c>
       <c r="U39">
+        <v>37</v>
+      </c>
+      <c r="V39">
+        <v>37</v>
+      </c>
+      <c r="W39">
+        <v>37</v>
+      </c>
+      <c r="X39">
+        <v>37</v>
+      </c>
+      <c r="Y39">
         <v>3151</v>
       </c>
-      <c r="V39">
+      <c r="Z39">
         <v>3314</v>
       </c>
-      <c r="W39" t="s">
-        <v>61</v>
-      </c>
-      <c r="X39">
+      <c r="AA39" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB39">
         <v>163</v>
       </c>
-      <c r="Y39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25">
+      <c r="AC39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3829,22 +4309,34 @@
         <v>38</v>
       </c>
       <c r="U40">
+        <v>38</v>
+      </c>
+      <c r="V40">
+        <v>38</v>
+      </c>
+      <c r="W40">
+        <v>38</v>
+      </c>
+      <c r="X40">
+        <v>38</v>
+      </c>
+      <c r="Y40">
         <v>3275</v>
       </c>
-      <c r="V40">
+      <c r="Z40">
         <v>3443</v>
       </c>
-      <c r="W40" t="s">
-        <v>62</v>
-      </c>
-      <c r="X40">
+      <c r="AA40" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB40">
         <v>168</v>
       </c>
-      <c r="Y40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25">
+      <c r="AC40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3906,22 +4398,34 @@
         <v>39</v>
       </c>
       <c r="U41">
+        <v>39</v>
+      </c>
+      <c r="V41">
+        <v>39</v>
+      </c>
+      <c r="W41">
+        <v>39</v>
+      </c>
+      <c r="X41">
+        <v>39</v>
+      </c>
+      <c r="Y41">
         <v>3396</v>
       </c>
-      <c r="V41">
+      <c r="Z41">
         <v>3570</v>
       </c>
-      <c r="W41" t="s">
-        <v>63</v>
-      </c>
-      <c r="X41">
+      <c r="AA41" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB41">
         <v>174</v>
       </c>
-      <c r="Y41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25">
+      <c r="AC41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3983,22 +4487,34 @@
         <v>40</v>
       </c>
       <c r="U42">
+        <v>40</v>
+      </c>
+      <c r="V42">
+        <v>40</v>
+      </c>
+      <c r="W42">
+        <v>40</v>
+      </c>
+      <c r="X42">
+        <v>40</v>
+      </c>
+      <c r="Y42">
         <v>3491</v>
       </c>
-      <c r="V42">
+      <c r="Z42">
         <v>3665</v>
       </c>
-      <c r="W42" t="s">
-        <v>64</v>
-      </c>
-      <c r="X42">
+      <c r="AA42" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB42">
         <v>174</v>
       </c>
-      <c r="Y42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25">
+      <c r="AC42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4060,22 +4576,34 @@
         <v>41</v>
       </c>
       <c r="U43">
+        <v>41</v>
+      </c>
+      <c r="V43">
+        <v>41</v>
+      </c>
+      <c r="W43">
+        <v>41</v>
+      </c>
+      <c r="X43">
+        <v>41</v>
+      </c>
+      <c r="Y43">
         <v>3543</v>
       </c>
-      <c r="V43">
+      <c r="Z43">
         <v>3717</v>
       </c>
-      <c r="W43" t="s">
-        <v>65</v>
-      </c>
-      <c r="X43">
+      <c r="AA43" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB43">
         <v>174</v>
       </c>
-      <c r="Y43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25">
+      <c r="AC43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4137,22 +4665,34 @@
         <v>42</v>
       </c>
       <c r="U44">
+        <v>42</v>
+      </c>
+      <c r="V44">
+        <v>42</v>
+      </c>
+      <c r="W44">
+        <v>42</v>
+      </c>
+      <c r="X44">
+        <v>42</v>
+      </c>
+      <c r="Y44">
         <v>3607</v>
       </c>
-      <c r="V44">
+      <c r="Z44">
         <v>3793</v>
       </c>
-      <c r="W44" t="s">
-        <v>66</v>
-      </c>
-      <c r="X44">
+      <c r="AA44" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB44">
         <v>186</v>
       </c>
-      <c r="Y44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25">
+      <c r="AC44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4214,22 +4754,34 @@
         <v>43</v>
       </c>
       <c r="U45">
+        <v>43</v>
+      </c>
+      <c r="V45">
+        <v>43</v>
+      </c>
+      <c r="W45">
+        <v>43</v>
+      </c>
+      <c r="X45">
+        <v>43</v>
+      </c>
+      <c r="Y45">
         <v>3695</v>
       </c>
-      <c r="V45">
+      <c r="Z45">
         <v>3891</v>
       </c>
-      <c r="W45" t="s">
-        <v>67</v>
-      </c>
-      <c r="X45">
+      <c r="AA45" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB45">
         <v>196</v>
       </c>
-      <c r="Y45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25">
+      <c r="AC45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4291,22 +4843,34 @@
         <v>44</v>
       </c>
       <c r="U46">
+        <v>44</v>
+      </c>
+      <c r="V46">
+        <v>44</v>
+      </c>
+      <c r="W46">
+        <v>44</v>
+      </c>
+      <c r="X46">
+        <v>44</v>
+      </c>
+      <c r="Y46">
         <v>3777</v>
       </c>
-      <c r="V46">
+      <c r="Z46">
         <v>3979</v>
       </c>
-      <c r="W46" t="s">
-        <v>68</v>
-      </c>
-      <c r="X46">
+      <c r="AA46" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB46">
         <v>202</v>
       </c>
-      <c r="Y46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25">
+      <c r="AC46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4368,22 +4932,34 @@
         <v>45</v>
       </c>
       <c r="U47">
+        <v>45</v>
+      </c>
+      <c r="V47">
+        <v>45</v>
+      </c>
+      <c r="W47">
+        <v>45</v>
+      </c>
+      <c r="X47">
+        <v>45</v>
+      </c>
+      <c r="Y47">
         <v>3912</v>
       </c>
-      <c r="V47">
+      <c r="Z47">
         <v>4118</v>
       </c>
-      <c r="W47" t="s">
-        <v>69</v>
-      </c>
-      <c r="X47">
+      <c r="AA47" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB47">
         <v>206</v>
       </c>
-      <c r="Y47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25">
+      <c r="AC47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4445,22 +5021,34 @@
         <v>46</v>
       </c>
       <c r="U48">
+        <v>46</v>
+      </c>
+      <c r="V48">
+        <v>46</v>
+      </c>
+      <c r="W48">
+        <v>46</v>
+      </c>
+      <c r="X48">
+        <v>46</v>
+      </c>
+      <c r="Y48">
         <v>4010</v>
       </c>
-      <c r="V48">
+      <c r="Z48">
         <v>4225</v>
       </c>
-      <c r="W48" t="s">
-        <v>70</v>
-      </c>
-      <c r="X48">
+      <c r="AA48" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB48">
         <v>215</v>
       </c>
-      <c r="Y48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25">
+      <c r="AC48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4522,22 +5110,34 @@
         <v>47</v>
       </c>
       <c r="U49">
+        <v>47</v>
+      </c>
+      <c r="V49">
+        <v>47</v>
+      </c>
+      <c r="W49">
+        <v>47</v>
+      </c>
+      <c r="X49">
+        <v>47</v>
+      </c>
+      <c r="Y49">
         <v>4056</v>
       </c>
-      <c r="V49">
+      <c r="Z49">
         <v>4274</v>
       </c>
-      <c r="W49" t="s">
-        <v>71</v>
-      </c>
-      <c r="X49">
+      <c r="AA49" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB49">
         <v>218</v>
       </c>
-      <c r="Y49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25">
+      <c r="AC49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4599,22 +5199,34 @@
         <v>48</v>
       </c>
       <c r="U50">
+        <v>48</v>
+      </c>
+      <c r="V50">
+        <v>48</v>
+      </c>
+      <c r="W50">
+        <v>48</v>
+      </c>
+      <c r="X50">
+        <v>48</v>
+      </c>
+      <c r="Y50">
         <v>4188</v>
       </c>
-      <c r="V50">
+      <c r="Z50">
         <v>4411</v>
       </c>
-      <c r="W50" t="s">
-        <v>72</v>
-      </c>
-      <c r="X50">
+      <c r="AA50" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB50">
         <v>223</v>
       </c>
-      <c r="Y50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25">
+      <c r="AC50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4676,22 +5288,34 @@
         <v>49</v>
       </c>
       <c r="U51">
+        <v>49</v>
+      </c>
+      <c r="V51">
+        <v>49</v>
+      </c>
+      <c r="W51">
+        <v>49</v>
+      </c>
+      <c r="X51">
+        <v>49</v>
+      </c>
+      <c r="Y51">
         <v>4182</v>
       </c>
-      <c r="V51">
+      <c r="Z51">
         <v>4408</v>
       </c>
-      <c r="W51" t="s">
-        <v>73</v>
-      </c>
-      <c r="X51">
+      <c r="AA51" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB51">
         <v>226</v>
       </c>
-      <c r="Y51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25">
+      <c r="AC51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4753,22 +5377,34 @@
         <v>50</v>
       </c>
       <c r="U52">
+        <v>50</v>
+      </c>
+      <c r="V52">
+        <v>50</v>
+      </c>
+      <c r="W52">
+        <v>50</v>
+      </c>
+      <c r="X52">
+        <v>50</v>
+      </c>
+      <c r="Y52">
         <v>4235</v>
       </c>
-      <c r="V52">
+      <c r="Z52">
         <v>4473</v>
       </c>
-      <c r="W52" t="s">
-        <v>74</v>
-      </c>
-      <c r="X52">
+      <c r="AA52" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB52">
         <v>238</v>
       </c>
-      <c r="Y52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25">
+      <c r="AC52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4830,22 +5466,34 @@
         <v>51</v>
       </c>
       <c r="U53">
+        <v>51</v>
+      </c>
+      <c r="V53">
+        <v>51</v>
+      </c>
+      <c r="W53">
+        <v>51</v>
+      </c>
+      <c r="X53">
+        <v>51</v>
+      </c>
+      <c r="Y53">
         <v>4328</v>
       </c>
-      <c r="V53">
+      <c r="Z53">
         <v>4573</v>
       </c>
-      <c r="W53" t="s">
-        <v>75</v>
-      </c>
-      <c r="X53">
+      <c r="AA53" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB53">
         <v>245</v>
       </c>
-      <c r="Y53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25">
+      <c r="AC53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4907,22 +5555,34 @@
         <v>52</v>
       </c>
       <c r="U54">
+        <v>52</v>
+      </c>
+      <c r="V54">
+        <v>52</v>
+      </c>
+      <c r="W54">
+        <v>52</v>
+      </c>
+      <c r="X54">
+        <v>52</v>
+      </c>
+      <c r="Y54">
         <v>4328</v>
       </c>
-      <c r="V54">
+      <c r="Z54">
         <v>4573</v>
       </c>
-      <c r="W54" t="s">
-        <v>76</v>
-      </c>
-      <c r="X54">
+      <c r="AA54" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB54">
         <v>245</v>
       </c>
-      <c r="Y54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25">
+      <c r="AC54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4984,22 +5644,34 @@
         <v>53</v>
       </c>
       <c r="U55">
+        <v>53</v>
+      </c>
+      <c r="V55">
+        <v>53</v>
+      </c>
+      <c r="W55">
+        <v>53</v>
+      </c>
+      <c r="X55">
+        <v>53</v>
+      </c>
+      <c r="Y55">
         <v>4448</v>
       </c>
-      <c r="V55">
+      <c r="Z55">
         <v>4704</v>
       </c>
-      <c r="W55" t="s">
-        <v>77</v>
-      </c>
-      <c r="X55">
+      <c r="AA55" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB55">
         <v>256</v>
       </c>
-      <c r="Y55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25">
+      <c r="AC55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -5061,22 +5733,34 @@
         <v>54</v>
       </c>
       <c r="U56">
+        <v>54</v>
+      </c>
+      <c r="V56">
+        <v>54</v>
+      </c>
+      <c r="W56">
+        <v>54</v>
+      </c>
+      <c r="X56">
+        <v>54</v>
+      </c>
+      <c r="Y56">
         <v>4490</v>
       </c>
-      <c r="V56">
+      <c r="Z56">
         <v>4750</v>
       </c>
-      <c r="W56" t="s">
-        <v>78</v>
-      </c>
-      <c r="X56">
+      <c r="AA56" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB56">
         <v>260</v>
       </c>
-      <c r="Y56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25">
+      <c r="AC56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -5138,22 +5822,34 @@
         <v>55</v>
       </c>
       <c r="U57">
+        <v>55</v>
+      </c>
+      <c r="V57">
+        <v>55</v>
+      </c>
+      <c r="W57">
+        <v>55</v>
+      </c>
+      <c r="X57">
+        <v>55</v>
+      </c>
+      <c r="Y57">
         <v>4502</v>
       </c>
-      <c r="V57">
+      <c r="Z57">
         <v>4762</v>
       </c>
-      <c r="W57" t="s">
-        <v>79</v>
-      </c>
-      <c r="X57">
+      <c r="AA57" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB57">
         <v>260</v>
       </c>
-      <c r="Y57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25">
+      <c r="AC57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5215,22 +5911,34 @@
         <v>56</v>
       </c>
       <c r="U58">
+        <v>56</v>
+      </c>
+      <c r="V58">
+        <v>56</v>
+      </c>
+      <c r="W58">
+        <v>56</v>
+      </c>
+      <c r="X58">
+        <v>56</v>
+      </c>
+      <c r="Y58">
         <v>4602</v>
       </c>
-      <c r="V58">
+      <c r="Z58">
         <v>4869</v>
       </c>
-      <c r="W58" t="s">
-        <v>80</v>
-      </c>
-      <c r="X58">
+      <c r="AA58" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB58">
         <v>267</v>
       </c>
-      <c r="Y58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25">
+      <c r="AC58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5292,22 +6000,34 @@
         <v>57</v>
       </c>
       <c r="U59">
+        <v>57</v>
+      </c>
+      <c r="V59">
+        <v>57</v>
+      </c>
+      <c r="W59">
+        <v>57</v>
+      </c>
+      <c r="X59">
+        <v>57</v>
+      </c>
+      <c r="Y59">
         <v>4770</v>
       </c>
-      <c r="V59">
+      <c r="Z59">
         <v>5045</v>
       </c>
-      <c r="W59" t="s">
-        <v>81</v>
-      </c>
-      <c r="X59">
+      <c r="AA59" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB59">
         <v>275</v>
       </c>
-      <c r="Y59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25">
+      <c r="AC59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5369,22 +6089,34 @@
         <v>58</v>
       </c>
       <c r="U60">
+        <v>58</v>
+      </c>
+      <c r="V60">
+        <v>58</v>
+      </c>
+      <c r="W60">
+        <v>58</v>
+      </c>
+      <c r="X60">
+        <v>58</v>
+      </c>
+      <c r="Y60">
         <v>4770</v>
       </c>
-      <c r="V60">
+      <c r="Z60">
         <v>5045</v>
       </c>
-      <c r="W60" t="s">
-        <v>82</v>
-      </c>
-      <c r="X60">
+      <c r="AA60" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB60">
         <v>275</v>
       </c>
-      <c r="Y60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25">
+      <c r="AC60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5446,22 +6178,34 @@
         <v>59</v>
       </c>
       <c r="U61">
+        <v>59</v>
+      </c>
+      <c r="V61">
+        <v>59</v>
+      </c>
+      <c r="W61">
+        <v>59</v>
+      </c>
+      <c r="X61">
+        <v>59</v>
+      </c>
+      <c r="Y61">
         <v>4944</v>
       </c>
-      <c r="V61">
+      <c r="Z61">
         <v>5235</v>
       </c>
-      <c r="W61" t="s">
-        <v>83</v>
-      </c>
-      <c r="X61">
+      <c r="AA61" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB61">
         <v>291</v>
       </c>
-      <c r="Y61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25">
+      <c r="AC61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5523,22 +6267,34 @@
         <v>60</v>
       </c>
       <c r="U62">
+        <v>60</v>
+      </c>
+      <c r="V62">
+        <v>60</v>
+      </c>
+      <c r="W62">
+        <v>60</v>
+      </c>
+      <c r="X62">
+        <v>60</v>
+      </c>
+      <c r="Y62">
         <v>5005</v>
       </c>
-      <c r="V62">
+      <c r="Z62">
         <v>5298</v>
       </c>
-      <c r="W62" t="s">
-        <v>84</v>
-      </c>
-      <c r="X62">
+      <c r="AA62" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB62">
         <v>293</v>
       </c>
-      <c r="Y62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25">
+      <c r="AC62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5600,22 +6356,34 @@
         <v>61</v>
       </c>
       <c r="U63">
+        <v>61</v>
+      </c>
+      <c r="V63">
+        <v>61</v>
+      </c>
+      <c r="W63">
+        <v>61</v>
+      </c>
+      <c r="X63">
+        <v>61</v>
+      </c>
+      <c r="Y63">
         <v>5070</v>
       </c>
-      <c r="V63">
+      <c r="Z63">
         <v>5366</v>
       </c>
-      <c r="W63" t="s">
-        <v>85</v>
-      </c>
-      <c r="X63">
+      <c r="AA63" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB63">
         <v>296</v>
       </c>
-      <c r="Y63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25">
+      <c r="AC63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5677,22 +6445,34 @@
         <v>62</v>
       </c>
       <c r="U64">
+        <v>62</v>
+      </c>
+      <c r="V64">
+        <v>62</v>
+      </c>
+      <c r="W64">
+        <v>62</v>
+      </c>
+      <c r="X64">
+        <v>62</v>
+      </c>
+      <c r="Y64">
         <v>5167</v>
       </c>
-      <c r="V64">
+      <c r="Z64">
         <v>5463</v>
       </c>
-      <c r="W64" t="s">
-        <v>86</v>
-      </c>
-      <c r="X64">
+      <c r="AA64" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB64">
         <v>296</v>
       </c>
-      <c r="Y64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:25">
+      <c r="AC64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5754,22 +6534,34 @@
         <v>63</v>
       </c>
       <c r="U65">
+        <v>63</v>
+      </c>
+      <c r="V65">
+        <v>63</v>
+      </c>
+      <c r="W65">
+        <v>63</v>
+      </c>
+      <c r="X65">
+        <v>63</v>
+      </c>
+      <c r="Y65">
         <v>5167</v>
       </c>
-      <c r="V65">
+      <c r="Z65">
         <v>5463</v>
       </c>
-      <c r="W65" t="s">
-        <v>87</v>
-      </c>
-      <c r="X65">
+      <c r="AA65" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB65">
         <v>296</v>
       </c>
-      <c r="Y65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:25">
+      <c r="AC65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5831,22 +6623,34 @@
         <v>64</v>
       </c>
       <c r="U66">
+        <v>64</v>
+      </c>
+      <c r="V66">
+        <v>64</v>
+      </c>
+      <c r="W66">
+        <v>64</v>
+      </c>
+      <c r="X66">
+        <v>64</v>
+      </c>
+      <c r="Y66">
         <v>5336</v>
       </c>
-      <c r="V66">
+      <c r="Z66">
         <v>5650</v>
       </c>
-      <c r="W66" t="s">
-        <v>88</v>
-      </c>
-      <c r="X66">
+      <c r="AA66" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB66">
         <v>314</v>
       </c>
-      <c r="Y66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:25">
+      <c r="AC66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5908,22 +6712,34 @@
         <v>65</v>
       </c>
       <c r="U67">
+        <v>65</v>
+      </c>
+      <c r="V67">
+        <v>65</v>
+      </c>
+      <c r="W67">
+        <v>65</v>
+      </c>
+      <c r="X67">
+        <v>65</v>
+      </c>
+      <c r="Y67">
         <v>5414</v>
       </c>
-      <c r="V67">
+      <c r="Z67">
         <v>5734</v>
       </c>
-      <c r="W67" t="s">
-        <v>89</v>
-      </c>
-      <c r="X67">
+      <c r="AA67" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB67">
         <v>320</v>
       </c>
-      <c r="Y67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:25">
+      <c r="AC67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5985,22 +6801,34 @@
         <v>66</v>
       </c>
       <c r="U68">
+        <v>66</v>
+      </c>
+      <c r="V68">
+        <v>66</v>
+      </c>
+      <c r="W68">
+        <v>66</v>
+      </c>
+      <c r="X68">
+        <v>66</v>
+      </c>
+      <c r="Y68">
         <v>5493</v>
       </c>
-      <c r="V68">
+      <c r="Z68">
         <v>5815</v>
       </c>
-      <c r="W68" t="s">
-        <v>90</v>
-      </c>
-      <c r="X68">
+      <c r="AA68" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB68">
         <v>322</v>
       </c>
-      <c r="Y68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:25">
+      <c r="AC68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -6062,22 +6890,34 @@
         <v>67</v>
       </c>
       <c r="U69">
+        <v>67</v>
+      </c>
+      <c r="V69">
+        <v>67</v>
+      </c>
+      <c r="W69">
+        <v>67</v>
+      </c>
+      <c r="X69">
+        <v>67</v>
+      </c>
+      <c r="Y69">
         <v>5493</v>
       </c>
-      <c r="V69">
+      <c r="Z69">
         <v>5815</v>
       </c>
-      <c r="W69" t="s">
-        <v>91</v>
-      </c>
-      <c r="X69">
+      <c r="AA69" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB69">
         <v>322</v>
       </c>
-      <c r="Y69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:25">
+      <c r="AC69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -6139,22 +6979,34 @@
         <v>68</v>
       </c>
       <c r="U70">
+        <v>68</v>
+      </c>
+      <c r="V70">
+        <v>68</v>
+      </c>
+      <c r="W70">
+        <v>68</v>
+      </c>
+      <c r="X70">
+        <v>68</v>
+      </c>
+      <c r="Y70">
         <v>5818</v>
       </c>
-      <c r="V70">
+      <c r="Z70">
         <v>6140</v>
       </c>
-      <c r="W70" t="s">
-        <v>92</v>
-      </c>
-      <c r="X70">
+      <c r="AA70" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB70">
         <v>322</v>
       </c>
-      <c r="Y70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:25">
+      <c r="AC70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -6216,22 +7068,34 @@
         <v>69</v>
       </c>
       <c r="U71">
+        <v>69</v>
+      </c>
+      <c r="V71">
+        <v>69</v>
+      </c>
+      <c r="W71">
+        <v>69</v>
+      </c>
+      <c r="X71">
+        <v>69</v>
+      </c>
+      <c r="Y71">
         <v>5853</v>
       </c>
-      <c r="V71">
+      <c r="Z71">
         <v>6182</v>
       </c>
-      <c r="W71" t="s">
-        <v>93</v>
-      </c>
-      <c r="X71">
+      <c r="AA71" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB71">
         <v>329</v>
       </c>
-      <c r="Y71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:25">
+      <c r="AC71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -6293,22 +7157,34 @@
         <v>70</v>
       </c>
       <c r="U72">
+        <v>70</v>
+      </c>
+      <c r="V72">
+        <v>70</v>
+      </c>
+      <c r="W72">
+        <v>70</v>
+      </c>
+      <c r="X72">
+        <v>70</v>
+      </c>
+      <c r="Y72">
         <v>5897</v>
       </c>
-      <c r="V72">
+      <c r="Z72">
         <v>6226</v>
       </c>
-      <c r="W72" t="s">
-        <v>94</v>
-      </c>
-      <c r="X72">
+      <c r="AA72" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB72">
         <v>329</v>
       </c>
-      <c r="Y72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:25">
+      <c r="AC72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -6370,22 +7246,34 @@
         <v>71</v>
       </c>
       <c r="U73">
+        <v>71</v>
+      </c>
+      <c r="V73">
+        <v>71</v>
+      </c>
+      <c r="W73">
+        <v>71</v>
+      </c>
+      <c r="X73">
+        <v>71</v>
+      </c>
+      <c r="Y73">
         <v>5956</v>
       </c>
-      <c r="V73">
+      <c r="Z73">
         <v>6287</v>
       </c>
-      <c r="W73" t="s">
-        <v>95</v>
-      </c>
-      <c r="X73">
+      <c r="AA73" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB73">
         <v>331</v>
       </c>
-      <c r="Y73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:25">
+      <c r="AC73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -6447,22 +7335,34 @@
         <v>72</v>
       </c>
       <c r="U74">
+        <v>72</v>
+      </c>
+      <c r="V74">
+        <v>72</v>
+      </c>
+      <c r="W74">
+        <v>72</v>
+      </c>
+      <c r="X74">
+        <v>72</v>
+      </c>
+      <c r="Y74">
         <v>6013</v>
       </c>
-      <c r="V74">
+      <c r="Z74">
         <v>6352</v>
       </c>
-      <c r="W74" t="s">
-        <v>96</v>
-      </c>
-      <c r="X74">
+      <c r="AA74" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB74">
         <v>339</v>
       </c>
-      <c r="Y74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:25">
+      <c r="AC74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:29">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -6524,22 +7424,34 @@
         <v>73</v>
       </c>
       <c r="U75">
+        <v>73</v>
+      </c>
+      <c r="V75">
+        <v>73</v>
+      </c>
+      <c r="W75">
+        <v>73</v>
+      </c>
+      <c r="X75">
+        <v>73</v>
+      </c>
+      <c r="Y75">
         <v>6118</v>
       </c>
-      <c r="V75">
+      <c r="Z75">
         <v>6457</v>
       </c>
-      <c r="W75" t="s">
-        <v>97</v>
-      </c>
-      <c r="X75">
+      <c r="AA75" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB75">
         <v>339</v>
       </c>
-      <c r="Y75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:25">
+      <c r="AC75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -6601,22 +7513,34 @@
         <v>74</v>
       </c>
       <c r="U76">
+        <v>74</v>
+      </c>
+      <c r="V76">
+        <v>74</v>
+      </c>
+      <c r="W76">
+        <v>74</v>
+      </c>
+      <c r="X76">
+        <v>74</v>
+      </c>
+      <c r="Y76">
         <v>6236</v>
       </c>
-      <c r="V76">
+      <c r="Z76">
         <v>6579</v>
       </c>
-      <c r="W76" t="s">
-        <v>98</v>
-      </c>
-      <c r="X76">
+      <c r="AA76" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB76">
         <v>343</v>
       </c>
-      <c r="Y76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:25">
+      <c r="AC76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -6678,22 +7602,34 @@
         <v>75</v>
       </c>
       <c r="U77">
+        <v>75</v>
+      </c>
+      <c r="V77">
+        <v>75</v>
+      </c>
+      <c r="W77">
+        <v>75</v>
+      </c>
+      <c r="X77">
+        <v>75</v>
+      </c>
+      <c r="Y77">
         <v>6314</v>
       </c>
-      <c r="V77">
+      <c r="Z77">
         <v>6657</v>
       </c>
-      <c r="W77" t="s">
-        <v>99</v>
-      </c>
-      <c r="X77">
+      <c r="AA77" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB77">
         <v>343</v>
       </c>
-      <c r="Y77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:25">
+      <c r="AC77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -6755,22 +7691,34 @@
         <v>76</v>
       </c>
       <c r="U78">
+        <v>76</v>
+      </c>
+      <c r="V78">
+        <v>76</v>
+      </c>
+      <c r="W78">
+        <v>76</v>
+      </c>
+      <c r="X78">
+        <v>76</v>
+      </c>
+      <c r="Y78">
         <v>6376</v>
       </c>
-      <c r="V78">
+      <c r="Z78">
         <v>6719</v>
       </c>
-      <c r="W78" t="s">
-        <v>100</v>
-      </c>
-      <c r="X78">
+      <c r="AA78" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB78">
         <v>343</v>
       </c>
-      <c r="Y78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:25">
+      <c r="AC78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -6832,22 +7780,34 @@
         <v>77</v>
       </c>
       <c r="U79">
+        <v>77</v>
+      </c>
+      <c r="V79">
+        <v>77</v>
+      </c>
+      <c r="W79">
+        <v>77</v>
+      </c>
+      <c r="X79">
+        <v>77</v>
+      </c>
+      <c r="Y79">
         <v>6502</v>
       </c>
-      <c r="V79">
+      <c r="Z79">
         <v>6845</v>
       </c>
-      <c r="W79" t="s">
-        <v>101</v>
-      </c>
-      <c r="X79">
+      <c r="AA79" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB79">
         <v>343</v>
       </c>
-      <c r="Y79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:25">
+      <c r="AC79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -6909,22 +7869,34 @@
         <v>78</v>
       </c>
       <c r="U80">
+        <v>78</v>
+      </c>
+      <c r="V80">
+        <v>78</v>
+      </c>
+      <c r="W80">
+        <v>78</v>
+      </c>
+      <c r="X80">
+        <v>78</v>
+      </c>
+      <c r="Y80">
         <v>6568</v>
       </c>
-      <c r="V80">
+      <c r="Z80">
         <v>6923</v>
       </c>
-      <c r="W80" t="s">
-        <v>102</v>
-      </c>
-      <c r="X80">
+      <c r="AA80" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB80">
         <v>355</v>
       </c>
-      <c r="Y80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:25">
+      <c r="AC80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -6986,22 +7958,34 @@
         <v>79</v>
       </c>
       <c r="U81">
+        <v>79</v>
+      </c>
+      <c r="V81">
+        <v>79</v>
+      </c>
+      <c r="W81">
+        <v>79</v>
+      </c>
+      <c r="X81">
+        <v>79</v>
+      </c>
+      <c r="Y81">
         <v>6701</v>
       </c>
-      <c r="V81">
+      <c r="Z81">
         <v>7056</v>
       </c>
-      <c r="W81" t="s">
-        <v>103</v>
-      </c>
-      <c r="X81">
+      <c r="AA81" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB81">
         <v>355</v>
       </c>
-      <c r="Y81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:25">
+      <c r="AC81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -7063,22 +8047,34 @@
         <v>80</v>
       </c>
       <c r="U82">
+        <v>80</v>
+      </c>
+      <c r="V82">
+        <v>80</v>
+      </c>
+      <c r="W82">
+        <v>80</v>
+      </c>
+      <c r="X82">
+        <v>80</v>
+      </c>
+      <c r="Y82">
         <v>6829</v>
       </c>
-      <c r="V82">
+      <c r="Z82">
         <v>7186</v>
       </c>
-      <c r="W82" t="s">
-        <v>104</v>
-      </c>
-      <c r="X82">
+      <c r="AA82" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB82">
         <v>357</v>
       </c>
-      <c r="Y82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25">
+      <c r="AC82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -7140,22 +8136,34 @@
         <v>81</v>
       </c>
       <c r="U83">
+        <v>81</v>
+      </c>
+      <c r="V83">
+        <v>81</v>
+      </c>
+      <c r="W83">
+        <v>81</v>
+      </c>
+      <c r="X83">
+        <v>81</v>
+      </c>
+      <c r="Y83">
         <v>6973</v>
       </c>
-      <c r="V83">
+      <c r="Z83">
         <v>7331</v>
       </c>
-      <c r="W83" t="s">
-        <v>105</v>
-      </c>
-      <c r="X83">
+      <c r="AA83" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB83">
         <v>358</v>
       </c>
-      <c r="Y83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:25">
+      <c r="AC83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -7217,22 +8225,34 @@
         <v>82</v>
       </c>
       <c r="U84">
+        <v>82</v>
+      </c>
+      <c r="V84">
+        <v>82</v>
+      </c>
+      <c r="W84">
+        <v>82</v>
+      </c>
+      <c r="X84">
+        <v>82</v>
+      </c>
+      <c r="Y84">
         <v>7124</v>
       </c>
-      <c r="V84">
+      <c r="Z84">
         <v>7483</v>
       </c>
-      <c r="W84" t="s">
-        <v>106</v>
-      </c>
-      <c r="X84">
+      <c r="AA84" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB84">
         <v>359</v>
       </c>
-      <c r="Y84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25">
+      <c r="AC84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -7294,22 +8314,34 @@
         <v>83</v>
       </c>
       <c r="U85">
+        <v>83</v>
+      </c>
+      <c r="V85">
+        <v>83</v>
+      </c>
+      <c r="W85">
+        <v>83</v>
+      </c>
+      <c r="X85">
+        <v>83</v>
+      </c>
+      <c r="Y85">
         <v>7229</v>
       </c>
-      <c r="V85">
+      <c r="Z85">
         <v>7592</v>
       </c>
-      <c r="W85" t="s">
-        <v>107</v>
-      </c>
-      <c r="X85">
+      <c r="AA85" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB85">
         <v>363</v>
       </c>
-      <c r="Y85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:25">
+      <c r="AC85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -7371,22 +8403,34 @@
         <v>84</v>
       </c>
       <c r="U86">
+        <v>84</v>
+      </c>
+      <c r="V86">
+        <v>84</v>
+      </c>
+      <c r="W86">
+        <v>84</v>
+      </c>
+      <c r="X86">
+        <v>84</v>
+      </c>
+      <c r="Y86">
         <v>7434</v>
       </c>
-      <c r="V86">
+      <c r="Z86">
         <v>7799</v>
       </c>
-      <c r="W86" t="s">
-        <v>108</v>
-      </c>
-      <c r="X86">
+      <c r="AA86" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB86">
         <v>365</v>
       </c>
-      <c r="Y86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:25">
+      <c r="AC86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -7448,22 +8492,34 @@
         <v>85</v>
       </c>
       <c r="U87">
+        <v>85</v>
+      </c>
+      <c r="V87">
+        <v>85</v>
+      </c>
+      <c r="W87">
+        <v>85</v>
+      </c>
+      <c r="X87">
+        <v>85</v>
+      </c>
+      <c r="Y87">
         <v>7548</v>
       </c>
-      <c r="V87">
+      <c r="Z87">
         <v>7915</v>
       </c>
-      <c r="W87" t="s">
-        <v>109</v>
-      </c>
-      <c r="X87">
+      <c r="AA87" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB87">
         <v>367</v>
       </c>
-      <c r="Y87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:25">
+      <c r="AC87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -7525,22 +8581,34 @@
         <v>86</v>
       </c>
       <c r="U88">
+        <v>86</v>
+      </c>
+      <c r="V88">
+        <v>86</v>
+      </c>
+      <c r="W88">
+        <v>86</v>
+      </c>
+      <c r="X88">
+        <v>86</v>
+      </c>
+      <c r="Y88">
         <v>7725</v>
       </c>
-      <c r="V88">
+      <c r="Z88">
         <v>8100</v>
       </c>
-      <c r="W88" t="s">
-        <v>110</v>
-      </c>
-      <c r="X88">
+      <c r="AA88" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB88">
         <v>375</v>
       </c>
-      <c r="Y88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:25">
+      <c r="AC88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -7602,22 +8670,34 @@
         <v>87</v>
       </c>
       <c r="U89">
+        <v>87</v>
+      </c>
+      <c r="V89">
+        <v>87</v>
+      </c>
+      <c r="W89">
+        <v>87</v>
+      </c>
+      <c r="X89">
+        <v>87</v>
+      </c>
+      <c r="Y89">
         <v>7937</v>
       </c>
-      <c r="V89">
+      <c r="Z89">
         <v>8314</v>
       </c>
-      <c r="W89" t="s">
-        <v>111</v>
-      </c>
-      <c r="X89">
+      <c r="AA89" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB89">
         <v>377</v>
       </c>
-      <c r="Y89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:25">
+      <c r="AC89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -7679,22 +8759,34 @@
         <v>88</v>
       </c>
       <c r="U90">
+        <v>88</v>
+      </c>
+      <c r="V90">
+        <v>88</v>
+      </c>
+      <c r="W90">
+        <v>88</v>
+      </c>
+      <c r="X90">
+        <v>88</v>
+      </c>
+      <c r="Y90">
         <v>8179</v>
       </c>
-      <c r="V90">
+      <c r="Z90">
         <v>8556</v>
       </c>
-      <c r="W90" t="s">
-        <v>112</v>
-      </c>
-      <c r="X90">
+      <c r="AA90" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB90">
         <v>377</v>
       </c>
-      <c r="Y90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:25">
+      <c r="AC90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -7737,23 +8829,35 @@
       <c r="N91">
         <v>89</v>
       </c>
-      <c r="U91">
+      <c r="O91">
+        <v>89</v>
+      </c>
+      <c r="P91">
+        <v>89</v>
+      </c>
+      <c r="Q91">
+        <v>89</v>
+      </c>
+      <c r="R91">
+        <v>89</v>
+      </c>
+      <c r="Y91">
         <v>8357</v>
       </c>
-      <c r="V91">
+      <c r="Z91">
         <v>8735</v>
       </c>
-      <c r="W91" t="s">
-        <v>113</v>
-      </c>
-      <c r="X91">
+      <c r="AA91" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB91">
         <v>378</v>
       </c>
-      <c r="Y91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:25">
+      <c r="AC91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -7793,23 +8897,35 @@
       <c r="M92">
         <v>90</v>
       </c>
-      <c r="U92">
+      <c r="N92">
+        <v>90</v>
+      </c>
+      <c r="O92">
+        <v>90</v>
+      </c>
+      <c r="P92">
+        <v>90</v>
+      </c>
+      <c r="Q92">
+        <v>90</v>
+      </c>
+      <c r="Y92">
         <v>8436</v>
       </c>
-      <c r="V92">
+      <c r="Z92">
         <v>8815</v>
       </c>
-      <c r="W92" t="s">
-        <v>114</v>
-      </c>
-      <c r="X92">
+      <c r="AA92" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB92">
         <v>379</v>
       </c>
-      <c r="Y92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:25">
+      <c r="AC92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -7849,23 +8965,35 @@
       <c r="M93">
         <v>91</v>
       </c>
-      <c r="U93">
+      <c r="N93">
+        <v>91</v>
+      </c>
+      <c r="O93">
+        <v>91</v>
+      </c>
+      <c r="P93">
+        <v>91</v>
+      </c>
+      <c r="Q93">
+        <v>91</v>
+      </c>
+      <c r="Y93">
         <v>8777</v>
       </c>
-      <c r="V93">
+      <c r="Z93">
         <v>9157</v>
       </c>
-      <c r="W93" t="s">
-        <v>115</v>
-      </c>
-      <c r="X93">
+      <c r="AA93" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB93">
         <v>380</v>
       </c>
-      <c r="Y93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25">
+      <c r="AC93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -7902,23 +9030,35 @@
       <c r="L94">
         <v>92</v>
       </c>
-      <c r="U94">
+      <c r="M94">
+        <v>92</v>
+      </c>
+      <c r="N94">
+        <v>92</v>
+      </c>
+      <c r="O94">
+        <v>92</v>
+      </c>
+      <c r="P94">
+        <v>92</v>
+      </c>
+      <c r="Y94">
         <v>8932</v>
       </c>
-      <c r="V94">
+      <c r="Z94">
         <v>9318</v>
       </c>
-      <c r="W94" t="s">
-        <v>116</v>
-      </c>
-      <c r="X94">
+      <c r="AA94" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB94">
         <v>386</v>
       </c>
-      <c r="Y94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:25">
+      <c r="AC94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -7952,23 +9092,35 @@
       <c r="K95">
         <v>93</v>
       </c>
-      <c r="U95">
+      <c r="L95">
+        <v>93</v>
+      </c>
+      <c r="M95">
+        <v>93</v>
+      </c>
+      <c r="N95">
+        <v>93</v>
+      </c>
+      <c r="O95">
+        <v>93</v>
+      </c>
+      <c r="Y95">
         <v>9148</v>
       </c>
-      <c r="V95">
+      <c r="Z95">
         <v>9535</v>
       </c>
-      <c r="W95" t="s">
-        <v>117</v>
-      </c>
-      <c r="X95">
+      <c r="AA95" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB95">
         <v>387</v>
       </c>
-      <c r="Y95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:25">
+      <c r="AC95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -8002,23 +9154,35 @@
       <c r="K96">
         <v>94</v>
       </c>
-      <c r="U96">
+      <c r="L96">
+        <v>94</v>
+      </c>
+      <c r="M96">
+        <v>94</v>
+      </c>
+      <c r="N96">
+        <v>94</v>
+      </c>
+      <c r="O96">
+        <v>94</v>
+      </c>
+      <c r="Y96">
         <v>9462</v>
       </c>
-      <c r="V96">
+      <c r="Z96">
         <v>9852</v>
       </c>
-      <c r="W96" t="s">
-        <v>118</v>
-      </c>
-      <c r="X96">
+      <c r="AA96" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB96">
         <v>390</v>
       </c>
-      <c r="Y96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:25">
+      <c r="AC96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -8052,23 +9216,35 @@
       <c r="K97">
         <v>95</v>
       </c>
-      <c r="U97">
+      <c r="L97">
+        <v>95</v>
+      </c>
+      <c r="M97">
+        <v>95</v>
+      </c>
+      <c r="N97">
+        <v>95</v>
+      </c>
+      <c r="O97">
+        <v>95</v>
+      </c>
+      <c r="Y97">
         <v>9862</v>
       </c>
-      <c r="V97">
+      <c r="Z97">
         <v>10259</v>
       </c>
-      <c r="W97" t="s">
-        <v>119</v>
-      </c>
-      <c r="X97">
+      <c r="AA97" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB97">
         <v>397</v>
       </c>
-      <c r="Y97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:25">
+      <c r="AC97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -8102,23 +9278,35 @@
       <c r="K98">
         <v>96</v>
       </c>
-      <c r="U98">
+      <c r="L98">
+        <v>96</v>
+      </c>
+      <c r="M98">
+        <v>96</v>
+      </c>
+      <c r="N98">
+        <v>96</v>
+      </c>
+      <c r="O98">
+        <v>96</v>
+      </c>
+      <c r="Y98">
         <v>10088</v>
       </c>
-      <c r="V98">
+      <c r="Z98">
         <v>10486</v>
       </c>
-      <c r="W98" t="s">
-        <v>120</v>
-      </c>
-      <c r="X98">
+      <c r="AA98" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB98">
         <v>398</v>
       </c>
-      <c r="Y98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:25">
+      <c r="AC98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:29">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -8137,23 +9325,35 @@
       <c r="F99">
         <v>97</v>
       </c>
-      <c r="U99">
+      <c r="G99">
+        <v>97</v>
+      </c>
+      <c r="H99">
+        <v>97</v>
+      </c>
+      <c r="I99">
+        <v>97</v>
+      </c>
+      <c r="J99">
+        <v>97</v>
+      </c>
+      <c r="Y99">
         <v>10374</v>
       </c>
-      <c r="V99">
+      <c r="Z99">
         <v>10774</v>
       </c>
-      <c r="W99" t="s">
-        <v>121</v>
-      </c>
-      <c r="X99">
+      <c r="AA99" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB99">
         <v>400</v>
       </c>
-      <c r="Y99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:25">
+      <c r="AC99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -8169,162 +9369,258 @@
       <c r="E100">
         <v>98</v>
       </c>
-      <c r="U100">
+      <c r="F100">
+        <v>98</v>
+      </c>
+      <c r="G100">
+        <v>98</v>
+      </c>
+      <c r="H100">
+        <v>98</v>
+      </c>
+      <c r="I100">
+        <v>98</v>
+      </c>
+      <c r="Y100">
         <v>10374</v>
       </c>
-      <c r="V100">
+      <c r="Z100">
         <v>10774</v>
       </c>
-      <c r="W100" t="s">
-        <v>122</v>
-      </c>
-      <c r="X100">
+      <c r="AA100" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB100">
         <v>400</v>
       </c>
-      <c r="Y100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:25">
+      <c r="AC100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:29">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101">
         <v>99</v>
       </c>
-      <c r="U101">
+      <c r="C101">
+        <v>99</v>
+      </c>
+      <c r="D101">
+        <v>99</v>
+      </c>
+      <c r="E101">
+        <v>99</v>
+      </c>
+      <c r="F101">
+        <v>99</v>
+      </c>
+      <c r="Y101">
         <v>10374</v>
       </c>
-      <c r="V101">
+      <c r="Z101">
         <v>10774</v>
       </c>
-      <c r="W101" t="s">
-        <v>123</v>
-      </c>
-      <c r="X101">
+      <c r="AA101" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB101">
         <v>400</v>
       </c>
-      <c r="Y101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:25">
+      <c r="AC101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:29">
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="U102">
+      <c r="B102">
+        <v>100</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+      <c r="D102">
+        <v>100</v>
+      </c>
+      <c r="E102">
+        <v>100</v>
+      </c>
+      <c r="Y102">
         <v>11473</v>
       </c>
-      <c r="V102">
+      <c r="Z102">
         <v>11878</v>
       </c>
-      <c r="W102" t="s">
-        <v>124</v>
-      </c>
-      <c r="X102">
+      <c r="AA102" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB102">
         <v>405</v>
       </c>
-      <c r="Y102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:25">
+      <c r="AC102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:29">
       <c r="A103" s="1">
         <v>101</v>
       </c>
-      <c r="U103">
+      <c r="B103">
+        <v>101</v>
+      </c>
+      <c r="C103">
+        <v>101</v>
+      </c>
+      <c r="D103">
+        <v>101</v>
+      </c>
+      <c r="E103">
+        <v>101</v>
+      </c>
+      <c r="Y103">
         <v>11796</v>
       </c>
-      <c r="V103">
+      <c r="Z103">
         <v>12204</v>
       </c>
-      <c r="W103" t="s">
-        <v>125</v>
-      </c>
-      <c r="X103">
+      <c r="AA103" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB103">
         <v>408</v>
       </c>
-      <c r="Y103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:25">
+      <c r="AC103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:29">
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="U104">
+      <c r="B104">
+        <v>102</v>
+      </c>
+      <c r="C104">
+        <v>102</v>
+      </c>
+      <c r="D104">
+        <v>102</v>
+      </c>
+      <c r="E104">
+        <v>102</v>
+      </c>
+      <c r="Y104">
         <v>12764</v>
       </c>
-      <c r="V104">
+      <c r="Z104">
         <v>13174</v>
       </c>
-      <c r="W104" t="s">
-        <v>126</v>
-      </c>
-      <c r="X104">
+      <c r="AA104" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB104">
         <v>410</v>
       </c>
-      <c r="Y104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:25">
+      <c r="AC104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:29">
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="U105">
+      <c r="B105">
+        <v>103</v>
+      </c>
+      <c r="C105">
+        <v>103</v>
+      </c>
+      <c r="D105">
+        <v>103</v>
+      </c>
+      <c r="E105">
+        <v>103</v>
+      </c>
+      <c r="Y105">
         <v>13500</v>
       </c>
-      <c r="V105">
+      <c r="Z105">
         <v>13910</v>
       </c>
-      <c r="W105" t="s">
-        <v>127</v>
-      </c>
-      <c r="X105">
+      <c r="AA105" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB105">
         <v>410</v>
       </c>
-      <c r="Y105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:25">
+      <c r="AC105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:29">
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="U106">
+      <c r="B106">
+        <v>104</v>
+      </c>
+      <c r="C106">
+        <v>104</v>
+      </c>
+      <c r="D106">
+        <v>104</v>
+      </c>
+      <c r="E106">
+        <v>104</v>
+      </c>
+      <c r="Y106">
         <v>14193</v>
       </c>
-      <c r="V106">
+      <c r="Z106">
         <v>14607</v>
       </c>
-      <c r="W106" t="s">
-        <v>128</v>
-      </c>
-      <c r="X106">
+      <c r="AA106" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB106">
         <v>414</v>
       </c>
-      <c r="Y106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:25">
+      <c r="AC106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:29">
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="U107">
+      <c r="B107">
+        <v>105</v>
+      </c>
+      <c r="C107">
+        <v>105</v>
+      </c>
+      <c r="D107">
+        <v>105</v>
+      </c>
+      <c r="E107">
+        <v>105</v>
+      </c>
+      <c r="Y107">
         <v>14679</v>
       </c>
-      <c r="V107">
+      <c r="Z107">
         <v>15095</v>
       </c>
-      <c r="W107" t="s">
-        <v>129</v>
-      </c>
-      <c r="X107">
+      <c r="AA107" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB107">
         <v>416</v>
       </c>
-      <c r="Y107">
+      <c r="AC107">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Miami-Dade County, FL
</commit_message>
<xml_diff>
--- a/Clark_Data.xlsx
+++ b/Clark_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
   </si>
   <si>
     <t>Active</t>
@@ -830,13 +839,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG122"/>
+  <dimension ref="A1:AJ122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:36">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -933,8 +942,17 @@
       <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:36">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1023,19 +1041,28 @@
         <v>0</v>
       </c>
       <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
         <v>1</v>
       </c>
-      <c r="AE2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
+      <c r="AH2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:36">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1121,22 +1148,31 @@
         <v>1</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3">
         <v>1</v>
       </c>
-      <c r="AE3" t="s">
-        <v>33</v>
+      <c r="AE3">
+        <v>1</v>
       </c>
       <c r="AF3">
         <v>0</v>
       </c>
       <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:36">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1222,22 +1258,31 @@
         <v>2</v>
       </c>
       <c r="AC4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD4">
+        <v>2</v>
+      </c>
+      <c r="AE4">
+        <v>2</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
         <v>1</v>
       </c>
-      <c r="AE4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
+      <c r="AH4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:36">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1323,22 +1368,31 @@
         <v>3</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD5">
+        <v>3</v>
+      </c>
+      <c r="AE5">
+        <v>3</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
         <v>2</v>
       </c>
-      <c r="AE5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
+      <c r="AH5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:36">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1424,22 +1478,31 @@
         <v>4</v>
       </c>
       <c r="AC6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD6">
+        <v>4</v>
+      </c>
+      <c r="AE6">
+        <v>4</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
         <v>2</v>
       </c>
-      <c r="AE6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
+      <c r="AH6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:36">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1525,22 +1588,31 @@
         <v>5</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AD7">
+        <v>5</v>
+      </c>
+      <c r="AE7">
+        <v>5</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <v>126</v>
       </c>
-      <c r="AE7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF7">
+      <c r="AH7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI7">
         <v>2</v>
       </c>
-      <c r="AG7">
+      <c r="AJ7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:36">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1626,22 +1698,31 @@
         <v>6</v>
       </c>
       <c r="AC8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AD8">
+        <v>6</v>
+      </c>
+      <c r="AE8">
+        <v>6</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
         <v>126</v>
       </c>
-      <c r="AE8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF8">
+      <c r="AH8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI8">
         <v>4</v>
       </c>
-      <c r="AG8">
+      <c r="AJ8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:36">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1727,22 +1808,31 @@
         <v>7</v>
       </c>
       <c r="AC9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9">
+        <v>7</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
         <v>212</v>
       </c>
-      <c r="AE9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF9">
+      <c r="AH9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI9">
         <v>4</v>
       </c>
-      <c r="AG9">
+      <c r="AJ9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:36">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1828,22 +1918,31 @@
         <v>8</v>
       </c>
       <c r="AC10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD10">
+        <v>8</v>
+      </c>
+      <c r="AE10">
+        <v>8</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
         <v>249</v>
       </c>
-      <c r="AE10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF10">
+      <c r="AH10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI10">
         <v>6</v>
       </c>
-      <c r="AG10">
+      <c r="AJ10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:36">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1929,22 +2028,31 @@
         <v>9</v>
       </c>
       <c r="AC11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AD11">
+        <v>9</v>
+      </c>
+      <c r="AE11">
+        <v>9</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
         <v>350</v>
       </c>
-      <c r="AE11" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF11">
+      <c r="AH11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI11">
         <v>6</v>
       </c>
-      <c r="AG11">
+      <c r="AJ11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:36">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2030,22 +2138,31 @@
         <v>10</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD12">
+        <v>10</v>
+      </c>
+      <c r="AE12">
+        <v>10</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
         <v>443</v>
       </c>
-      <c r="AE12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF12">
+      <c r="AH12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI12">
         <v>10</v>
       </c>
-      <c r="AG12">
+      <c r="AJ12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:36">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2131,22 +2248,31 @@
         <v>11</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AD13">
+        <v>11</v>
+      </c>
+      <c r="AE13">
+        <v>11</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
         <v>443</v>
       </c>
-      <c r="AE13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF13">
+      <c r="AH13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI13">
         <v>10</v>
       </c>
-      <c r="AG13">
+      <c r="AJ13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:36">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2232,22 +2358,31 @@
         <v>12</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AD14">
+        <v>12</v>
+      </c>
+      <c r="AE14">
+        <v>12</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
         <v>528</v>
       </c>
-      <c r="AE14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF14">
+      <c r="AH14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI14">
         <v>14</v>
       </c>
-      <c r="AG14">
+      <c r="AJ14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:36">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2333,22 +2468,31 @@
         <v>13</v>
       </c>
       <c r="AC15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AD15">
+        <v>13</v>
+      </c>
+      <c r="AE15">
+        <v>13</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
         <v>753</v>
       </c>
-      <c r="AE15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF15">
+      <c r="AH15" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI15">
         <v>14</v>
       </c>
-      <c r="AG15">
+      <c r="AJ15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:36">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2434,22 +2578,31 @@
         <v>14</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AD16">
+        <v>14</v>
+      </c>
+      <c r="AE16">
+        <v>14</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
         <v>869</v>
       </c>
-      <c r="AE16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF16">
+      <c r="AH16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI16">
         <v>23</v>
       </c>
-      <c r="AG16">
+      <c r="AJ16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:36">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2535,22 +2688,31 @@
         <v>15</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD17">
+        <v>15</v>
+      </c>
+      <c r="AE17">
+        <v>15</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
         <v>961</v>
       </c>
-      <c r="AE17" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF17">
+      <c r="AH17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI17">
         <v>28</v>
       </c>
-      <c r="AG17">
+      <c r="AJ17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:36">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2636,22 +2798,31 @@
         <v>16</v>
       </c>
       <c r="AC18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD18">
+        <v>16</v>
+      </c>
+      <c r="AE18">
+        <v>16</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
         <v>1125</v>
       </c>
-      <c r="AE18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF18">
+      <c r="AH18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI18">
         <v>34</v>
       </c>
-      <c r="AG18">
+      <c r="AJ18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:36">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2737,22 +2908,31 @@
         <v>17</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AD19">
+        <v>17</v>
+      </c>
+      <c r="AE19">
+        <v>17</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
         <v>1279</v>
       </c>
-      <c r="AE19" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF19">
+      <c r="AH19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI19">
         <v>39</v>
       </c>
-      <c r="AG19">
+      <c r="AJ19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:36">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2838,22 +3018,31 @@
         <v>18</v>
       </c>
       <c r="AC20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AD20">
+        <v>18</v>
+      </c>
+      <c r="AE20">
+        <v>18</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
         <v>1418</v>
       </c>
-      <c r="AE20" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF20">
+      <c r="AH20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI20">
         <v>41</v>
       </c>
-      <c r="AG20">
+      <c r="AJ20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:36">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2939,22 +3128,31 @@
         <v>19</v>
       </c>
       <c r="AC21">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AD21">
+        <v>19</v>
+      </c>
+      <c r="AE21">
+        <v>19</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
         <v>1519</v>
       </c>
-      <c r="AE21" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF21">
+      <c r="AH21" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI21">
         <v>41</v>
       </c>
-      <c r="AG21">
+      <c r="AJ21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:36">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3040,22 +3238,31 @@
         <v>20</v>
       </c>
       <c r="AC22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AD22">
+        <v>20</v>
+      </c>
+      <c r="AE22">
+        <v>20</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
         <v>1608</v>
       </c>
-      <c r="AE22" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF22">
+      <c r="AH22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI22">
         <v>41</v>
       </c>
-      <c r="AG22">
+      <c r="AJ22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:36">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3141,22 +3348,31 @@
         <v>21</v>
       </c>
       <c r="AC23">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AD23">
+        <v>21</v>
+      </c>
+      <c r="AE23">
+        <v>21</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
         <v>1734</v>
       </c>
-      <c r="AE23" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF23">
+      <c r="AH23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI23">
         <v>54</v>
       </c>
-      <c r="AG23">
+      <c r="AJ23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:36">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3242,22 +3458,31 @@
         <v>22</v>
       </c>
       <c r="AC24">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AD24">
+        <v>22</v>
+      </c>
+      <c r="AE24">
+        <v>22</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
         <v>1878</v>
       </c>
-      <c r="AE24" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF24">
+      <c r="AH24" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI24">
         <v>65</v>
       </c>
-      <c r="AG24">
+      <c r="AJ24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:36">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3343,22 +3568,31 @@
         <v>23</v>
       </c>
       <c r="AC25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="AD25">
+        <v>23</v>
+      </c>
+      <c r="AE25">
+        <v>23</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
         <v>2009</v>
       </c>
-      <c r="AE25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF25">
+      <c r="AH25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI25">
         <v>71</v>
       </c>
-      <c r="AG25">
+      <c r="AJ25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:36">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3444,22 +3678,31 @@
         <v>24</v>
       </c>
       <c r="AC26">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AD26">
+        <v>24</v>
+      </c>
+      <c r="AE26">
+        <v>24</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
         <v>2144</v>
       </c>
-      <c r="AE26" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF26">
+      <c r="AH26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI26">
         <v>75</v>
       </c>
-      <c r="AG26">
+      <c r="AJ26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:36">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3545,22 +3788,31 @@
         <v>25</v>
       </c>
       <c r="AC27">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AD27">
+        <v>25</v>
+      </c>
+      <c r="AE27">
+        <v>25</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
         <v>2144</v>
       </c>
-      <c r="AE27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF27">
+      <c r="AH27" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI27">
         <v>75</v>
       </c>
-      <c r="AG27">
+      <c r="AJ27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:36">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3646,22 +3898,31 @@
         <v>26</v>
       </c>
       <c r="AC28">
+        <v>26</v>
+      </c>
+      <c r="AD28">
+        <v>26</v>
+      </c>
+      <c r="AE28">
+        <v>26</v>
+      </c>
+      <c r="AF28">
         <v>2224</v>
       </c>
-      <c r="AD28">
+      <c r="AG28">
         <v>2324</v>
       </c>
-      <c r="AE28" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF28">
+      <c r="AH28" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI28">
         <v>100</v>
       </c>
-      <c r="AG28">
+      <c r="AJ28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:36">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3747,22 +4008,31 @@
         <v>27</v>
       </c>
       <c r="AC29">
+        <v>27</v>
+      </c>
+      <c r="AD29">
+        <v>27</v>
+      </c>
+      <c r="AE29">
+        <v>27</v>
+      </c>
+      <c r="AF29">
         <v>2343</v>
       </c>
-      <c r="AD29">
+      <c r="AG29">
         <v>2444</v>
       </c>
-      <c r="AE29" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF29">
+      <c r="AH29" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI29">
         <v>101</v>
       </c>
-      <c r="AG29">
+      <c r="AJ29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:36">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3848,22 +4118,31 @@
         <v>28</v>
       </c>
       <c r="AC30">
+        <v>28</v>
+      </c>
+      <c r="AD30">
+        <v>28</v>
+      </c>
+      <c r="AE30">
+        <v>28</v>
+      </c>
+      <c r="AF30">
         <v>2403</v>
       </c>
-      <c r="AD30">
+      <c r="AG30">
         <v>2509</v>
       </c>
-      <c r="AE30" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF30">
+      <c r="AH30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI30">
         <v>106</v>
       </c>
-      <c r="AG30">
+      <c r="AJ30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:36">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3949,22 +4228,31 @@
         <v>29</v>
       </c>
       <c r="AC31">
+        <v>29</v>
+      </c>
+      <c r="AD31">
+        <v>29</v>
+      </c>
+      <c r="AE31">
+        <v>29</v>
+      </c>
+      <c r="AF31">
         <v>2444</v>
       </c>
-      <c r="AD31">
+      <c r="AG31">
         <v>2559</v>
       </c>
-      <c r="AE31" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF31">
+      <c r="AH31" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI31">
         <v>115</v>
       </c>
-      <c r="AG31">
+      <c r="AJ31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:36">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4050,22 +4338,31 @@
         <v>30</v>
       </c>
       <c r="AC32">
+        <v>30</v>
+      </c>
+      <c r="AD32">
+        <v>30</v>
+      </c>
+      <c r="AE32">
+        <v>30</v>
+      </c>
+      <c r="AF32">
         <v>2444</v>
       </c>
-      <c r="AD32">
+      <c r="AG32">
         <v>2559</v>
       </c>
-      <c r="AE32" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF32">
+      <c r="AH32" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI32">
         <v>115</v>
       </c>
-      <c r="AG32">
+      <c r="AJ32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:36">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4151,22 +4448,31 @@
         <v>31</v>
       </c>
       <c r="AC33">
+        <v>31</v>
+      </c>
+      <c r="AD33">
+        <v>31</v>
+      </c>
+      <c r="AE33">
+        <v>31</v>
+      </c>
+      <c r="AF33">
         <v>2614</v>
       </c>
-      <c r="AD33">
+      <c r="AG33">
         <v>2738</v>
       </c>
-      <c r="AE33" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF33">
+      <c r="AH33" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI33">
         <v>124</v>
       </c>
-      <c r="AG33">
+      <c r="AJ33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:36">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4252,22 +4558,31 @@
         <v>32</v>
       </c>
       <c r="AC34">
+        <v>32</v>
+      </c>
+      <c r="AD34">
+        <v>32</v>
+      </c>
+      <c r="AE34">
+        <v>32</v>
+      </c>
+      <c r="AF34">
         <v>2749</v>
       </c>
-      <c r="AD34">
+      <c r="AG34">
         <v>2882</v>
       </c>
-      <c r="AE34" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF34">
+      <c r="AH34" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI34">
         <v>133</v>
       </c>
-      <c r="AG34">
+      <c r="AJ34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:36">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4353,22 +4668,31 @@
         <v>33</v>
       </c>
       <c r="AC35">
+        <v>33</v>
+      </c>
+      <c r="AD35">
+        <v>33</v>
+      </c>
+      <c r="AE35">
+        <v>33</v>
+      </c>
+      <c r="AF35">
         <v>2803</v>
       </c>
-      <c r="AD35">
+      <c r="AG35">
         <v>2940</v>
       </c>
-      <c r="AE35" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF35">
+      <c r="AH35" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI35">
         <v>137</v>
       </c>
-      <c r="AG35">
+      <c r="AJ35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:36">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4454,22 +4778,31 @@
         <v>34</v>
       </c>
       <c r="AC36">
+        <v>34</v>
+      </c>
+      <c r="AD36">
+        <v>34</v>
+      </c>
+      <c r="AE36">
+        <v>34</v>
+      </c>
+      <c r="AF36">
         <v>2861</v>
       </c>
-      <c r="AD36">
+      <c r="AG36">
         <v>2998</v>
       </c>
-      <c r="AE36" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF36">
+      <c r="AH36" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI36">
         <v>137</v>
       </c>
-      <c r="AG36">
+      <c r="AJ36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:36">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4555,22 +4888,31 @@
         <v>35</v>
       </c>
       <c r="AC37">
+        <v>35</v>
+      </c>
+      <c r="AD37">
+        <v>35</v>
+      </c>
+      <c r="AE37">
+        <v>35</v>
+      </c>
+      <c r="AF37">
         <v>2958</v>
       </c>
-      <c r="AD37">
+      <c r="AG37">
         <v>3099</v>
       </c>
-      <c r="AE37" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF37">
+      <c r="AH37" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI37">
         <v>141</v>
       </c>
-      <c r="AG37">
+      <c r="AJ37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:36">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4656,22 +4998,31 @@
         <v>36</v>
       </c>
       <c r="AC38">
+        <v>36</v>
+      </c>
+      <c r="AD38">
+        <v>36</v>
+      </c>
+      <c r="AE38">
+        <v>36</v>
+      </c>
+      <c r="AF38">
         <v>3068</v>
       </c>
-      <c r="AD38">
+      <c r="AG38">
         <v>3218</v>
       </c>
-      <c r="AE38" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF38">
+      <c r="AH38" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI38">
         <v>150</v>
       </c>
-      <c r="AG38">
+      <c r="AJ38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:36">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4757,22 +5108,31 @@
         <v>37</v>
       </c>
       <c r="AC39">
+        <v>37</v>
+      </c>
+      <c r="AD39">
+        <v>37</v>
+      </c>
+      <c r="AE39">
+        <v>37</v>
+      </c>
+      <c r="AF39">
         <v>3151</v>
       </c>
-      <c r="AD39">
+      <c r="AG39">
         <v>3314</v>
       </c>
-      <c r="AE39" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF39">
+      <c r="AH39" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI39">
         <v>163</v>
       </c>
-      <c r="AG39">
+      <c r="AJ39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:36">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4858,22 +5218,31 @@
         <v>38</v>
       </c>
       <c r="AC40">
+        <v>38</v>
+      </c>
+      <c r="AD40">
+        <v>38</v>
+      </c>
+      <c r="AE40">
+        <v>38</v>
+      </c>
+      <c r="AF40">
         <v>3275</v>
       </c>
-      <c r="AD40">
+      <c r="AG40">
         <v>3443</v>
       </c>
-      <c r="AE40" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF40">
+      <c r="AH40" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI40">
         <v>168</v>
       </c>
-      <c r="AG40">
+      <c r="AJ40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:36">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4959,22 +5328,31 @@
         <v>39</v>
       </c>
       <c r="AC41">
+        <v>39</v>
+      </c>
+      <c r="AD41">
+        <v>39</v>
+      </c>
+      <c r="AE41">
+        <v>39</v>
+      </c>
+      <c r="AF41">
         <v>3396</v>
       </c>
-      <c r="AD41">
+      <c r="AG41">
         <v>3570</v>
       </c>
-      <c r="AE41" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF41">
+      <c r="AH41" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI41">
         <v>174</v>
       </c>
-      <c r="AG41">
+      <c r="AJ41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:36">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -5060,22 +5438,31 @@
         <v>40</v>
       </c>
       <c r="AC42">
+        <v>40</v>
+      </c>
+      <c r="AD42">
+        <v>40</v>
+      </c>
+      <c r="AE42">
+        <v>40</v>
+      </c>
+      <c r="AF42">
         <v>3491</v>
       </c>
-      <c r="AD42">
+      <c r="AG42">
         <v>3665</v>
       </c>
-      <c r="AE42" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF42">
+      <c r="AH42" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI42">
         <v>174</v>
       </c>
-      <c r="AG42">
+      <c r="AJ42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:36">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -5161,22 +5548,31 @@
         <v>41</v>
       </c>
       <c r="AC43">
+        <v>41</v>
+      </c>
+      <c r="AD43">
+        <v>41</v>
+      </c>
+      <c r="AE43">
+        <v>41</v>
+      </c>
+      <c r="AF43">
         <v>3543</v>
       </c>
-      <c r="AD43">
+      <c r="AG43">
         <v>3717</v>
       </c>
-      <c r="AE43" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF43">
+      <c r="AH43" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI43">
         <v>174</v>
       </c>
-      <c r="AG43">
+      <c r="AJ43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:36">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -5262,22 +5658,31 @@
         <v>42</v>
       </c>
       <c r="AC44">
+        <v>42</v>
+      </c>
+      <c r="AD44">
+        <v>42</v>
+      </c>
+      <c r="AE44">
+        <v>42</v>
+      </c>
+      <c r="AF44">
         <v>3607</v>
       </c>
-      <c r="AD44">
+      <c r="AG44">
         <v>3793</v>
       </c>
-      <c r="AE44" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF44">
+      <c r="AH44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI44">
         <v>186</v>
       </c>
-      <c r="AG44">
+      <c r="AJ44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:36">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -5363,22 +5768,31 @@
         <v>43</v>
       </c>
       <c r="AC45">
+        <v>43</v>
+      </c>
+      <c r="AD45">
+        <v>43</v>
+      </c>
+      <c r="AE45">
+        <v>43</v>
+      </c>
+      <c r="AF45">
         <v>3695</v>
       </c>
-      <c r="AD45">
+      <c r="AG45">
         <v>3891</v>
       </c>
-      <c r="AE45" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF45">
+      <c r="AH45" t="s">
+        <v>78</v>
+      </c>
+      <c r="AI45">
         <v>196</v>
       </c>
-      <c r="AG45">
+      <c r="AJ45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:36">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5464,22 +5878,31 @@
         <v>44</v>
       </c>
       <c r="AC46">
+        <v>44</v>
+      </c>
+      <c r="AD46">
+        <v>44</v>
+      </c>
+      <c r="AE46">
+        <v>44</v>
+      </c>
+      <c r="AF46">
         <v>3777</v>
       </c>
-      <c r="AD46">
+      <c r="AG46">
         <v>3979</v>
       </c>
-      <c r="AE46" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF46">
+      <c r="AH46" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI46">
         <v>202</v>
       </c>
-      <c r="AG46">
+      <c r="AJ46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:36">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5565,22 +5988,31 @@
         <v>45</v>
       </c>
       <c r="AC47">
+        <v>45</v>
+      </c>
+      <c r="AD47">
+        <v>45</v>
+      </c>
+      <c r="AE47">
+        <v>45</v>
+      </c>
+      <c r="AF47">
         <v>3912</v>
       </c>
-      <c r="AD47">
+      <c r="AG47">
         <v>4118</v>
       </c>
-      <c r="AE47" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF47">
+      <c r="AH47" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI47">
         <v>206</v>
       </c>
-      <c r="AG47">
+      <c r="AJ47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:36">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -5666,22 +6098,31 @@
         <v>46</v>
       </c>
       <c r="AC48">
+        <v>46</v>
+      </c>
+      <c r="AD48">
+        <v>46</v>
+      </c>
+      <c r="AE48">
+        <v>46</v>
+      </c>
+      <c r="AF48">
         <v>4010</v>
       </c>
-      <c r="AD48">
+      <c r="AG48">
         <v>4225</v>
       </c>
-      <c r="AE48" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF48">
+      <c r="AH48" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI48">
         <v>215</v>
       </c>
-      <c r="AG48">
+      <c r="AJ48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:36">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -5767,22 +6208,31 @@
         <v>47</v>
       </c>
       <c r="AC49">
+        <v>47</v>
+      </c>
+      <c r="AD49">
+        <v>47</v>
+      </c>
+      <c r="AE49">
+        <v>47</v>
+      </c>
+      <c r="AF49">
         <v>4056</v>
       </c>
-      <c r="AD49">
+      <c r="AG49">
         <v>4274</v>
       </c>
-      <c r="AE49" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF49">
+      <c r="AH49" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI49">
         <v>218</v>
       </c>
-      <c r="AG49">
+      <c r="AJ49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:36">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -5868,22 +6318,31 @@
         <v>48</v>
       </c>
       <c r="AC50">
+        <v>48</v>
+      </c>
+      <c r="AD50">
+        <v>48</v>
+      </c>
+      <c r="AE50">
+        <v>48</v>
+      </c>
+      <c r="AF50">
         <v>4188</v>
       </c>
-      <c r="AD50">
+      <c r="AG50">
         <v>4411</v>
       </c>
-      <c r="AE50" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF50">
+      <c r="AH50" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI50">
         <v>223</v>
       </c>
-      <c r="AG50">
+      <c r="AJ50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:36">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -5969,22 +6428,31 @@
         <v>49</v>
       </c>
       <c r="AC51">
+        <v>49</v>
+      </c>
+      <c r="AD51">
+        <v>49</v>
+      </c>
+      <c r="AE51">
+        <v>49</v>
+      </c>
+      <c r="AF51">
         <v>4182</v>
       </c>
-      <c r="AD51">
+      <c r="AG51">
         <v>4408</v>
       </c>
-      <c r="AE51" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF51">
+      <c r="AH51" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI51">
         <v>226</v>
       </c>
-      <c r="AG51">
+      <c r="AJ51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:36">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6070,22 +6538,31 @@
         <v>50</v>
       </c>
       <c r="AC52">
+        <v>50</v>
+      </c>
+      <c r="AD52">
+        <v>50</v>
+      </c>
+      <c r="AE52">
+        <v>50</v>
+      </c>
+      <c r="AF52">
         <v>4235</v>
       </c>
-      <c r="AD52">
+      <c r="AG52">
         <v>4473</v>
       </c>
-      <c r="AE52" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF52">
+      <c r="AH52" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI52">
         <v>238</v>
       </c>
-      <c r="AG52">
+      <c r="AJ52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:36">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6171,22 +6648,31 @@
         <v>51</v>
       </c>
       <c r="AC53">
+        <v>51</v>
+      </c>
+      <c r="AD53">
+        <v>51</v>
+      </c>
+      <c r="AE53">
+        <v>51</v>
+      </c>
+      <c r="AF53">
         <v>4328</v>
       </c>
-      <c r="AD53">
+      <c r="AG53">
         <v>4573</v>
       </c>
-      <c r="AE53" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF53">
+      <c r="AH53" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI53">
         <v>245</v>
       </c>
-      <c r="AG53">
+      <c r="AJ53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:36">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6272,22 +6758,31 @@
         <v>52</v>
       </c>
       <c r="AC54">
+        <v>52</v>
+      </c>
+      <c r="AD54">
+        <v>52</v>
+      </c>
+      <c r="AE54">
+        <v>52</v>
+      </c>
+      <c r="AF54">
         <v>4328</v>
       </c>
-      <c r="AD54">
+      <c r="AG54">
         <v>4573</v>
       </c>
-      <c r="AE54" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF54">
+      <c r="AH54" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI54">
         <v>245</v>
       </c>
-      <c r="AG54">
+      <c r="AJ54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:36">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6373,22 +6868,31 @@
         <v>53</v>
       </c>
       <c r="AC55">
+        <v>53</v>
+      </c>
+      <c r="AD55">
+        <v>53</v>
+      </c>
+      <c r="AE55">
+        <v>53</v>
+      </c>
+      <c r="AF55">
         <v>4448</v>
       </c>
-      <c r="AD55">
+      <c r="AG55">
         <v>4704</v>
       </c>
-      <c r="AE55" t="s">
-        <v>85</v>
-      </c>
-      <c r="AF55">
+      <c r="AH55" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI55">
         <v>256</v>
       </c>
-      <c r="AG55">
+      <c r="AJ55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:36">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6474,22 +6978,31 @@
         <v>54</v>
       </c>
       <c r="AC56">
+        <v>54</v>
+      </c>
+      <c r="AD56">
+        <v>54</v>
+      </c>
+      <c r="AE56">
+        <v>54</v>
+      </c>
+      <c r="AF56">
         <v>4490</v>
       </c>
-      <c r="AD56">
+      <c r="AG56">
         <v>4750</v>
       </c>
-      <c r="AE56" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF56">
+      <c r="AH56" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI56">
         <v>260</v>
       </c>
-      <c r="AG56">
+      <c r="AJ56">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:36">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6575,22 +7088,31 @@
         <v>55</v>
       </c>
       <c r="AC57">
+        <v>55</v>
+      </c>
+      <c r="AD57">
+        <v>55</v>
+      </c>
+      <c r="AE57">
+        <v>55</v>
+      </c>
+      <c r="AF57">
         <v>4502</v>
       </c>
-      <c r="AD57">
+      <c r="AG57">
         <v>4762</v>
       </c>
-      <c r="AE57" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF57">
+      <c r="AH57" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI57">
         <v>260</v>
       </c>
-      <c r="AG57">
+      <c r="AJ57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:36">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6676,22 +7198,31 @@
         <v>56</v>
       </c>
       <c r="AC58">
+        <v>56</v>
+      </c>
+      <c r="AD58">
+        <v>56</v>
+      </c>
+      <c r="AE58">
+        <v>56</v>
+      </c>
+      <c r="AF58">
         <v>4602</v>
       </c>
-      <c r="AD58">
+      <c r="AG58">
         <v>4869</v>
       </c>
-      <c r="AE58" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF58">
+      <c r="AH58" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI58">
         <v>267</v>
       </c>
-      <c r="AG58">
+      <c r="AJ58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:36">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6777,22 +7308,31 @@
         <v>57</v>
       </c>
       <c r="AC59">
+        <v>57</v>
+      </c>
+      <c r="AD59">
+        <v>57</v>
+      </c>
+      <c r="AE59">
+        <v>57</v>
+      </c>
+      <c r="AF59">
         <v>4770</v>
       </c>
-      <c r="AD59">
+      <c r="AG59">
         <v>5045</v>
       </c>
-      <c r="AE59" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF59">
+      <c r="AH59" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI59">
         <v>275</v>
       </c>
-      <c r="AG59">
+      <c r="AJ59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:36">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -6878,22 +7418,31 @@
         <v>58</v>
       </c>
       <c r="AC60">
+        <v>58</v>
+      </c>
+      <c r="AD60">
+        <v>58</v>
+      </c>
+      <c r="AE60">
+        <v>58</v>
+      </c>
+      <c r="AF60">
         <v>4770</v>
       </c>
-      <c r="AD60">
+      <c r="AG60">
         <v>5045</v>
       </c>
-      <c r="AE60" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF60">
+      <c r="AH60" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI60">
         <v>275</v>
       </c>
-      <c r="AG60">
+      <c r="AJ60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:36">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -6979,22 +7528,31 @@
         <v>59</v>
       </c>
       <c r="AC61">
+        <v>59</v>
+      </c>
+      <c r="AD61">
+        <v>59</v>
+      </c>
+      <c r="AE61">
+        <v>59</v>
+      </c>
+      <c r="AF61">
         <v>4944</v>
       </c>
-      <c r="AD61">
+      <c r="AG61">
         <v>5235</v>
       </c>
-      <c r="AE61" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF61">
+      <c r="AH61" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI61">
         <v>291</v>
       </c>
-      <c r="AG61">
+      <c r="AJ61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:36">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7080,22 +7638,31 @@
         <v>60</v>
       </c>
       <c r="AC62">
+        <v>60</v>
+      </c>
+      <c r="AD62">
+        <v>60</v>
+      </c>
+      <c r="AE62">
+        <v>60</v>
+      </c>
+      <c r="AF62">
         <v>5005</v>
       </c>
-      <c r="AD62">
+      <c r="AG62">
         <v>5298</v>
       </c>
-      <c r="AE62" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF62">
+      <c r="AH62" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI62">
         <v>293</v>
       </c>
-      <c r="AG62">
+      <c r="AJ62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:36">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7181,22 +7748,31 @@
         <v>61</v>
       </c>
       <c r="AC63">
+        <v>61</v>
+      </c>
+      <c r="AD63">
+        <v>61</v>
+      </c>
+      <c r="AE63">
+        <v>61</v>
+      </c>
+      <c r="AF63">
         <v>5070</v>
       </c>
-      <c r="AD63">
+      <c r="AG63">
         <v>5366</v>
       </c>
-      <c r="AE63" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF63">
+      <c r="AH63" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI63">
         <v>296</v>
       </c>
-      <c r="AG63">
+      <c r="AJ63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:36">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7282,22 +7858,31 @@
         <v>62</v>
       </c>
       <c r="AC64">
+        <v>62</v>
+      </c>
+      <c r="AD64">
+        <v>62</v>
+      </c>
+      <c r="AE64">
+        <v>62</v>
+      </c>
+      <c r="AF64">
         <v>5167</v>
       </c>
-      <c r="AD64">
+      <c r="AG64">
         <v>5463</v>
       </c>
-      <c r="AE64" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF64">
+      <c r="AH64" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI64">
         <v>296</v>
       </c>
-      <c r="AG64">
+      <c r="AJ64">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:36">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7383,22 +7968,31 @@
         <v>63</v>
       </c>
       <c r="AC65">
+        <v>63</v>
+      </c>
+      <c r="AD65">
+        <v>63</v>
+      </c>
+      <c r="AE65">
+        <v>63</v>
+      </c>
+      <c r="AF65">
         <v>5167</v>
       </c>
-      <c r="AD65">
+      <c r="AG65">
         <v>5463</v>
       </c>
-      <c r="AE65" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF65">
+      <c r="AH65" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI65">
         <v>296</v>
       </c>
-      <c r="AG65">
+      <c r="AJ65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:36">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7484,22 +8078,31 @@
         <v>64</v>
       </c>
       <c r="AC66">
+        <v>64</v>
+      </c>
+      <c r="AD66">
+        <v>64</v>
+      </c>
+      <c r="AE66">
+        <v>64</v>
+      </c>
+      <c r="AF66">
         <v>5336</v>
       </c>
-      <c r="AD66">
+      <c r="AG66">
         <v>5650</v>
       </c>
-      <c r="AE66" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF66">
+      <c r="AH66" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI66">
         <v>314</v>
       </c>
-      <c r="AG66">
+      <c r="AJ66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:36">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7585,22 +8188,31 @@
         <v>65</v>
       </c>
       <c r="AC67">
+        <v>65</v>
+      </c>
+      <c r="AD67">
+        <v>65</v>
+      </c>
+      <c r="AE67">
+        <v>65</v>
+      </c>
+      <c r="AF67">
         <v>5414</v>
       </c>
-      <c r="AD67">
+      <c r="AG67">
         <v>5734</v>
       </c>
-      <c r="AE67" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF67">
+      <c r="AH67" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI67">
         <v>320</v>
       </c>
-      <c r="AG67">
+      <c r="AJ67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:36">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7686,22 +8298,31 @@
         <v>66</v>
       </c>
       <c r="AC68">
+        <v>66</v>
+      </c>
+      <c r="AD68">
+        <v>66</v>
+      </c>
+      <c r="AE68">
+        <v>66</v>
+      </c>
+      <c r="AF68">
         <v>5493</v>
       </c>
-      <c r="AD68">
+      <c r="AG68">
         <v>5815</v>
       </c>
-      <c r="AE68" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF68">
+      <c r="AH68" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI68">
         <v>322</v>
       </c>
-      <c r="AG68">
+      <c r="AJ68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:36">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7787,22 +8408,31 @@
         <v>67</v>
       </c>
       <c r="AC69">
+        <v>67</v>
+      </c>
+      <c r="AD69">
+        <v>67</v>
+      </c>
+      <c r="AE69">
+        <v>67</v>
+      </c>
+      <c r="AF69">
         <v>5493</v>
       </c>
-      <c r="AD69">
+      <c r="AG69">
         <v>5815</v>
       </c>
-      <c r="AE69" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF69">
+      <c r="AH69" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI69">
         <v>322</v>
       </c>
-      <c r="AG69">
+      <c r="AJ69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:36">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7888,22 +8518,31 @@
         <v>68</v>
       </c>
       <c r="AC70">
+        <v>68</v>
+      </c>
+      <c r="AD70">
+        <v>68</v>
+      </c>
+      <c r="AE70">
+        <v>68</v>
+      </c>
+      <c r="AF70">
         <v>5818</v>
       </c>
-      <c r="AD70">
+      <c r="AG70">
         <v>6140</v>
       </c>
-      <c r="AE70" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF70">
+      <c r="AH70" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI70">
         <v>322</v>
       </c>
-      <c r="AG70">
+      <c r="AJ70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:36">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7989,22 +8628,31 @@
         <v>69</v>
       </c>
       <c r="AC71">
+        <v>69</v>
+      </c>
+      <c r="AD71">
+        <v>69</v>
+      </c>
+      <c r="AE71">
+        <v>69</v>
+      </c>
+      <c r="AF71">
         <v>5853</v>
       </c>
-      <c r="AD71">
+      <c r="AG71">
         <v>6182</v>
       </c>
-      <c r="AE71" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF71">
+      <c r="AH71" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI71">
         <v>329</v>
       </c>
-      <c r="AG71">
+      <c r="AJ71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:36">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -8090,22 +8738,31 @@
         <v>70</v>
       </c>
       <c r="AC72">
+        <v>70</v>
+      </c>
+      <c r="AD72">
+        <v>70</v>
+      </c>
+      <c r="AE72">
+        <v>70</v>
+      </c>
+      <c r="AF72">
         <v>5897</v>
       </c>
-      <c r="AD72">
+      <c r="AG72">
         <v>6226</v>
       </c>
-      <c r="AE72" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF72">
+      <c r="AH72" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI72">
         <v>329</v>
       </c>
-      <c r="AG72">
+      <c r="AJ72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:36">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -8191,22 +8848,31 @@
         <v>71</v>
       </c>
       <c r="AC73">
+        <v>71</v>
+      </c>
+      <c r="AD73">
+        <v>71</v>
+      </c>
+      <c r="AE73">
+        <v>71</v>
+      </c>
+      <c r="AF73">
         <v>5956</v>
       </c>
-      <c r="AD73">
+      <c r="AG73">
         <v>6287</v>
       </c>
-      <c r="AE73" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF73">
+      <c r="AH73" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI73">
         <v>331</v>
       </c>
-      <c r="AG73">
+      <c r="AJ73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:36">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -8292,22 +8958,31 @@
         <v>72</v>
       </c>
       <c r="AC74">
+        <v>72</v>
+      </c>
+      <c r="AD74">
+        <v>72</v>
+      </c>
+      <c r="AE74">
+        <v>72</v>
+      </c>
+      <c r="AF74">
         <v>6013</v>
       </c>
-      <c r="AD74">
+      <c r="AG74">
         <v>6352</v>
       </c>
-      <c r="AE74" t="s">
-        <v>104</v>
-      </c>
-      <c r="AF74">
+      <c r="AH74" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI74">
         <v>339</v>
       </c>
-      <c r="AG74">
+      <c r="AJ74">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:36">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8393,22 +9068,31 @@
         <v>73</v>
       </c>
       <c r="AC75">
+        <v>73</v>
+      </c>
+      <c r="AD75">
+        <v>73</v>
+      </c>
+      <c r="AE75">
+        <v>73</v>
+      </c>
+      <c r="AF75">
         <v>6118</v>
       </c>
-      <c r="AD75">
+      <c r="AG75">
         <v>6457</v>
       </c>
-      <c r="AE75" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF75">
+      <c r="AH75" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI75">
         <v>339</v>
       </c>
-      <c r="AG75">
+      <c r="AJ75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:36">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8494,22 +9178,31 @@
         <v>74</v>
       </c>
       <c r="AC76">
+        <v>74</v>
+      </c>
+      <c r="AD76">
+        <v>74</v>
+      </c>
+      <c r="AE76">
+        <v>74</v>
+      </c>
+      <c r="AF76">
         <v>6236</v>
       </c>
-      <c r="AD76">
+      <c r="AG76">
         <v>6579</v>
       </c>
-      <c r="AE76" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF76">
+      <c r="AH76" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI76">
         <v>343</v>
       </c>
-      <c r="AG76">
+      <c r="AJ76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:36">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8595,22 +9288,31 @@
         <v>75</v>
       </c>
       <c r="AC77">
+        <v>75</v>
+      </c>
+      <c r="AD77">
+        <v>75</v>
+      </c>
+      <c r="AE77">
+        <v>75</v>
+      </c>
+      <c r="AF77">
         <v>6314</v>
       </c>
-      <c r="AD77">
+      <c r="AG77">
         <v>6657</v>
       </c>
-      <c r="AE77" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF77">
+      <c r="AH77" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI77">
         <v>343</v>
       </c>
-      <c r="AG77">
+      <c r="AJ77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:36">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8696,22 +9398,31 @@
         <v>76</v>
       </c>
       <c r="AC78">
+        <v>76</v>
+      </c>
+      <c r="AD78">
+        <v>76</v>
+      </c>
+      <c r="AE78">
+        <v>76</v>
+      </c>
+      <c r="AF78">
         <v>6376</v>
       </c>
-      <c r="AD78">
+      <c r="AG78">
         <v>6719</v>
       </c>
-      <c r="AE78" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF78">
+      <c r="AH78" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI78">
         <v>343</v>
       </c>
-      <c r="AG78">
+      <c r="AJ78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:36">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8797,22 +9508,31 @@
         <v>77</v>
       </c>
       <c r="AC79">
+        <v>77</v>
+      </c>
+      <c r="AD79">
+        <v>77</v>
+      </c>
+      <c r="AE79">
+        <v>77</v>
+      </c>
+      <c r="AF79">
         <v>6502</v>
       </c>
-      <c r="AD79">
+      <c r="AG79">
         <v>6845</v>
       </c>
-      <c r="AE79" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF79">
+      <c r="AH79" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI79">
         <v>343</v>
       </c>
-      <c r="AG79">
+      <c r="AJ79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:36">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8898,22 +9618,31 @@
         <v>78</v>
       </c>
       <c r="AC80">
+        <v>78</v>
+      </c>
+      <c r="AD80">
+        <v>78</v>
+      </c>
+      <c r="AE80">
+        <v>78</v>
+      </c>
+      <c r="AF80">
         <v>6568</v>
       </c>
-      <c r="AD80">
+      <c r="AG80">
         <v>6923</v>
       </c>
-      <c r="AE80" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF80">
+      <c r="AH80" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI80">
         <v>355</v>
       </c>
-      <c r="AG80">
+      <c r="AJ80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:36">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8999,22 +9728,31 @@
         <v>79</v>
       </c>
       <c r="AC81">
+        <v>79</v>
+      </c>
+      <c r="AD81">
+        <v>79</v>
+      </c>
+      <c r="AE81">
+        <v>79</v>
+      </c>
+      <c r="AF81">
         <v>6701</v>
       </c>
-      <c r="AD81">
+      <c r="AG81">
         <v>7056</v>
       </c>
-      <c r="AE81" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF81">
+      <c r="AH81" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI81">
         <v>355</v>
       </c>
-      <c r="AG81">
+      <c r="AJ81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:36">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -9100,22 +9838,31 @@
         <v>80</v>
       </c>
       <c r="AC82">
+        <v>80</v>
+      </c>
+      <c r="AD82">
+        <v>80</v>
+      </c>
+      <c r="AE82">
+        <v>80</v>
+      </c>
+      <c r="AF82">
         <v>6829</v>
       </c>
-      <c r="AD82">
+      <c r="AG82">
         <v>7186</v>
       </c>
-      <c r="AE82" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF82">
+      <c r="AH82" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI82">
         <v>357</v>
       </c>
-      <c r="AG82">
+      <c r="AJ82">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:36">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -9201,22 +9948,31 @@
         <v>81</v>
       </c>
       <c r="AC83">
+        <v>81</v>
+      </c>
+      <c r="AD83">
+        <v>81</v>
+      </c>
+      <c r="AE83">
+        <v>81</v>
+      </c>
+      <c r="AF83">
         <v>6973</v>
       </c>
-      <c r="AD83">
+      <c r="AG83">
         <v>7331</v>
       </c>
-      <c r="AE83" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF83">
+      <c r="AH83" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI83">
         <v>358</v>
       </c>
-      <c r="AG83">
+      <c r="AJ83">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:36">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -9302,22 +10058,31 @@
         <v>82</v>
       </c>
       <c r="AC84">
+        <v>82</v>
+      </c>
+      <c r="AD84">
+        <v>82</v>
+      </c>
+      <c r="AE84">
+        <v>82</v>
+      </c>
+      <c r="AF84">
         <v>7124</v>
       </c>
-      <c r="AD84">
+      <c r="AG84">
         <v>7483</v>
       </c>
-      <c r="AE84" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF84">
+      <c r="AH84" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI84">
         <v>359</v>
       </c>
-      <c r="AG84">
+      <c r="AJ84">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:36">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -9403,22 +10168,31 @@
         <v>83</v>
       </c>
       <c r="AC85">
+        <v>83</v>
+      </c>
+      <c r="AD85">
+        <v>83</v>
+      </c>
+      <c r="AE85">
+        <v>83</v>
+      </c>
+      <c r="AF85">
         <v>7229</v>
       </c>
-      <c r="AD85">
+      <c r="AG85">
         <v>7592</v>
       </c>
-      <c r="AE85" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF85">
+      <c r="AH85" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI85">
         <v>363</v>
       </c>
-      <c r="AG85">
+      <c r="AJ85">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:36">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -9504,22 +10278,31 @@
         <v>84</v>
       </c>
       <c r="AC86">
+        <v>84</v>
+      </c>
+      <c r="AD86">
+        <v>84</v>
+      </c>
+      <c r="AE86">
+        <v>84</v>
+      </c>
+      <c r="AF86">
         <v>7434</v>
       </c>
-      <c r="AD86">
+      <c r="AG86">
         <v>7799</v>
       </c>
-      <c r="AE86" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF86">
+      <c r="AH86" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI86">
         <v>365</v>
       </c>
-      <c r="AG86">
+      <c r="AJ86">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:36">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -9605,22 +10388,31 @@
         <v>85</v>
       </c>
       <c r="AC87">
+        <v>85</v>
+      </c>
+      <c r="AD87">
+        <v>85</v>
+      </c>
+      <c r="AE87">
+        <v>85</v>
+      </c>
+      <c r="AF87">
         <v>7548</v>
       </c>
-      <c r="AD87">
+      <c r="AG87">
         <v>7915</v>
       </c>
-      <c r="AE87" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF87">
+      <c r="AH87" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI87">
         <v>367</v>
       </c>
-      <c r="AG87">
+      <c r="AJ87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:36">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -9706,22 +10498,31 @@
         <v>86</v>
       </c>
       <c r="AC88">
+        <v>86</v>
+      </c>
+      <c r="AD88">
+        <v>86</v>
+      </c>
+      <c r="AE88">
+        <v>86</v>
+      </c>
+      <c r="AF88">
         <v>7725</v>
       </c>
-      <c r="AD88">
+      <c r="AG88">
         <v>8100</v>
       </c>
-      <c r="AE88" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF88">
+      <c r="AH88" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI88">
         <v>375</v>
       </c>
-      <c r="AG88">
+      <c r="AJ88">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:36">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -9807,22 +10608,31 @@
         <v>87</v>
       </c>
       <c r="AC89">
+        <v>87</v>
+      </c>
+      <c r="AD89">
+        <v>87</v>
+      </c>
+      <c r="AE89">
+        <v>87</v>
+      </c>
+      <c r="AF89">
         <v>7937</v>
       </c>
-      <c r="AD89">
+      <c r="AG89">
         <v>8314</v>
       </c>
-      <c r="AE89" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF89">
+      <c r="AH89" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI89">
         <v>377</v>
       </c>
-      <c r="AG89">
+      <c r="AJ89">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:36">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -9908,22 +10718,31 @@
         <v>88</v>
       </c>
       <c r="AC90">
+        <v>88</v>
+      </c>
+      <c r="AD90">
+        <v>88</v>
+      </c>
+      <c r="AE90">
+        <v>88</v>
+      </c>
+      <c r="AF90">
         <v>8179</v>
       </c>
-      <c r="AD90">
+      <c r="AG90">
         <v>8556</v>
       </c>
-      <c r="AE90" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF90">
+      <c r="AH90" t="s">
+        <v>123</v>
+      </c>
+      <c r="AI90">
         <v>377</v>
       </c>
-      <c r="AG90">
+      <c r="AJ90">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:36">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -9990,23 +10809,32 @@
       <c r="V91">
         <v>89</v>
       </c>
-      <c r="AC91">
+      <c r="W91">
+        <v>89</v>
+      </c>
+      <c r="X91">
+        <v>89</v>
+      </c>
+      <c r="Y91">
+        <v>89</v>
+      </c>
+      <c r="AF91">
         <v>8357</v>
       </c>
-      <c r="AD91">
+      <c r="AG91">
         <v>8735</v>
       </c>
-      <c r="AE91" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF91">
+      <c r="AH91" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI91">
         <v>378</v>
       </c>
-      <c r="AG91">
+      <c r="AJ91">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:36">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -10070,23 +10898,32 @@
       <c r="U92">
         <v>90</v>
       </c>
-      <c r="AC92">
+      <c r="V92">
+        <v>90</v>
+      </c>
+      <c r="W92">
+        <v>90</v>
+      </c>
+      <c r="X92">
+        <v>90</v>
+      </c>
+      <c r="AF92">
         <v>8436</v>
       </c>
-      <c r="AD92">
+      <c r="AG92">
         <v>8815</v>
       </c>
-      <c r="AE92" t="s">
-        <v>122</v>
-      </c>
-      <c r="AF92">
+      <c r="AH92" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI92">
         <v>379</v>
       </c>
-      <c r="AG92">
+      <c r="AJ92">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:36">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -10150,23 +10987,32 @@
       <c r="U93">
         <v>91</v>
       </c>
-      <c r="AC93">
+      <c r="V93">
+        <v>91</v>
+      </c>
+      <c r="W93">
+        <v>91</v>
+      </c>
+      <c r="X93">
+        <v>91</v>
+      </c>
+      <c r="AF93">
         <v>8777</v>
       </c>
-      <c r="AD93">
+      <c r="AG93">
         <v>9157</v>
       </c>
-      <c r="AE93" t="s">
-        <v>123</v>
-      </c>
-      <c r="AF93">
+      <c r="AH93" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI93">
         <v>380</v>
       </c>
-      <c r="AG93">
+      <c r="AJ93">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:36">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -10227,23 +11073,32 @@
       <c r="T94">
         <v>92</v>
       </c>
-      <c r="AC94">
+      <c r="U94">
+        <v>92</v>
+      </c>
+      <c r="V94">
+        <v>92</v>
+      </c>
+      <c r="W94">
+        <v>92</v>
+      </c>
+      <c r="AF94">
         <v>8932</v>
       </c>
-      <c r="AD94">
+      <c r="AG94">
         <v>9318</v>
       </c>
-      <c r="AE94" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF94">
+      <c r="AH94" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI94">
         <v>386</v>
       </c>
-      <c r="AG94">
+      <c r="AJ94">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:33">
+    <row r="95" spans="1:36">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -10301,23 +11156,32 @@
       <c r="S95">
         <v>93</v>
       </c>
-      <c r="AC95">
+      <c r="T95">
+        <v>93</v>
+      </c>
+      <c r="U95">
+        <v>93</v>
+      </c>
+      <c r="V95">
+        <v>93</v>
+      </c>
+      <c r="AF95">
         <v>9148</v>
       </c>
-      <c r="AD95">
+      <c r="AG95">
         <v>9535</v>
       </c>
-      <c r="AE95" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF95">
+      <c r="AH95" t="s">
+        <v>128</v>
+      </c>
+      <c r="AI95">
         <v>387</v>
       </c>
-      <c r="AG95">
+      <c r="AJ95">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:36">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -10375,23 +11239,32 @@
       <c r="S96">
         <v>94</v>
       </c>
-      <c r="AC96">
+      <c r="T96">
+        <v>94</v>
+      </c>
+      <c r="U96">
+        <v>94</v>
+      </c>
+      <c r="V96">
+        <v>94</v>
+      </c>
+      <c r="AF96">
         <v>9462</v>
       </c>
-      <c r="AD96">
+      <c r="AG96">
         <v>9852</v>
       </c>
-      <c r="AE96" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF96">
+      <c r="AH96" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI96">
         <v>390</v>
       </c>
-      <c r="AG96">
+      <c r="AJ96">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:36">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -10449,23 +11322,32 @@
       <c r="S97">
         <v>95</v>
       </c>
-      <c r="AC97">
+      <c r="T97">
+        <v>95</v>
+      </c>
+      <c r="U97">
+        <v>95</v>
+      </c>
+      <c r="V97">
+        <v>95</v>
+      </c>
+      <c r="AF97">
         <v>9862</v>
       </c>
-      <c r="AD97">
+      <c r="AG97">
         <v>10259</v>
       </c>
-      <c r="AE97" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF97">
+      <c r="AH97" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI97">
         <v>397</v>
       </c>
-      <c r="AG97">
+      <c r="AJ97">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:33">
+    <row r="98" spans="1:36">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -10523,23 +11405,32 @@
       <c r="S98">
         <v>96</v>
       </c>
-      <c r="AC98">
+      <c r="T98">
+        <v>96</v>
+      </c>
+      <c r="U98">
+        <v>96</v>
+      </c>
+      <c r="V98">
+        <v>96</v>
+      </c>
+      <c r="AF98">
         <v>10088</v>
       </c>
-      <c r="AD98">
+      <c r="AG98">
         <v>10486</v>
       </c>
-      <c r="AE98" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF98">
+      <c r="AH98" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI98">
         <v>398</v>
       </c>
-      <c r="AG98">
+      <c r="AJ98">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33">
+    <row r="99" spans="1:36">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -10582,23 +11473,32 @@
       <c r="N99">
         <v>97</v>
       </c>
-      <c r="AC99">
+      <c r="O99">
+        <v>97</v>
+      </c>
+      <c r="P99">
+        <v>97</v>
+      </c>
+      <c r="Q99">
+        <v>97</v>
+      </c>
+      <c r="AF99">
         <v>10374</v>
       </c>
-      <c r="AD99">
+      <c r="AG99">
         <v>10774</v>
       </c>
-      <c r="AE99" t="s">
-        <v>129</v>
-      </c>
-      <c r="AF99">
+      <c r="AH99" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI99">
         <v>400</v>
       </c>
-      <c r="AG99">
+      <c r="AJ99">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:33">
+    <row r="100" spans="1:36">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -10638,23 +11538,32 @@
       <c r="M100">
         <v>98</v>
       </c>
-      <c r="AC100">
+      <c r="N100">
+        <v>98</v>
+      </c>
+      <c r="O100">
+        <v>98</v>
+      </c>
+      <c r="P100">
+        <v>98</v>
+      </c>
+      <c r="AF100">
         <v>10374</v>
       </c>
-      <c r="AD100">
+      <c r="AG100">
         <v>10774</v>
       </c>
-      <c r="AE100" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF100">
+      <c r="AH100" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI100">
         <v>400</v>
       </c>
-      <c r="AG100">
+      <c r="AJ100">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:33">
+    <row r="101" spans="1:36">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -10685,23 +11594,32 @@
       <c r="J101">
         <v>99</v>
       </c>
-      <c r="AC101">
+      <c r="K101">
+        <v>99</v>
+      </c>
+      <c r="L101">
+        <v>99</v>
+      </c>
+      <c r="M101">
+        <v>99</v>
+      </c>
+      <c r="AF101">
         <v>10374</v>
       </c>
-      <c r="AD101">
+      <c r="AG101">
         <v>10774</v>
       </c>
-      <c r="AE101" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF101">
+      <c r="AH101" t="s">
+        <v>134</v>
+      </c>
+      <c r="AI101">
         <v>400</v>
       </c>
-      <c r="AG101">
+      <c r="AJ101">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:33">
+    <row r="102" spans="1:36">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -10729,23 +11647,32 @@
       <c r="I102">
         <v>100</v>
       </c>
-      <c r="AC102">
+      <c r="J102">
+        <v>100</v>
+      </c>
+      <c r="K102">
+        <v>100</v>
+      </c>
+      <c r="L102">
+        <v>100</v>
+      </c>
+      <c r="AF102">
         <v>11473</v>
       </c>
-      <c r="AD102">
+      <c r="AG102">
         <v>11878</v>
       </c>
-      <c r="AE102" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF102">
+      <c r="AH102" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI102">
         <v>405</v>
       </c>
-      <c r="AG102">
+      <c r="AJ102">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:33">
+    <row r="103" spans="1:36">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -10773,23 +11700,32 @@
       <c r="I103">
         <v>101</v>
       </c>
-      <c r="AC103">
+      <c r="J103">
+        <v>101</v>
+      </c>
+      <c r="K103">
+        <v>101</v>
+      </c>
+      <c r="L103">
+        <v>101</v>
+      </c>
+      <c r="AF103">
         <v>11796</v>
       </c>
-      <c r="AD103">
+      <c r="AG103">
         <v>12204</v>
       </c>
-      <c r="AE103" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF103">
+      <c r="AH103" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI103">
         <v>408</v>
       </c>
-      <c r="AG103">
+      <c r="AJ103">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:33">
+    <row r="104" spans="1:36">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -10817,23 +11753,32 @@
       <c r="I104">
         <v>102</v>
       </c>
-      <c r="AC104">
+      <c r="J104">
+        <v>102</v>
+      </c>
+      <c r="K104">
+        <v>102</v>
+      </c>
+      <c r="L104">
+        <v>102</v>
+      </c>
+      <c r="AF104">
         <v>12764</v>
       </c>
-      <c r="AD104">
+      <c r="AG104">
         <v>13174</v>
       </c>
-      <c r="AE104" t="s">
-        <v>134</v>
-      </c>
-      <c r="AF104">
+      <c r="AH104" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI104">
         <v>410</v>
       </c>
-      <c r="AG104">
+      <c r="AJ104">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:36">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -10861,23 +11806,32 @@
       <c r="I105">
         <v>103</v>
       </c>
-      <c r="AC105">
+      <c r="J105">
+        <v>103</v>
+      </c>
+      <c r="K105">
+        <v>103</v>
+      </c>
+      <c r="L105">
+        <v>103</v>
+      </c>
+      <c r="AF105">
         <v>13500</v>
       </c>
-      <c r="AD105">
+      <c r="AG105">
         <v>13910</v>
       </c>
-      <c r="AE105" t="s">
-        <v>135</v>
-      </c>
-      <c r="AF105">
+      <c r="AH105" t="s">
+        <v>138</v>
+      </c>
+      <c r="AI105">
         <v>410</v>
       </c>
-      <c r="AG105">
+      <c r="AJ105">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:33">
+    <row r="106" spans="1:36">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -10905,23 +11859,32 @@
       <c r="I106">
         <v>104</v>
       </c>
-      <c r="AC106">
+      <c r="J106">
+        <v>104</v>
+      </c>
+      <c r="K106">
+        <v>104</v>
+      </c>
+      <c r="L106">
+        <v>104</v>
+      </c>
+      <c r="AF106">
         <v>14193</v>
       </c>
-      <c r="AD106">
+      <c r="AG106">
         <v>14607</v>
       </c>
-      <c r="AE106" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF106">
+      <c r="AH106" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI106">
         <v>414</v>
       </c>
-      <c r="AG106">
+      <c r="AJ106">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:36">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -10949,23 +11912,32 @@
       <c r="I107">
         <v>105</v>
       </c>
-      <c r="AC107">
+      <c r="J107">
+        <v>105</v>
+      </c>
+      <c r="K107">
+        <v>105</v>
+      </c>
+      <c r="L107">
+        <v>105</v>
+      </c>
+      <c r="AF107">
         <v>14679</v>
       </c>
-      <c r="AD107">
+      <c r="AG107">
         <v>15095</v>
       </c>
-      <c r="AE107" t="s">
-        <v>137</v>
-      </c>
-      <c r="AF107">
+      <c r="AH107" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI107">
         <v>416</v>
       </c>
-      <c r="AG107">
+      <c r="AJ107">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:33">
+    <row r="108" spans="1:36">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -10978,23 +11950,32 @@
       <c r="D108">
         <v>106</v>
       </c>
-      <c r="AC108">
+      <c r="E108">
+        <v>106</v>
+      </c>
+      <c r="F108">
+        <v>106</v>
+      </c>
+      <c r="G108">
+        <v>106</v>
+      </c>
+      <c r="AF108">
         <v>15184</v>
       </c>
-      <c r="AD108">
+      <c r="AG108">
         <v>15604</v>
       </c>
-      <c r="AE108" t="s">
-        <v>138</v>
-      </c>
-      <c r="AF108">
+      <c r="AH108" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI108">
         <v>420</v>
       </c>
-      <c r="AG108">
+      <c r="AJ108">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:33">
+    <row r="109" spans="1:36">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -11007,23 +11988,32 @@
       <c r="D109">
         <v>107</v>
       </c>
-      <c r="AC109">
+      <c r="E109">
+        <v>107</v>
+      </c>
+      <c r="F109">
+        <v>107</v>
+      </c>
+      <c r="G109">
+        <v>107</v>
+      </c>
+      <c r="AF109">
         <v>15748</v>
       </c>
-      <c r="AD109">
+      <c r="AG109">
         <v>16180</v>
       </c>
-      <c r="AE109" t="s">
-        <v>139</v>
-      </c>
-      <c r="AF109">
+      <c r="AH109" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI109">
         <v>432</v>
       </c>
-      <c r="AG109">
+      <c r="AJ109">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:33">
+    <row r="110" spans="1:36">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -11036,23 +12026,32 @@
       <c r="D110">
         <v>108</v>
       </c>
-      <c r="AC110">
+      <c r="E110">
+        <v>108</v>
+      </c>
+      <c r="F110">
+        <v>108</v>
+      </c>
+      <c r="G110">
+        <v>108</v>
+      </c>
+      <c r="AF110">
         <v>16593</v>
       </c>
-      <c r="AD110">
+      <c r="AG110">
         <v>17028</v>
       </c>
-      <c r="AE110" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF110">
+      <c r="AH110" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI110">
         <v>435</v>
       </c>
-      <c r="AG110">
+      <c r="AJ110">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:36">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -11065,23 +12064,32 @@
       <c r="D111">
         <v>109</v>
       </c>
-      <c r="AC111">
+      <c r="E111">
+        <v>109</v>
+      </c>
+      <c r="F111">
+        <v>109</v>
+      </c>
+      <c r="G111">
+        <v>109</v>
+      </c>
+      <c r="AF111">
         <v>17272</v>
       </c>
-      <c r="AD111">
+      <c r="AG111">
         <v>17707</v>
       </c>
-      <c r="AE111" t="s">
-        <v>141</v>
-      </c>
-      <c r="AF111">
+      <c r="AH111" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI111">
         <v>435</v>
       </c>
-      <c r="AG111">
+      <c r="AJ111">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:33">
+    <row r="112" spans="1:36">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -11094,23 +12102,32 @@
       <c r="D112">
         <v>110</v>
       </c>
-      <c r="AC112">
+      <c r="E112">
+        <v>110</v>
+      </c>
+      <c r="F112">
+        <v>110</v>
+      </c>
+      <c r="G112">
+        <v>110</v>
+      </c>
+      <c r="AF112">
         <v>18003</v>
       </c>
-      <c r="AD112">
+      <c r="AG112">
         <v>18442</v>
       </c>
-      <c r="AE112" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF112">
+      <c r="AH112" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI112">
         <v>439</v>
       </c>
-      <c r="AG112">
+      <c r="AJ112">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:33">
+    <row r="113" spans="1:36">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -11120,23 +12137,32 @@
       <c r="C113">
         <v>111</v>
       </c>
-      <c r="AC113">
+      <c r="D113">
+        <v>111</v>
+      </c>
+      <c r="E113">
+        <v>111</v>
+      </c>
+      <c r="F113">
+        <v>111</v>
+      </c>
+      <c r="AF113">
         <v>18379</v>
       </c>
-      <c r="AD113">
+      <c r="AG113">
         <v>18818</v>
       </c>
-      <c r="AE113" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF113">
+      <c r="AH113" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI113">
         <v>439</v>
       </c>
-      <c r="AG113">
+      <c r="AJ113">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:33">
+    <row r="114" spans="1:36">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -11146,23 +12172,32 @@
       <c r="C114">
         <v>112</v>
       </c>
-      <c r="AC114">
+      <c r="D114">
+        <v>112</v>
+      </c>
+      <c r="E114">
+        <v>112</v>
+      </c>
+      <c r="F114">
+        <v>112</v>
+      </c>
+      <c r="AF114">
         <v>19204</v>
       </c>
-      <c r="AD114">
+      <c r="AG114">
         <v>19654</v>
       </c>
-      <c r="AE114" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF114">
+      <c r="AH114" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI114">
         <v>450</v>
       </c>
-      <c r="AG114">
+      <c r="AJ114">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:36">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -11172,23 +12207,32 @@
       <c r="C115">
         <v>113</v>
       </c>
-      <c r="AC115">
+      <c r="D115">
+        <v>113</v>
+      </c>
+      <c r="E115">
+        <v>113</v>
+      </c>
+      <c r="F115">
+        <v>113</v>
+      </c>
+      <c r="AF115">
         <v>19672</v>
       </c>
-      <c r="AD115">
+      <c r="AG115">
         <v>20126</v>
       </c>
-      <c r="AE115" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF115">
+      <c r="AH115" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI115">
         <v>454</v>
       </c>
-      <c r="AG115">
+      <c r="AJ115">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:33">
+    <row r="116" spans="1:36">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -11198,23 +12242,32 @@
       <c r="C116">
         <v>114</v>
       </c>
-      <c r="AC116">
+      <c r="D116">
+        <v>114</v>
+      </c>
+      <c r="E116">
+        <v>114</v>
+      </c>
+      <c r="F116">
+        <v>114</v>
+      </c>
+      <c r="AF116">
         <v>20154</v>
       </c>
-      <c r="AD116">
+      <c r="AG116">
         <v>20622</v>
       </c>
-      <c r="AE116" t="s">
-        <v>146</v>
-      </c>
-      <c r="AF116">
+      <c r="AH116" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI116">
         <v>468</v>
       </c>
-      <c r="AG116">
+      <c r="AJ116">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:33">
+    <row r="117" spans="1:36">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -11224,23 +12277,32 @@
       <c r="C117">
         <v>115</v>
       </c>
-      <c r="AC117">
+      <c r="D117">
+        <v>115</v>
+      </c>
+      <c r="E117">
+        <v>115</v>
+      </c>
+      <c r="F117">
+        <v>115</v>
+      </c>
+      <c r="AF117">
         <v>20976</v>
       </c>
-      <c r="AD117">
+      <c r="AG117">
         <v>21449</v>
       </c>
-      <c r="AE117" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF117">
+      <c r="AH117" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI117">
         <v>473</v>
       </c>
-      <c r="AG117">
+      <c r="AJ117">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:33">
+    <row r="118" spans="1:36">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -11250,23 +12312,32 @@
       <c r="C118">
         <v>116</v>
       </c>
-      <c r="AC118">
+      <c r="D118">
+        <v>116</v>
+      </c>
+      <c r="E118">
+        <v>116</v>
+      </c>
+      <c r="F118">
+        <v>116</v>
+      </c>
+      <c r="AF118">
         <v>21803</v>
       </c>
-      <c r="AD118">
+      <c r="AG118">
         <v>22286</v>
       </c>
-      <c r="AE118" t="s">
-        <v>148</v>
-      </c>
-      <c r="AF118">
+      <c r="AH118" t="s">
+        <v>151</v>
+      </c>
+      <c r="AI118">
         <v>483</v>
       </c>
-      <c r="AG118">
+      <c r="AJ118">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:36">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -11276,23 +12347,32 @@
       <c r="C119">
         <v>117</v>
       </c>
-      <c r="AC119">
+      <c r="D119">
+        <v>117</v>
+      </c>
+      <c r="E119">
+        <v>117</v>
+      </c>
+      <c r="F119">
+        <v>117</v>
+      </c>
+      <c r="AF119">
         <v>22565</v>
       </c>
-      <c r="AD119">
+      <c r="AG119">
         <v>23048</v>
       </c>
-      <c r="AE119" t="s">
-        <v>149</v>
-      </c>
-      <c r="AF119">
+      <c r="AH119" t="s">
+        <v>152</v>
+      </c>
+      <c r="AI119">
         <v>483</v>
       </c>
-      <c r="AG119">
+      <c r="AJ119">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:36">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -11302,59 +12382,86 @@
       <c r="C120">
         <v>118</v>
       </c>
-      <c r="AC120">
+      <c r="D120">
+        <v>118</v>
+      </c>
+      <c r="E120">
+        <v>118</v>
+      </c>
+      <c r="F120">
+        <v>118</v>
+      </c>
+      <c r="AF120">
         <v>23320</v>
       </c>
-      <c r="AD120">
+      <c r="AG120">
         <v>23803</v>
       </c>
-      <c r="AE120" t="s">
-        <v>150</v>
-      </c>
-      <c r="AF120">
+      <c r="AH120" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI120">
         <v>483</v>
       </c>
-      <c r="AG120">
+      <c r="AJ120">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:36">
       <c r="A121" s="1">
         <v>119</v>
       </c>
-      <c r="AC121">
+      <c r="B121">
+        <v>119</v>
+      </c>
+      <c r="C121">
+        <v>119</v>
+      </c>
+      <c r="D121">
+        <v>119</v>
+      </c>
+      <c r="AF121">
         <v>24326</v>
       </c>
-      <c r="AD121">
+      <c r="AG121">
         <v>24824</v>
       </c>
-      <c r="AE121" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF121">
+      <c r="AH121" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI121">
         <v>498</v>
       </c>
-      <c r="AG121">
+      <c r="AJ121">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:33">
+    <row r="122" spans="1:36">
       <c r="A122" s="1">
         <v>120</v>
       </c>
-      <c r="AC122">
+      <c r="B122">
+        <v>120</v>
+      </c>
+      <c r="C122">
+        <v>120</v>
+      </c>
+      <c r="D122">
+        <v>120</v>
+      </c>
+      <c r="AF122">
         <v>25109</v>
       </c>
-      <c r="AD122">
+      <c r="AG122">
         <v>25611</v>
       </c>
-      <c r="AE122" t="s">
-        <v>152</v>
-      </c>
-      <c r="AF122">
+      <c r="AH122" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI122">
         <v>502</v>
       </c>
-      <c r="AG122">
+      <c r="AJ122">
         <v>0</v>
       </c>
     </row>

</xml_diff>